<commit_message>
Melhora arquivo de saida pela quadragesima quinta vez
</commit_message>
<xml_diff>
--- a/planilha_alocacoes.xlsx
+++ b/planilha_alocacoes.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -37,8 +37,11 @@
       <name val="Arial"/>
       <b val="1"/>
     </font>
+    <font>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -58,6 +61,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00E0E0E0"/>
         <bgColor rgb="00E0E0E0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ffa500"/>
+        <bgColor rgb="00ff7b59"/>
       </patternFill>
     </fill>
   </fills>
@@ -139,7 +148,7 @@
       </bottom>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -147,8 +156,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -170,12 +182,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
     <cellStyle name="estilo_header" xfId="1" hidden="0"/>
     <cellStyle name="estilo_index" xfId="2" hidden="0"/>
+    <cellStyle name="compartilhamento" xfId="3" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1716,29 +1732,29 @@
           <t>301-A</t>
         </is>
       </c>
-      <c r="C14" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="C14" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 8 (GCA269_1) | AGRO - 3 (GCB030_1) </t>
         </is>
       </c>
       <c r="D14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GEX431_1)</t>
         </is>
       </c>
       <c r="E14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 8 (GCS073_1)</t>
         </is>
       </c>
       <c r="F14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G14" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>AGRO - 8 (GCA257_1)</t>
+        </is>
+      </c>
+      <c r="G14" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - opt (GCA312_1) | AGRO - opt (GCA655_1) </t>
         </is>
       </c>
       <c r="H14" s="7" t="inlineStr">
@@ -1748,27 +1764,27 @@
       </c>
       <c r="I14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 3 (GCS005_1)</t>
         </is>
       </c>
       <c r="J14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 8 (GCS056_1)</t>
         </is>
       </c>
       <c r="K14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 8 (GCA221_1)</t>
         </is>
       </c>
       <c r="L14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 8 (GCA255_1)</t>
         </is>
       </c>
       <c r="M14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 9 (GCA282_1)</t>
         </is>
       </c>
       <c r="N14" s="7" t="inlineStr">
@@ -1798,7 +1814,7 @@
       </c>
       <c r="S14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 9 (GCA282_1)</t>
         </is>
       </c>
       <c r="T14" s="7" t="inlineStr">
@@ -1816,62 +1832,62 @@
       </c>
       <c r="C15" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 6 (GCA250_1)</t>
         </is>
       </c>
       <c r="D15" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E15" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>AGRO - 6 (GCA025_1)</t>
+        </is>
+      </c>
+      <c r="E15" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 6 (GCA239_1) | AGRO - 6 (GCB054_1) </t>
         </is>
       </c>
       <c r="F15" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 6 (GEX080_1)</t>
         </is>
       </c>
       <c r="G15" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA657_1)</t>
         </is>
       </c>
       <c r="H15" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 10 (GCA283_1)</t>
         </is>
       </c>
       <c r="I15" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 6 (GCS243_1)</t>
         </is>
       </c>
       <c r="J15" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 10 (GCA283_1)</t>
         </is>
       </c>
       <c r="K15" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 6 (GCA241_1)</t>
         </is>
       </c>
       <c r="L15" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 6 (GCA050_1)</t>
         </is>
       </c>
       <c r="M15" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA315_1)</t>
         </is>
       </c>
       <c r="N15" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 10 (GCA283_1)</t>
         </is>
       </c>
       <c r="O15" s="7" t="inlineStr">
@@ -1901,7 +1917,7 @@
       </c>
       <c r="T15" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 10 (GCA283_1)</t>
         </is>
       </c>
     </row>
@@ -1912,9 +1928,9 @@
           <t>303-A</t>
         </is>
       </c>
-      <c r="C16" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="C16" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 4 (GCA210_1) | AGRO - 2 (GCA218_1) </t>
         </is>
       </c>
       <c r="D16" s="7" t="inlineStr">
@@ -1924,17 +1940,17 @@
       </c>
       <c r="E16" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F16" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G16" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>AGRO - 2 (GCB107_1)</t>
+        </is>
+      </c>
+      <c r="F16" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 2 (GCA210_3) | AGRO - 2 (GCB056_5) </t>
+        </is>
+      </c>
+      <c r="G16" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 4 (GCA045_1) | AGRO - 2 (GEX190_2) </t>
         </is>
       </c>
       <c r="H16" s="7" t="inlineStr">
@@ -1944,27 +1960,27 @@
       </c>
       <c r="I16" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J16" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>AGRO - 4 (GEX116_1)</t>
+        </is>
+      </c>
+      <c r="J16" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 2 (GCB056_5) | AGRO - 4 (GCH012_1) </t>
         </is>
       </c>
       <c r="K16" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 4 (GCA034_1)</t>
         </is>
       </c>
       <c r="L16" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 1 (GCH292_3)</t>
         </is>
       </c>
       <c r="M16" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 2 (GEX179_1)</t>
         </is>
       </c>
       <c r="N16" s="7" t="inlineStr">
@@ -2010,29 +2026,29 @@
           <t>304-A</t>
         </is>
       </c>
-      <c r="C17" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="C17" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 4 (GCA210_1) | AGRO - 4 (GCA210_2) </t>
         </is>
       </c>
       <c r="D17" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E17" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F17" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G17" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>AGRO - 8 (GCA245_1)</t>
+        </is>
+      </c>
+      <c r="E17" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 4 (GCA218_2) | AGRO - 4 (GCB130_1) </t>
+        </is>
+      </c>
+      <c r="F17" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 2 (GCA210_4) | AGRO - 2 (GCB056_4) </t>
+        </is>
+      </c>
+      <c r="G17" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 2 (GEX190_1) | AGRO - 2 (GEX190_2) </t>
         </is>
       </c>
       <c r="H17" s="7" t="inlineStr">
@@ -2042,12 +2058,12 @@
       </c>
       <c r="I17" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J17" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>AGRO - 8 (GCA224_1)</t>
+        </is>
+      </c>
+      <c r="J17" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 2 (GCB056_4) | AGRO - 2 (GCB056_5) </t>
         </is>
       </c>
       <c r="K17" s="7" t="inlineStr">
@@ -2057,12 +2073,12 @@
       </c>
       <c r="L17" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 4 (GCH008_1)</t>
         </is>
       </c>
       <c r="M17" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 7 (GCA287_1)</t>
         </is>
       </c>
       <c r="N17" s="7" t="inlineStr">
@@ -2077,7 +2093,7 @@
       </c>
       <c r="P17" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 7 (GCA225_1)</t>
         </is>
       </c>
       <c r="Q17" s="7" t="inlineStr">
@@ -2125,12 +2141,12 @@
       </c>
       <c r="F18" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 4 (GCA037_2)</t>
         </is>
       </c>
       <c r="G18" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA588_1)</t>
         </is>
       </c>
       <c r="H18" s="7" t="inlineStr">
@@ -2140,12 +2156,12 @@
       </c>
       <c r="I18" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 4 (GEX116_2)</t>
         </is>
       </c>
       <c r="J18" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 6 (GCA286_1)</t>
         </is>
       </c>
       <c r="K18" s="7" t="inlineStr">
@@ -2223,12 +2239,12 @@
       </c>
       <c r="F19" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 4 (GCA037_1)</t>
         </is>
       </c>
       <c r="G19" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA675_1)</t>
         </is>
       </c>
       <c r="H19" s="7" t="inlineStr">
@@ -2243,7 +2259,7 @@
       </c>
       <c r="J19" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 6 (GCA286_2)</t>
         </is>
       </c>
       <c r="K19" s="7" t="inlineStr">
@@ -4296,7 +4312,7 @@
       </c>
       <c r="I40" s="7" t="inlineStr">
         <is>
-          <t>CC - 2 (GEN253_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J40" s="7" t="inlineStr">
@@ -4326,22 +4342,22 @@
       </c>
       <c r="O40" s="7" t="inlineStr">
         <is>
-          <t>CC - 2 (GEX605_1)</t>
+          <t>CC - 1 (GCH293_2)</t>
         </is>
       </c>
       <c r="P40" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 1 (GEX208_1)</t>
         </is>
       </c>
       <c r="Q40" s="7" t="inlineStr">
         <is>
-          <t>CC - 2 (GLA104_2)</t>
+          <t>CC - 1 (GEX213_1)</t>
         </is>
       </c>
       <c r="R40" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 1 (GEX003_1)</t>
         </is>
       </c>
       <c r="S40" s="7" t="inlineStr">
@@ -4424,22 +4440,22 @@
       </c>
       <c r="O41" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GCH293_2)</t>
+          <t>CC - 3 (GEX098_2)</t>
         </is>
       </c>
       <c r="P41" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX208_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q41" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 3 (GEX608_1)</t>
         </is>
       </c>
       <c r="R41" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_2)</t>
+          <t>CC - 3 (GEX606_1)</t>
         </is>
       </c>
       <c r="S41" s="7" t="inlineStr">
@@ -4492,7 +4508,7 @@
       </c>
       <c r="I42" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 2 (GEN253_1)</t>
         </is>
       </c>
       <c r="J42" s="7" t="inlineStr">
@@ -4522,7 +4538,7 @@
       </c>
       <c r="O42" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX098_2)</t>
+          <t>CC - 2 (GEX605_1)</t>
         </is>
       </c>
       <c r="P42" s="7" t="inlineStr">
@@ -4532,12 +4548,12 @@
       </c>
       <c r="Q42" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX608_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R42" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX606_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S42" s="7" t="inlineStr">
@@ -4560,12 +4576,12 @@
       </c>
       <c r="C43" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX612_1)</t>
         </is>
       </c>
       <c r="D43" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX612_1)</t>
         </is>
       </c>
       <c r="E43" s="7" t="inlineStr">
@@ -4575,37 +4591,37 @@
       </c>
       <c r="F43" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 9 (GEX657_1)</t>
         </is>
       </c>
       <c r="G43" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 9 (GEX657_1)</t>
         </is>
       </c>
       <c r="H43" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I43" s="7" t="inlineStr">
-        <is>
-          <t>CC - 2 (GEX178_1) | CC - 4 (GEX613_2)</t>
+          <t>CC - 9 (GEX657_1)</t>
+        </is>
+      </c>
+      <c r="I43" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEX612_1) | CC - 4 (GEX613_2) </t>
         </is>
       </c>
       <c r="J43" s="7" t="inlineStr">
         <is>
-          <t>CC - 2 (GEX605_2)</t>
-        </is>
-      </c>
-      <c r="K43" s="7" t="inlineStr">
-        <is>
-          <t>CC - opt (GEX1082_1) | CC - 2 (GEX178_1)</t>
-        </is>
-      </c>
-      <c r="L43" s="7" t="inlineStr">
-        <is>
-          <t>CC - opt (GEX1082_1) | CC - 2 (GEX605_2)</t>
+          <t>CC - 4 (GEX102_1)</t>
+        </is>
+      </c>
+      <c r="K43" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - opt (GEX1082_1) | CC - 4 (GEX612_1) </t>
+        </is>
+      </c>
+      <c r="L43" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEX102_1) | CC - opt (GEX1082_1) </t>
         </is>
       </c>
       <c r="M43" s="7" t="inlineStr">
@@ -4625,7 +4641,7 @@
       </c>
       <c r="P43" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX392_1)</t>
+          <t>CC - 1 (GEX208_2)</t>
         </is>
       </c>
       <c r="Q43" s="7" t="inlineStr">
@@ -4635,12 +4651,12 @@
       </c>
       <c r="R43" s="7" t="inlineStr">
         <is>
-          <t>CC - opt (GEX1083_1)</t>
+          <t>CC - 1 (GEX003_2)</t>
         </is>
       </c>
       <c r="S43" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX609_1)</t>
+          <t>CC - 1 (GEX210_2)</t>
         </is>
       </c>
       <c r="T43" s="7" t="inlineStr">
@@ -4673,42 +4689,42 @@
       </c>
       <c r="F44" s="7" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G44" s="7" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H44" s="7" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
-        </is>
-      </c>
-      <c r="I44" s="7" t="inlineStr">
-        <is>
-          <t>CC - 6 (GEX105_1) | CC - 6 (GEX108_1)</t>
-        </is>
-      </c>
-      <c r="J44" s="7" t="inlineStr">
-        <is>
-          <t>CC - 6 (GCS580_1) | CC - 6 (GEX614_1)</t>
-        </is>
-      </c>
-      <c r="K44" s="7" t="inlineStr">
-        <is>
-          <t>CC - 6 (GCH292_2)</t>
-        </is>
-      </c>
-      <c r="L44" s="7" t="inlineStr">
-        <is>
-          <t>CC - 6 (GCS580_1) | CC - 6 (GEX105_1)</t>
-        </is>
-      </c>
-      <c r="M44" s="7" t="inlineStr">
-        <is>
-          <t>CC - 6 (GEX108_1) | CC - 6 (GEX614_1)</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I44" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 2 (GEX178_1) | CC - 4 (GEX613_1) </t>
+        </is>
+      </c>
+      <c r="J44" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEN254_1) | CC - 2 (GEX605_2) </t>
+        </is>
+      </c>
+      <c r="K44" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEX090_1) | CC - 2 (GEX178_1) </t>
+        </is>
+      </c>
+      <c r="L44" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEN254_1) | CC - 2 (GEX605_2) </t>
+        </is>
+      </c>
+      <c r="M44" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEX090_1) | CC - 4 (GEX613_1) </t>
         </is>
       </c>
       <c r="N44" s="7" t="inlineStr">
@@ -4756,12 +4772,12 @@
       </c>
       <c r="C45" s="7" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX612_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D45" s="7" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX612_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E45" s="7" t="inlineStr">
@@ -4784,29 +4800,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I45" s="7" t="inlineStr">
-        <is>
-          <t>CC - 4 (GEX612_1) | CC - 4 (GEX613_1)</t>
-        </is>
-      </c>
-      <c r="J45" s="7" t="inlineStr">
-        <is>
-          <t>CC - 4 (GEN254_1) | CC - 4 (GEX102_1)</t>
+      <c r="I45" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 6 (GEX105_1) | CC - 6 (GEX108_1) </t>
+        </is>
+      </c>
+      <c r="J45" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 6 (GCS580_1) | CC - 6 (GEX614_1) </t>
         </is>
       </c>
       <c r="K45" s="7" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX090_1) | CC - 4 (GEX612_1)</t>
-        </is>
-      </c>
-      <c r="L45" s="7" t="inlineStr">
-        <is>
-          <t>CC - 4 (GEN254_1) | CC - 4 (GEX102_1)</t>
-        </is>
-      </c>
-      <c r="M45" s="7" t="inlineStr">
-        <is>
-          <t>CC - 4 (GEX090_1) | CC - 4 (GEX613_1)</t>
+          <t>CC - 6 (GCH292_2)</t>
+        </is>
+      </c>
+      <c r="L45" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 6 (GCS580_1) | CC - 6 (GEX105_1) </t>
+        </is>
+      </c>
+      <c r="M45" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 6 (GEX108_1) | CC - 6 (GEX614_1) </t>
         </is>
       </c>
       <c r="N45" s="7" t="inlineStr">
@@ -4887,9 +4903,9 @@
           <t>CC - 8 (GCS239_2)</t>
         </is>
       </c>
-      <c r="J46" s="7" t="inlineStr">
-        <is>
-          <t>CC - 2 (GEN253_1) | CC - 2 (GEX605_3)</t>
+      <c r="J46" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 2 (GEN253_1) | CC - 2 (GEX605_3) </t>
         </is>
       </c>
       <c r="K46" s="7" t="inlineStr">
@@ -4897,14 +4913,14 @@
           <t>CC - 2 (GEX195_1)</t>
         </is>
       </c>
-      <c r="L46" s="7" t="inlineStr">
-        <is>
-          <t>CC - 2 (GEX055_1) | CC - 2 (GEX605_3)</t>
-        </is>
-      </c>
-      <c r="M46" s="7" t="inlineStr">
-        <is>
-          <t>CC - 2 (GEX055_1) | CC - 2 (GEX195_1)</t>
+      <c r="L46" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 2 (GEX055_1) | CC - 2 (GEX605_3) </t>
+        </is>
+      </c>
+      <c r="M46" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 2 (GEX055_1) | CC - 2 (GEX195_1) </t>
         </is>
       </c>
       <c r="N46" s="7" t="inlineStr">
@@ -4919,22 +4935,22 @@
       </c>
       <c r="P46" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX208_2)</t>
+          <t>CC - 3 (GEX392_1)</t>
         </is>
       </c>
       <c r="Q46" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX213_1)</t>
+          <t>CC - 2 (GLA104_2)</t>
         </is>
       </c>
       <c r="R46" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_1)</t>
+          <t>CC - opt (GEX1083_1)</t>
         </is>
       </c>
       <c r="S46" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX210_2)</t>
+          <t>CC - 3 (GEX609_1)</t>
         </is>
       </c>
       <c r="T46" s="7" t="inlineStr">
@@ -5924,7 +5940,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="9" t="n"/>
+      <c r="A57" s="10" t="n"/>
       <c r="B57" s="6" t="inlineStr">
         <is>
           <t>110-DE</t>

</xml_diff>

<commit_message>
Leve correção no agrupamento + anotações
</commit_message>
<xml_diff>
--- a/planilha_alocacoes.xlsx
+++ b/planilha_alocacoes.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -71,14 +71,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ab93f5"/>
-        <bgColor rgb="00ab93f5"/>
+        <fgColor rgb="00ff7b59"/>
+        <bgColor rgb="00ff7b59"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ff7b59"/>
-        <bgColor rgb="00ff7b59"/>
+        <fgColor rgb="00ab93f5"/>
+        <bgColor rgb="00ab93f5"/>
       </patternFill>
     </fill>
   </fills>
@@ -216,8 +216,8 @@
     <cellStyle name="estilo_header" xfId="1" hidden="0"/>
     <cellStyle name="estilo_index" xfId="2" hidden="0"/>
     <cellStyle name="compartilhamento" xfId="3" hidden="0"/>
-    <cellStyle name="agrupamento" xfId="4" hidden="0"/>
-    <cellStyle name="fusao" xfId="5" hidden="0"/>
+    <cellStyle name="fusao" xfId="4" hidden="0"/>
+    <cellStyle name="agrupamento" xfId="5" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -876,59 +876,59 @@
           <t>202-A</t>
         </is>
       </c>
-      <c r="C5" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D5" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E5" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F5" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G5" s="7" t="inlineStr">
-        <is>
-          <t>AGRO - opt (GCA675_1)</t>
+      <c r="C5" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - 8 (GCS253_1) | EAS - opt (GEN195_1) </t>
+        </is>
+      </c>
+      <c r="D5" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - 8 (GCS254_1) | EAS - 8 (GEN111_1) </t>
+        </is>
+      </c>
+      <c r="E5" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - 8 (GEN026_1) | EAS - 8 (GEN111_1) </t>
+        </is>
+      </c>
+      <c r="F5" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - 8 (GEN109_1) | EAS - 8 (GEN167_1) </t>
+        </is>
+      </c>
+      <c r="G5" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - 8 (GEN026_1) | EAS - 8 (GEN110_1) </t>
         </is>
       </c>
       <c r="H5" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - opt (GEN204_1)</t>
         </is>
       </c>
       <c r="I5" s="7" t="inlineStr">
         <is>
-          <t>EAS - 10 (GEN119_1)</t>
-        </is>
-      </c>
-      <c r="J5" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 6 (GCA286_1 - GCA286_2) </t>
+          <t>EAS - opt (GEN196_1)</t>
+        </is>
+      </c>
+      <c r="J5" s="7" t="inlineStr">
+        <is>
+          <t>EAS - opt (GEX458_1)</t>
         </is>
       </c>
       <c r="K5" s="7" t="inlineStr">
         <is>
-          <t>EAS - 9 (GEN113_1)</t>
+          <t>EAS - opt (GCA321_1)</t>
         </is>
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">EAS - 9 (GEN112_1) | EAS - 10 (GEN119_1) </t>
+          <t xml:space="preserve">EAS - 8 (GCS241_1) | EAS - opt (GEN204_1) </t>
         </is>
       </c>
       <c r="M5" s="7" t="inlineStr">
         <is>
-          <t>EAS - 10 (GEN119_1)</t>
+          <t>EAS - 10 (GEN118_1)</t>
         </is>
       </c>
       <c r="N5" s="7" t="inlineStr">
@@ -938,27 +938,27 @@
       </c>
       <c r="O5" s="7" t="inlineStr">
         <is>
-          <t>MAT - 4 (GEX979_1)</t>
-        </is>
-      </c>
-      <c r="P5" s="7" t="inlineStr">
-        <is>
-          <t>MAT - 4 (GEX978_1)</t>
+          <t>MAT - 6 (GEX984_1)</t>
+        </is>
+      </c>
+      <c r="P5" s="10" t="inlineStr">
+        <is>
+          <t>MAT - 6 + PED - 5 (GCH837_2)</t>
         </is>
       </c>
       <c r="Q5" s="7" t="inlineStr">
         <is>
-          <t>EAS - 10 (GEN119_1)</t>
+          <t>MAT - 6 (GEX985_1)</t>
         </is>
       </c>
       <c r="R5" s="7" t="inlineStr">
         <is>
-          <t>MAT - 4 (GEX977_1)</t>
+          <t>EAS - 8 (GCS241_1)</t>
         </is>
       </c>
       <c r="S5" s="7" t="inlineStr">
         <is>
-          <t>MAT - 4 (GEX976_1)</t>
+          <t>EAS - 10 (GEN118_1)</t>
         </is>
       </c>
       <c r="T5" s="7" t="inlineStr">
@@ -974,59 +974,59 @@
           <t>203-A</t>
         </is>
       </c>
-      <c r="C6" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 8 (GCS253_1) | EAS - opt (GEN195_1) </t>
-        </is>
-      </c>
-      <c r="D6" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 8 (GCS254_1) | EAS - 8 (GEN111_1) </t>
-        </is>
-      </c>
-      <c r="E6" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 8 (GEN026_1) | EAS - 8 (GEN111_1) </t>
-        </is>
-      </c>
-      <c r="F6" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 8 (GEN109_1) | EAS - 8 (GEN167_1) </t>
-        </is>
-      </c>
-      <c r="G6" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 8 (GEN026_1) | EAS - 8 (GEN110_1) </t>
+      <c r="C6" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D6" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E6" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F6" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G6" s="7" t="inlineStr">
+        <is>
+          <t>AGRO - 4 (GCA045_1)</t>
         </is>
       </c>
       <c r="H6" s="7" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN204_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I6" s="7" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN196_1)</t>
-        </is>
-      </c>
-      <c r="J6" s="7" t="inlineStr">
-        <is>
-          <t>EAS - opt (GEX458_1)</t>
+          <t>EAS - 10 (GEN119_1)</t>
+        </is>
+      </c>
+      <c r="J6" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 6 (GCA286_1 - GCA286_2) </t>
         </is>
       </c>
       <c r="K6" s="7" t="inlineStr">
         <is>
-          <t>EAS - opt (GCA321_1)</t>
-        </is>
-      </c>
-      <c r="L6" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 8 (GCS241_1) | EAS - opt (GEN204_1) </t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L6" s="7" t="inlineStr">
+        <is>
+          <t>EAS - 10 (GEN119_1)</t>
         </is>
       </c>
       <c r="M6" s="7" t="inlineStr">
         <is>
-          <t>EAS - 10 (GEN118_1)</t>
+          <t>EAS - 10 (GEN119_1)</t>
         </is>
       </c>
       <c r="N6" s="7" t="inlineStr">
@@ -1034,29 +1034,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O6" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MAT - 8 (GEX993_1 - GEX994_1) </t>
+      <c r="O6" s="7" t="inlineStr">
+        <is>
+          <t>MAT - 4 (GEX979_1)</t>
         </is>
       </c>
       <c r="P6" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MAT - 4 (GEX978_1)</t>
         </is>
       </c>
       <c r="Q6" s="7" t="inlineStr">
         <is>
-          <t>MAT - 8 (GEX991_1)</t>
+          <t>EAS - 10 (GEN119_1)</t>
         </is>
       </c>
       <c r="R6" s="7" t="inlineStr">
         <is>
-          <t>EAS - 8 (GCS241_1)</t>
+          <t>MAT - 4 (GEX977_1)</t>
         </is>
       </c>
       <c r="S6" s="7" t="inlineStr">
         <is>
-          <t>EAS - 10 (GEN118_1)</t>
+          <t>MAT - 4 (GEX976_1)</t>
         </is>
       </c>
       <c r="T6" s="7" t="inlineStr">
@@ -1114,12 +1114,12 @@
       </c>
       <c r="K7" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - 9 (GEN113_1)</t>
         </is>
       </c>
       <c r="L7" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - 9 (GEN112_1)</t>
         </is>
       </c>
       <c r="M7" s="7" t="inlineStr">
@@ -1134,17 +1134,17 @@
       </c>
       <c r="O7" s="7" t="inlineStr">
         <is>
-          <t>MAT - 6 (GEX984_1)</t>
-        </is>
-      </c>
-      <c r="P7" s="11" t="inlineStr">
-        <is>
-          <t>MAT - 6 + PED - 5 (GCH837_2)</t>
+          <t>MAT - 2 (GEX970_1)</t>
+        </is>
+      </c>
+      <c r="P7" s="7" t="inlineStr">
+        <is>
+          <t>MAT - 2 (GCH293_7)</t>
         </is>
       </c>
       <c r="Q7" s="7" t="inlineStr">
         <is>
-          <t>MAT - 6 (GEX985_1)</t>
+          <t>MAT - 2 (GEX509_1)</t>
         </is>
       </c>
       <c r="R7" s="7" t="inlineStr">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="S7" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MAT - 2 (GEX971_1)</t>
         </is>
       </c>
       <c r="T7" s="7" t="inlineStr">
@@ -1170,7 +1170,7 @@
           <t>205-A</t>
         </is>
       </c>
-      <c r="C8" s="11" t="inlineStr">
+      <c r="C8" s="10" t="inlineStr">
         <is>
           <t>EAS - 2 + PED - 2 (GCH291_1)</t>
         </is>
@@ -1230,19 +1230,19 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O8" s="7" t="inlineStr">
-        <is>
-          <t>MAT - 2 (GEX970_1)</t>
+      <c r="O8" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MAT - 8 (GEX993_1 - GEX994_1) </t>
         </is>
       </c>
       <c r="P8" s="7" t="inlineStr">
         <is>
-          <t>MAT - 2 (GCH293_7)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q8" s="7" t="inlineStr">
         <is>
-          <t>MAT - 2 (GEX509_1)</t>
+          <t>MAT - 8 (GEX991_1)</t>
         </is>
       </c>
       <c r="R8" s="7" t="inlineStr">
@@ -1252,7 +1252,7 @@
       </c>
       <c r="S8" s="7" t="inlineStr">
         <is>
-          <t>MAT - 2 (GEX971_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T8" s="7" t="inlineStr">
@@ -1305,12 +1305,12 @@
       </c>
       <c r="J9" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - 10 (GLA054_1)</t>
         </is>
       </c>
       <c r="K9" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - 10 (GLA041_1)</t>
         </is>
       </c>
       <c r="L9" s="7" t="inlineStr">
@@ -1330,27 +1330,27 @@
       </c>
       <c r="O9" s="7" t="inlineStr">
         <is>
-          <t>LET - 2 (GCS238_4)</t>
-        </is>
-      </c>
-      <c r="P9" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 2 (GCH290_14 - GLA358_1) </t>
+          <t>LET - 10 (GLA043_1)</t>
+        </is>
+      </c>
+      <c r="P9" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="Q9" s="7" t="inlineStr">
         <is>
-          <t>LET - 2 (GLA359_1)</t>
+          <t>LET - 10 (GLA041_1)</t>
         </is>
       </c>
       <c r="R9" s="7" t="inlineStr">
         <is>
-          <t>LET - 2 (GCH293_5)</t>
+          <t>LET - 10 (GLA041_1)</t>
         </is>
       </c>
       <c r="S9" s="7" t="inlineStr">
         <is>
-          <t>LET - 2 (GLA360_1)</t>
+          <t>LET - 10 (GLA059_1)</t>
         </is>
       </c>
       <c r="T9" s="7" t="inlineStr">
@@ -1391,24 +1391,24 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H10" s="7" t="inlineStr">
-        <is>
-          <t>LET - opt (GLA168_1)</t>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="H10" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 6 (GLA373_1 - GLA376_1) </t>
+        </is>
+      </c>
+      <c r="I10" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 6 (GLA374_1 - GLA375_1) </t>
         </is>
       </c>
       <c r="J10" s="7" t="inlineStr">
         <is>
-          <t>LET - 9 (GLA061_1)</t>
-        </is>
-      </c>
-      <c r="K10" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - opt (GLA104_5 - GLA552_1) </t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K10" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="L10" s="7" t="inlineStr">
@@ -1421,34 +1421,34 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N10" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O10" s="7" t="inlineStr">
-        <is>
-          <t>LET - opt (GEX212_3)</t>
+      <c r="N10" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 6 (GLA373_1 - GLA376_1) </t>
+        </is>
+      </c>
+      <c r="O10" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 6 (GLA374_1 - GLA375_1) </t>
         </is>
       </c>
       <c r="P10" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - 6 (GLA378_1)</t>
         </is>
       </c>
       <c r="Q10" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GLA168_1)</t>
+          <t>LET - 6 (GCH1031_2)</t>
         </is>
       </c>
       <c r="R10" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GLA528_1)</t>
-        </is>
-      </c>
-      <c r="S10" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>LET - 6 (GLA377_1)</t>
+        </is>
+      </c>
+      <c r="S10" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 6 (GLA373_1 - GLA376_1) </t>
         </is>
       </c>
       <c r="T10" s="7" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="D11" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 2 (GEX212_1)</t>
         </is>
       </c>
       <c r="E11" s="7" t="inlineStr">
@@ -1496,22 +1496,22 @@
       </c>
       <c r="I11" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 2 (GCB064_1)</t>
         </is>
       </c>
       <c r="J11" s="7" t="inlineStr">
         <is>
-          <t>LET - 10 (GLA054_1)</t>
+          <t>ENF - 4 (GSA014_1)</t>
         </is>
       </c>
       <c r="K11" s="7" t="inlineStr">
         <is>
-          <t>LET - 10 (GLA041_1)</t>
+          <t>ENF - 4 (GSA012_1)</t>
         </is>
       </c>
       <c r="L11" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 2 (GCB019_1)</t>
         </is>
       </c>
       <c r="M11" s="7" t="inlineStr">
@@ -1524,9 +1524,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O11" s="7" t="inlineStr">
-        <is>
-          <t>LET - 10 (GLA043_1)</t>
+      <c r="O11" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 4 (GLA365_1 - GLA367_1) </t>
         </is>
       </c>
       <c r="P11" s="7" t="inlineStr">
@@ -1536,17 +1536,17 @@
       </c>
       <c r="Q11" s="7" t="inlineStr">
         <is>
-          <t>LET - 10 (GLA041_1)</t>
+          <t>LET - 4 (GLA366_1)</t>
         </is>
       </c>
       <c r="R11" s="7" t="inlineStr">
         <is>
-          <t>LET - 10 (GLA041_1)</t>
+          <t>LET - 4 (GLA368_1)</t>
         </is>
       </c>
       <c r="S11" s="7" t="inlineStr">
         <is>
-          <t>LET - 10 (GLA059_1)</t>
+          <t>LET - 4 (GLA364_1)</t>
         </is>
       </c>
       <c r="T11" s="7" t="inlineStr">
@@ -1594,27 +1594,27 @@
       </c>
       <c r="I12" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA552_1)</t>
         </is>
       </c>
       <c r="J12" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA552_1)</t>
         </is>
       </c>
       <c r="K12" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA552_1)</t>
         </is>
       </c>
       <c r="L12" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA552_1)</t>
         </is>
       </c>
       <c r="M12" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA552_1)</t>
         </is>
       </c>
       <c r="N12" s="7" t="inlineStr">
@@ -1624,27 +1624,27 @@
       </c>
       <c r="O12" s="7" t="inlineStr">
         <is>
-          <t>LET - 8 (GLA391_1)</t>
-        </is>
-      </c>
-      <c r="P12" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 8 (GLA388_1 - GLA389_1) </t>
+          <t>LET - 2 (GCS238_4)</t>
+        </is>
+      </c>
+      <c r="P12" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 2 (GCH290_14 - GLA358_1) </t>
         </is>
       </c>
       <c r="Q12" s="7" t="inlineStr">
         <is>
-          <t>LET - 8 (GLA390_1)</t>
+          <t>LET - 2 (GLA359_1)</t>
         </is>
       </c>
       <c r="R12" s="7" t="inlineStr">
         <is>
-          <t>LET - 8 (GLA392_1)</t>
+          <t>LET - 2 (GCH293_5)</t>
         </is>
       </c>
       <c r="S12" s="7" t="inlineStr">
         <is>
-          <t>LET - 8 (GLA387_1)</t>
+          <t>LET - 2 (GLA360_1)</t>
         </is>
       </c>
       <c r="T12" s="7" t="inlineStr">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="H13" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA168_1)</t>
         </is>
       </c>
       <c r="I13" s="7" t="inlineStr">
@@ -1697,12 +1697,12 @@
       </c>
       <c r="J13" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - 9 (GLA061_1)</t>
         </is>
       </c>
       <c r="K13" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA104_5)</t>
         </is>
       </c>
       <c r="L13" s="7" t="inlineStr">
@@ -1720,9 +1720,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O13" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 4 (GLA365_1 - GLA367_1) </t>
+      <c r="O13" s="7" t="inlineStr">
+        <is>
+          <t>LET - opt (GEX212_3)</t>
         </is>
       </c>
       <c r="P13" s="7" t="inlineStr">
@@ -1732,17 +1732,17 @@
       </c>
       <c r="Q13" s="7" t="inlineStr">
         <is>
-          <t>LET - 4 (GLA366_1)</t>
+          <t>LET - opt (GLA168_1)</t>
         </is>
       </c>
       <c r="R13" s="7" t="inlineStr">
         <is>
-          <t>LET - 4 (GLA368_1)</t>
+          <t>LET - opt (GLA528_1)</t>
         </is>
       </c>
       <c r="S13" s="7" t="inlineStr">
         <is>
-          <t>LET - 4 (GLA364_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T13" s="7" t="inlineStr">
@@ -1758,64 +1758,64 @@
           <t>301-A</t>
         </is>
       </c>
-      <c r="C14" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 2 (GCA218_1) | AGRO - 3 (GCB030_1) </t>
+      <c r="C14" s="7" t="inlineStr">
+        <is>
+          <t>AGRO - 6 (GCA250_1)</t>
         </is>
       </c>
       <c r="D14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E14" s="7" t="inlineStr">
-        <is>
-          <t>AGRO - 2 (GCB107_1)</t>
-        </is>
-      </c>
-      <c r="F14" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 2 (GCA210_3 - GCA210_4)  | AGRO - 2 (GCB056_4 - GCB056_5)  </t>
-        </is>
-      </c>
-      <c r="G14" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 2 (GEX190_1 - GEX190_2) </t>
+          <t>AGRO - 6 (GCA025_1)</t>
+        </is>
+      </c>
+      <c r="E14" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 6 (GCA239_1) | AGRO - 6 (GCB054_1) </t>
+        </is>
+      </c>
+      <c r="F14" s="7" t="inlineStr">
+        <is>
+          <t>AGRO - 6 (GEX080_1)</t>
+        </is>
+      </c>
+      <c r="G14" s="7" t="inlineStr">
+        <is>
+          <t>AGRO - opt (GCA655_1)</t>
         </is>
       </c>
       <c r="H14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 10 (GCA283_1)</t>
         </is>
       </c>
       <c r="I14" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">AGRO - 3 (GCS005_1) | MED - opt (GSA299_1) </t>
-        </is>
-      </c>
-      <c r="J14" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 2 (GCB056_4 - GCB056_5) </t>
+          <t xml:space="preserve">AGRO - 6 (GCS243_1) | MED - opt (GSA299_1) </t>
+        </is>
+      </c>
+      <c r="J14" s="7" t="inlineStr">
+        <is>
+          <t>AGRO - 10 (GCA283_1)</t>
         </is>
       </c>
       <c r="K14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 6 (GCA241_1)</t>
         </is>
       </c>
       <c r="L14" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 1 (GCH292_3)</t>
-        </is>
-      </c>
-      <c r="M14" s="7" t="inlineStr">
-        <is>
-          <t>AGRO - 2 (GEX179_1)</t>
+          <t>AGRO - 6 (GCA050_1)</t>
+        </is>
+      </c>
+      <c r="M14" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 9 (GCA282_1) | AGRO - 7 (GCA287_1) </t>
         </is>
       </c>
       <c r="N14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 10 (GCA283_1)</t>
         </is>
       </c>
       <c r="O14" s="7" t="inlineStr">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="P14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 7 (GCA225_1)</t>
         </is>
       </c>
       <c r="Q14" s="7" t="inlineStr">
@@ -1840,12 +1840,12 @@
       </c>
       <c r="S14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 9 (GCA282_1)</t>
         </is>
       </c>
       <c r="T14" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 10 (GCA283_1)</t>
         </is>
       </c>
     </row>
@@ -1856,64 +1856,64 @@
           <t>302-A</t>
         </is>
       </c>
-      <c r="C15" s="7" t="inlineStr">
-        <is>
-          <t>AGRO - 6 (GCA250_1)</t>
+      <c r="C15" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 2 (GCA218_1) | AGRO - 3 (GCB030_1) </t>
         </is>
       </c>
       <c r="D15" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 6 (GCA025_1)</t>
-        </is>
-      </c>
-      <c r="E15" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 6 (GCA239_1) | AGRO - 6 (GCB054_1) </t>
-        </is>
-      </c>
-      <c r="F15" s="7" t="inlineStr">
-        <is>
-          <t>AGRO - 6 (GEX080_1)</t>
-        </is>
-      </c>
-      <c r="G15" s="7" t="inlineStr">
-        <is>
-          <t>AGRO - opt (GCA655_1)</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E15" s="7" t="inlineStr">
+        <is>
+          <t>AGRO - 2 (GCB107_1)</t>
+        </is>
+      </c>
+      <c r="F15" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 2 (GCA210_3 - GCA210_4)  | AGRO - 2 (GCB056_4 - GCB056_5)  </t>
+        </is>
+      </c>
+      <c r="G15" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 2 (GEX190_1 - GEX190_2) </t>
         </is>
       </c>
       <c r="H15" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 10 (GCA283_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I15" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 6 (GCS243_1)</t>
-        </is>
-      </c>
-      <c r="J15" s="7" t="inlineStr">
-        <is>
-          <t>AGRO - 10 (GCA283_1)</t>
+          <t>AGRO - 3 (GCS005_1)</t>
+        </is>
+      </c>
+      <c r="J15" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 2 (GCB056_4 - GCB056_5) </t>
         </is>
       </c>
       <c r="K15" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 6 (GCA241_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L15" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 6 (GCA050_1)</t>
-        </is>
-      </c>
-      <c r="M15" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 9 (GCA282_1) | AGRO - 7 (GCA287_1) </t>
+          <t>AGRO - 1 (GCH292_3)</t>
+        </is>
+      </c>
+      <c r="M15" s="7" t="inlineStr">
+        <is>
+          <t>AGRO - 2 (GEX179_1)</t>
         </is>
       </c>
       <c r="N15" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 10 (GCA283_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O15" s="7" t="inlineStr">
@@ -1923,7 +1923,7 @@
       </c>
       <c r="P15" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 7 (GCA225_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q15" s="7" t="inlineStr">
@@ -1938,12 +1938,12 @@
       </c>
       <c r="S15" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 9 (GCA282_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T15" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 10 (GCA283_1)</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1954,7 +1954,7 @@
           <t>303-A</t>
         </is>
       </c>
-      <c r="C16" s="10" t="inlineStr">
+      <c r="C16" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">AGRO - 4 (GCA210_1 - GCA210_2) </t>
         </is>
@@ -1969,14 +1969,14 @@
           <t xml:space="preserve">AGRO - 4 (GCA218_2) | AGRO - 4 (GCB130_1) </t>
         </is>
       </c>
-      <c r="F16" s="10" t="inlineStr">
+      <c r="F16" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">AGRO - 4 (GCA037_1 - GCA037_2) </t>
         </is>
       </c>
       <c r="G16" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">AGRO - opt (GCA312_1) | AGRO - opt (GCA588_1) </t>
+          <t xml:space="preserve">AGRO - opt (GCA312_1) | AGRO - opt (GCA675_1) </t>
         </is>
       </c>
       <c r="H16" s="7" t="inlineStr">
@@ -1984,7 +1984,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I16" s="10" t="inlineStr">
+      <c r="I16" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">AGRO - 4 (GEX116_1 - GEX116_2) </t>
         </is>
@@ -2014,7 +2014,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O16" s="10" t="inlineStr">
+      <c r="O16" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">CS - 2 (GCH1325_1 - GLA102_1) </t>
         </is>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="G18" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 4 (GCA045_1)</t>
+          <t>AGRO - opt (GCA588_1)</t>
         </is>
       </c>
       <c r="H18" s="7" t="inlineStr">
@@ -2220,7 +2220,7 @@
           <t>CS - 8 (GCH1410_1)</t>
         </is>
       </c>
-      <c r="Q18" s="10" t="inlineStr">
+      <c r="Q18" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">CS - opt (GCH1420_1 - GCH1433_1) </t>
         </is>
@@ -2250,22 +2250,22 @@
       </c>
       <c r="C19" s="7" t="inlineStr">
         <is>
-          <t>ENF - 8 (GSA024_1)</t>
+          <t>HIS - 6 (GCH382_1)</t>
         </is>
       </c>
       <c r="D19" s="7" t="inlineStr">
         <is>
-          <t>ENF - 8 (GSA011_1)</t>
+          <t>ENF - 10 (GSA049_1)</t>
         </is>
       </c>
       <c r="E19" s="7" t="inlineStr">
         <is>
-          <t>ENF - 8 (GSA011_1)</t>
+          <t>ENF - 2 (GSA0304_1)</t>
         </is>
       </c>
       <c r="F19" s="7" t="inlineStr">
         <is>
-          <t>ENF - 8 (GSA024_1)</t>
+          <t>ENF - 2 (GSA0305_1)</t>
         </is>
       </c>
       <c r="G19" s="7" t="inlineStr">
@@ -2275,32 +2275,32 @@
       </c>
       <c r="H19" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 6 (GCH381_1)</t>
         </is>
       </c>
       <c r="I19" s="7" t="inlineStr">
         <is>
-          <t>ENF - 8 (GSA025_1)</t>
+          <t>ENF - 10 (GSA047_1)</t>
         </is>
       </c>
       <c r="J19" s="7" t="inlineStr">
         <is>
-          <t>ENF - 8 (GSA024_1)</t>
+          <t>ENF - 10 (GSA047_1)</t>
         </is>
       </c>
       <c r="K19" s="7" t="inlineStr">
         <is>
-          <t>ENF - 8 (GSA023_1)</t>
+          <t>ENF - 10 (GSA047_1)</t>
         </is>
       </c>
       <c r="L19" s="7" t="inlineStr">
         <is>
-          <t>ENF - 8 (GSA011_1)</t>
+          <t>ENF - 10 (GSA047_1)</t>
         </is>
       </c>
       <c r="M19" s="7" t="inlineStr">
         <is>
-          <t>ENF - 8 (GSA023_1)</t>
+          <t>ENF - 10 (GSA047_1)</t>
         </is>
       </c>
       <c r="N19" s="7" t="inlineStr">
@@ -2310,27 +2310,27 @@
       </c>
       <c r="O19" s="7" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH290_15)</t>
+          <t>HIS - 6 (GCH382_1)</t>
         </is>
       </c>
       <c r="P19" s="7" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH291_3)</t>
+          <t>HIS - 7 (GLA108_1)</t>
         </is>
       </c>
       <c r="Q19" s="7" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH366_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R19" s="7" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH365_1)</t>
+          <t>HIS - 6 (GCH381_1)</t>
         </is>
       </c>
       <c r="S19" s="7" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH367_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T19" s="7" t="inlineStr">
@@ -2348,22 +2348,22 @@
       </c>
       <c r="C20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GCB064_2)</t>
+          <t>ENF - 6 (GSA021_1)</t>
         </is>
       </c>
       <c r="D20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GSA017_1)</t>
+          <t>ENF - 6 (GSA021_1)</t>
         </is>
       </c>
       <c r="E20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GSA017_1)</t>
+          <t>ENF - 6 (GSA021_1)</t>
         </is>
       </c>
       <c r="F20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GSA017_1)</t>
+          <t>ENF - 6 (GSA021_1)</t>
         </is>
       </c>
       <c r="G20" s="7" t="inlineStr">
@@ -2378,27 +2378,27 @@
       </c>
       <c r="I20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 2 (GCB064_1)</t>
+          <t>ENF - 6 (GSA021_1)</t>
         </is>
       </c>
       <c r="J20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 2 (GSA0303_1)</t>
+          <t>ENF - 6 (GSA044_1)</t>
         </is>
       </c>
       <c r="K20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 2 (GSA0303_1)</t>
+          <t>ENF - 6 (GSA021_1)</t>
         </is>
       </c>
       <c r="L20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 2 (GCB019_1)</t>
+          <t>ENF - 6 (GSA044_1)</t>
         </is>
       </c>
       <c r="M20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GCB019_2)</t>
+          <t>ENF - 6 (GSA021_1)</t>
         </is>
       </c>
       <c r="N20" s="7" t="inlineStr">
@@ -2408,27 +2408,27 @@
       </c>
       <c r="O20" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 2 (GCH290_15)</t>
         </is>
       </c>
       <c r="P20" s="7" t="inlineStr">
         <is>
-          <t>HIS - 4 (GCH372_1)</t>
+          <t>HIS - 2 (GCH291_3)</t>
         </is>
       </c>
       <c r="Q20" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 2 (GCH366_1)</t>
         </is>
       </c>
       <c r="R20" s="7" t="inlineStr">
         <is>
-          <t>HIS - 4 (GCH371_1)</t>
+          <t>HIS - 2 (GCH365_1)</t>
         </is>
       </c>
       <c r="S20" s="7" t="inlineStr">
         <is>
-          <t>HIS - 4 (GCH373_1)</t>
+          <t>HIS - 2 (GCH367_1)</t>
         </is>
       </c>
       <c r="T20" s="7" t="inlineStr">
@@ -2446,22 +2446,22 @@
       </c>
       <c r="C21" s="7" t="inlineStr">
         <is>
-          <t>HIS - 6 (GCH382_1)</t>
+          <t>ENF - 4 (GCB064_2)</t>
         </is>
       </c>
       <c r="D21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 2 (GEX212_1)</t>
+          <t>ENF - 4 (GSA017_1)</t>
         </is>
       </c>
       <c r="E21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 2 (GSA0304_1)</t>
+          <t>ENF - 4 (GSA017_1)</t>
         </is>
       </c>
       <c r="F21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 2 (GSA0305_1)</t>
+          <t>ENF - 4 (GSA017_1)</t>
         </is>
       </c>
       <c r="G21" s="7" t="inlineStr">
@@ -2471,32 +2471,32 @@
       </c>
       <c r="H21" s="7" t="inlineStr">
         <is>
-          <t>HIS - 6 (GCH381_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>ENF - 4 (GCH012_2)</t>
         </is>
       </c>
       <c r="J21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>ENF - 2 (GSA0303_1)</t>
         </is>
       </c>
       <c r="K21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
-        </is>
-      </c>
-      <c r="L21" s="7" t="inlineStr">
-        <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>ENF - 2 (GSA0303_1)</t>
+        </is>
+      </c>
+      <c r="L21" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ENF - 4 (GCB029_1 - GCB076_1) </t>
         </is>
       </c>
       <c r="M21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>ENF - 4 (GCB019_2)</t>
         </is>
       </c>
       <c r="N21" s="7" t="inlineStr">
@@ -2506,12 +2506,12 @@
       </c>
       <c r="O21" s="7" t="inlineStr">
         <is>
-          <t>HIS - 6 (GCH382_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P21" s="7" t="inlineStr">
         <is>
-          <t>HIS - 7 (GLA108_1)</t>
+          <t>HIS - 4 (GCH372_1)</t>
         </is>
       </c>
       <c r="Q21" s="7" t="inlineStr">
@@ -2521,12 +2521,12 @@
       </c>
       <c r="R21" s="7" t="inlineStr">
         <is>
-          <t>HIS - 6 (GCH381_1)</t>
+          <t>HIS - 4 (GCH371_1)</t>
         </is>
       </c>
       <c r="S21" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 4 (GCH373_1)</t>
         </is>
       </c>
       <c r="T21" s="7" t="inlineStr">
@@ -2544,22 +2544,22 @@
       </c>
       <c r="C22" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA021_1)</t>
+          <t>ENF - 8 (GSA024_1)</t>
         </is>
       </c>
       <c r="D22" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA021_1)</t>
+          <t>ENF - 8 (GSA011_1)</t>
         </is>
       </c>
       <c r="E22" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA021_1)</t>
+          <t>ENF - 8 (GSA011_1)</t>
         </is>
       </c>
       <c r="F22" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA021_1)</t>
+          <t>ENF - 8 (GSA024_1)</t>
         </is>
       </c>
       <c r="G22" s="7" t="inlineStr">
@@ -2567,64 +2567,64 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H22" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 6 (GLA373_1 - GLA376_1) </t>
-        </is>
-      </c>
-      <c r="I22" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ENF - 6 (GSA021_1) | LET - 6 (GLA374_1 - GLA375_1)  </t>
+      <c r="H22" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I22" s="7" t="inlineStr">
+        <is>
+          <t>ENF - 8 (GSA025_1)</t>
         </is>
       </c>
       <c r="J22" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA044_1)</t>
+          <t>ENF - 8 (GSA024_1)</t>
         </is>
       </c>
       <c r="K22" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA021_1)</t>
+          <t>ENF - 8 (GSA023_1)</t>
         </is>
       </c>
       <c r="L22" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA044_1)</t>
+          <t>ENF - 8 (GSA011_1)</t>
         </is>
       </c>
       <c r="M22" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA021_1)</t>
-        </is>
-      </c>
-      <c r="N22" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 6 (GLA373_1 - GLA376_1) </t>
-        </is>
-      </c>
-      <c r="O22" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 6 (GLA374_1 - GLA375_1) </t>
-        </is>
-      </c>
-      <c r="P22" s="7" t="inlineStr">
-        <is>
-          <t>LET - 6 (GLA378_1)</t>
+          <t>ENF - 8 (GSA023_1)</t>
+        </is>
+      </c>
+      <c r="N22" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O22" s="7" t="inlineStr">
+        <is>
+          <t>LET - 8 (GLA391_1)</t>
+        </is>
+      </c>
+      <c r="P22" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 8 (GLA388_1 - GLA389_1) </t>
         </is>
       </c>
       <c r="Q22" s="7" t="inlineStr">
         <is>
-          <t>LET - 6 (GCH1031_2)</t>
+          <t>LET - 8 (GLA390_1)</t>
         </is>
       </c>
       <c r="R22" s="7" t="inlineStr">
         <is>
-          <t>LET - 6 (GLA377_1)</t>
-        </is>
-      </c>
-      <c r="S22" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 6 (GLA373_1 - GLA376_1) </t>
+          <t>LET - 8 (GLA392_1)</t>
+        </is>
+      </c>
+      <c r="S22" s="7" t="inlineStr">
+        <is>
+          <t>LET - 8 (GLA387_1)</t>
         </is>
       </c>
       <c r="T22" s="7" t="inlineStr">
@@ -2700,29 +2700,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="O23" s="10" t="inlineStr">
+        <is>
+          <t>CS - 8 + HIS - 4 (GCS238_5)</t>
         </is>
       </c>
       <c r="P23" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>CS - 4 (GCH1397_1)</t>
+        </is>
+      </c>
+      <c r="Q23" s="10" t="inlineStr">
+        <is>
+          <t>CS - 4 + FIL - 4 + MAT - 4 (GCH838_1)</t>
+        </is>
+      </c>
+      <c r="R23" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CS - 8 (GCH1457_1 - GCH1460_1) </t>
+        </is>
+      </c>
+      <c r="S23" s="10" t="inlineStr">
+        <is>
+          <t>CS - 8 + MAT - 6 + PED - 7 (GCH1031_1)</t>
         </is>
       </c>
       <c r="T23" s="7" t="inlineStr">
@@ -2745,7 +2745,7 @@
       </c>
       <c r="D24" s="7" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA049_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E24" s="7" t="inlineStr">
@@ -2770,22 +2770,22 @@
       </c>
       <c r="I24" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GCH012_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J24" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GSA014_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K24" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GSA012_1)</t>
-        </is>
-      </c>
-      <c r="L24" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ENF - 4 (GCB029_1 - GCB076_1) </t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="M24" s="7" t="inlineStr">
@@ -2798,29 +2798,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O24" s="11" t="inlineStr">
-        <is>
-          <t>CS - 8 + HIS - 4 (GCS238_5)</t>
+      <c r="O24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="P24" s="7" t="inlineStr">
         <is>
-          <t>CS - 4 (GCH1397_1)</t>
-        </is>
-      </c>
-      <c r="Q24" s="11" t="inlineStr">
-        <is>
-          <t>CS - 4 + FIL - 4 + MAT - 4 (GCH838_1)</t>
-        </is>
-      </c>
-      <c r="R24" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CS - 8 (GCH1457_1 - GCH1460_1) </t>
-        </is>
-      </c>
-      <c r="S24" s="11" t="inlineStr">
-        <is>
-          <t>CS - 8 + MAT - 6 + PED - 7 (GCH1031_1)</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="T24" s="7" t="inlineStr">
@@ -2906,7 +2906,7 @@
           <t>LET - opt (GCS239_10)</t>
         </is>
       </c>
-      <c r="Q25" s="10" t="inlineStr">
+      <c r="Q25" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">LET - opt (GCH293_4 - GLA004_3) </t>
         </is>
@@ -3011,7 +3011,7 @@
       </c>
       <c r="R26" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_1)</t>
+          <t>CC - 1 (GEX003_2)</t>
         </is>
       </c>
       <c r="S26" s="7" t="inlineStr">
@@ -3054,7 +3054,7 @@
       </c>
       <c r="G27" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 6 (GCH1116_1)</t>
         </is>
       </c>
       <c r="H27" s="7" t="inlineStr">
@@ -3250,7 +3250,7 @@
       </c>
       <c r="G29" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 8 (GCH1126_1)</t>
         </is>
       </c>
       <c r="H29" s="7" t="inlineStr">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="I29" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 2 (GEN253_1)</t>
         </is>
       </c>
       <c r="J29" s="7" t="inlineStr">
@@ -3290,17 +3290,17 @@
       </c>
       <c r="O29" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX098_2)</t>
+          <t>CC - 3 (GEX098_1)</t>
         </is>
       </c>
       <c r="P29" s="7" t="inlineStr">
         <is>
-          <t>ADM - 5 (GCS540_1)</t>
+          <t>ADM - 9 (GCS549_1)</t>
         </is>
       </c>
       <c r="Q29" s="7" t="inlineStr">
         <is>
-          <t>ADM - 5 (GCS536_1)</t>
+          <t>ADM - 9 (GCS551_1)</t>
         </is>
       </c>
       <c r="R29" s="7" t="inlineStr">
@@ -3310,7 +3310,7 @@
       </c>
       <c r="S29" s="7" t="inlineStr">
         <is>
-          <t>ADM - 5 (GCS539_1)</t>
+          <t>ADM - 9 (GCS573_1)</t>
         </is>
       </c>
       <c r="T29" s="7" t="inlineStr">
@@ -3328,32 +3328,32 @@
       </c>
       <c r="C30" s="7" t="inlineStr">
         <is>
-          <t>PED - 10 (GCH1133_1)</t>
+          <t>PED - 6 (GLA239_1)</t>
         </is>
       </c>
       <c r="D30" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E30" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - opt (GCH1302_1 - GCH1303_1) </t>
-        </is>
-      </c>
-      <c r="F30" s="7" t="inlineStr">
-        <is>
-          <t>PED - 10 (GCS238_3)</t>
-        </is>
-      </c>
-      <c r="G30" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 10 (GCH1132_1 - GCH1134_1) </t>
-        </is>
-      </c>
-      <c r="H30" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 7 (GCH1117_1 - GCH1120_1) </t>
+          <t>PED - 6 (GCH1112_1)</t>
+        </is>
+      </c>
+      <c r="E30" s="7" t="inlineStr">
+        <is>
+          <t>PED - 6 (GLA238_1)</t>
+        </is>
+      </c>
+      <c r="F30" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 6 (GCH1114_1 - GCH1115_1) </t>
+        </is>
+      </c>
+      <c r="G30" s="7" t="inlineStr">
+        <is>
+          <t>PED - 6 (GCH1113_1)</t>
+        </is>
+      </c>
+      <c r="H30" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="I30" s="7" t="inlineStr">
@@ -3381,34 +3381,34 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N30" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 7 (GCH1117_1 - GCH1120_1) </t>
+      <c r="N30" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="O30" s="7" t="inlineStr">
         <is>
-          <t>PED - 7 (GLA213_1)</t>
-        </is>
-      </c>
-      <c r="P30" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 7 (GCH1118_1 - GEX776_1) </t>
-        </is>
-      </c>
-      <c r="Q30" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 7 (GCH1117_1 - GCH1120_1) </t>
-        </is>
-      </c>
-      <c r="R30" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 7 (GCH160_1 - GLA240_1) </t>
-        </is>
-      </c>
-      <c r="S30" s="7" t="inlineStr">
-        <is>
-          <t>PED - opt (GCH1284_1)</t>
+          <t>PED - 5 (GLA237_1)</t>
+        </is>
+      </c>
+      <c r="P30" s="7" t="inlineStr">
+        <is>
+          <t>PED - 5 (GCH1111_1)</t>
+        </is>
+      </c>
+      <c r="Q30" s="7" t="inlineStr">
+        <is>
+          <t>PED - 5 (GCH1110_1)</t>
+        </is>
+      </c>
+      <c r="R30" s="7" t="inlineStr">
+        <is>
+          <t>PED - 5 (GCH1107_1)</t>
+        </is>
+      </c>
+      <c r="S30" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 5 (GCH1108_1 - GCH1109_1) </t>
         </is>
       </c>
       <c r="T30" s="7" t="inlineStr">
@@ -3429,7 +3429,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D31" s="10" t="inlineStr">
+      <c r="D31" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">PED - 2 (GCH1038_1 - GCH1039_1) </t>
         </is>
@@ -3484,7 +3484,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O31" s="10" t="inlineStr">
+      <c r="O31" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">PED - 1 (GCH1036_1 - GCH1100_1) </t>
         </is>
@@ -3524,32 +3524,32 @@
       </c>
       <c r="C32" s="7" t="inlineStr">
         <is>
-          <t>PED - 6 (GLA239_1)</t>
+          <t>PED - 10 (GCH1133_1)</t>
         </is>
       </c>
       <c r="D32" s="7" t="inlineStr">
         <is>
-          <t>PED - 6 (GCH1112_1)</t>
-        </is>
-      </c>
-      <c r="E32" s="7" t="inlineStr">
-        <is>
-          <t>PED - 6 (GLA238_1)</t>
-        </is>
-      </c>
-      <c r="F32" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 6 (GCH1114_1 - GCH1115_1) </t>
-        </is>
-      </c>
-      <c r="G32" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 6 (GCH1113_1 - GCH1116_1) </t>
-        </is>
-      </c>
-      <c r="H32" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - opt (GCH1302_1 - GCH1303_1) </t>
+        </is>
+      </c>
+      <c r="F32" s="7" t="inlineStr">
+        <is>
+          <t>PED - 10 (GCS238_3)</t>
+        </is>
+      </c>
+      <c r="G32" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 10 (GCH1132_1 - GCH1134_1) </t>
+        </is>
+      </c>
+      <c r="H32" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 7 (GCH1117_1 - GCH1120_1) </t>
         </is>
       </c>
       <c r="I32" s="7" t="inlineStr">
@@ -3577,34 +3577,34 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N32" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="N32" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 7 (GCH1117_1 - GCH1120_1) </t>
         </is>
       </c>
       <c r="O32" s="7" t="inlineStr">
         <is>
-          <t>PED - 3 (GCH1086_1)</t>
-        </is>
-      </c>
-      <c r="P32" s="7" t="inlineStr">
-        <is>
-          <t>PED - 3 (GCH1087_1)</t>
-        </is>
-      </c>
-      <c r="Q32" s="7" t="inlineStr">
-        <is>
-          <t>PED - 3 (GCH833_2)</t>
-        </is>
-      </c>
-      <c r="R32" s="7" t="inlineStr">
-        <is>
-          <t>PED - 3 (GCH840_2)</t>
-        </is>
-      </c>
-      <c r="S32" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 3 (GCH1088_1 - GCH1099_1) </t>
+          <t>PED - 7 (GLA213_1)</t>
+        </is>
+      </c>
+      <c r="P32" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 7 (GCH1118_1 - GEX776_1) </t>
+        </is>
+      </c>
+      <c r="Q32" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 7 (GCH1117_1 - GCH1120_1) </t>
+        </is>
+      </c>
+      <c r="R32" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 7 (GCH160_1 - GLA240_1) </t>
+        </is>
+      </c>
+      <c r="S32" s="7" t="inlineStr">
+        <is>
+          <t>PED - opt (GCH1284_1)</t>
         </is>
       </c>
       <c r="T32" s="7" t="inlineStr">
@@ -3620,7 +3620,7 @@
           <t>205-B</t>
         </is>
       </c>
-      <c r="C33" s="10" t="inlineStr">
+      <c r="C33" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">PED - 4 (GCH1102_1 - GCH1106_1) </t>
         </is>
@@ -3630,7 +3630,7 @@
           <t>PED - 4 (GCH838_2)</t>
         </is>
       </c>
-      <c r="E33" s="10" t="inlineStr">
+      <c r="E33" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">PED - 4 (GCH1104_1 - GCH1105_1) </t>
         </is>
@@ -3645,7 +3645,7 @@
           <t>PED - 4 (GEX210_4)</t>
         </is>
       </c>
-      <c r="H33" s="10" t="inlineStr">
+      <c r="H33" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">PED - 9 (GCH1128_1 - GCH1131_1) </t>
         </is>
@@ -3675,7 +3675,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N33" s="10" t="inlineStr">
+      <c r="N33" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">PED - 9 (GCH1128_1 - GCH1131_1) </t>
         </is>
@@ -3685,12 +3685,12 @@
           <t>PED - 9 (GCH1130_1)</t>
         </is>
       </c>
-      <c r="P33" s="10" t="inlineStr">
+      <c r="P33" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">PED - 9 (GCH1128_1 - GCH1131_1) </t>
         </is>
       </c>
-      <c r="Q33" s="10" t="inlineStr">
+      <c r="Q33" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">PED - 9 (GCH1129_1 - GCH1279_1) </t>
         </is>
@@ -3738,9 +3738,9 @@
           <t>PED - 8 (GCH1124_1)</t>
         </is>
       </c>
-      <c r="G34" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 8 (GCH1122_1 - GCH1126_1) </t>
+      <c r="G34" s="7" t="inlineStr">
+        <is>
+          <t>PED - 8 (GCH1122_1)</t>
         </is>
       </c>
       <c r="H34" s="7" t="inlineStr">
@@ -3780,27 +3780,27 @@
       </c>
       <c r="O34" s="7" t="inlineStr">
         <is>
-          <t>PED - 5 (GLA237_1)</t>
+          <t>PED - 3 (GCH1086_1)</t>
         </is>
       </c>
       <c r="P34" s="7" t="inlineStr">
         <is>
-          <t>PED - 5 (GCH1111_1)</t>
+          <t>PED - 3 (GCH1087_1)</t>
         </is>
       </c>
       <c r="Q34" s="7" t="inlineStr">
         <is>
-          <t>PED - 5 (GCH1110_1)</t>
+          <t>PED - 3 (GCH833_2)</t>
         </is>
       </c>
       <c r="R34" s="7" t="inlineStr">
         <is>
-          <t>PED - 5 (GCH1107_1)</t>
-        </is>
-      </c>
-      <c r="S34" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 5 (GCH1108_1 - GCH1109_1) </t>
+          <t>PED - 3 (GCH840_2)</t>
+        </is>
+      </c>
+      <c r="S34" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 3 (GCH1088_1 - GCH1099_1) </t>
         </is>
       </c>
       <c r="T34" s="7" t="inlineStr">
@@ -3858,12 +3858,12 @@
       </c>
       <c r="K35" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 9 (GCS552_1)</t>
         </is>
       </c>
       <c r="L35" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 9 (GCS552_1)</t>
         </is>
       </c>
       <c r="M35" s="7" t="inlineStr">
@@ -3878,27 +3878,27 @@
       </c>
       <c r="O35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 7 (GCS080_1)</t>
+          <t>ADM - 1 (GEX212_4)</t>
         </is>
       </c>
       <c r="P35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 7 (GCS077_1)</t>
+          <t>ADM - 1 (GCH290_11)</t>
         </is>
       </c>
       <c r="Q35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 7 (GCS544_1)</t>
+          <t>ADM - 1 (GCS534_1)</t>
         </is>
       </c>
       <c r="R35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 7 (GCS545_1)</t>
+          <t>ADM - 1 (GLA104_3)</t>
         </is>
       </c>
       <c r="S35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 7 (GCS239_3)</t>
+          <t>ADM - 1 (GCS525_1)</t>
         </is>
       </c>
       <c r="T35" s="7" t="inlineStr">
@@ -3916,27 +3916,27 @@
       </c>
       <c r="C36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 2 (GCH293_3)</t>
+          <t>ADM - 4 (GCS532_1)</t>
         </is>
       </c>
       <c r="D36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 2 (GCS527_1)</t>
+          <t>ADM - 4 (GCS535_1)</t>
         </is>
       </c>
       <c r="E36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 2 (GEX094_1)</t>
+          <t>ADM - 4 (GCS533_1)</t>
         </is>
       </c>
       <c r="F36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 2 (GCS526_1)</t>
+          <t>ADM - 4 (GCS066_1)</t>
         </is>
       </c>
       <c r="G36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 2 (GCS238_9)</t>
+          <t>ADM - 4 (GCS068_1)</t>
         </is>
       </c>
       <c r="H36" s="7" t="inlineStr">
@@ -3976,27 +3976,27 @@
       </c>
       <c r="O36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 1 (GEX212_4)</t>
+          <t>ADM - 7 (GCS080_1)</t>
         </is>
       </c>
       <c r="P36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 1 (GCH290_11)</t>
+          <t>ADM - 7 (GCS077_1)</t>
         </is>
       </c>
       <c r="Q36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 1 (GCS534_1)</t>
+          <t>ADM - 7 (GCS544_1)</t>
         </is>
       </c>
       <c r="R36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 1 (GLA104_3)</t>
+          <t>ADM - 7 (GCS545_1)</t>
         </is>
       </c>
       <c r="S36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 1 (GCS525_1)</t>
+          <t>ADM - 7 (GCS239_3)</t>
         </is>
       </c>
       <c r="T36" s="7" t="inlineStr">
@@ -4014,32 +4014,32 @@
       </c>
       <c r="C37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 4 (GCS532_1)</t>
+          <t>ADM - 2 (GCH293_3)</t>
         </is>
       </c>
       <c r="D37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 4 (GCS535_1)</t>
+          <t>ADM - 2 (GCS527_1)</t>
         </is>
       </c>
       <c r="E37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 4 (GCS533_1)</t>
+          <t>ADM - 2 (GEX094_1)</t>
         </is>
       </c>
       <c r="F37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 4 (GCS066_1)</t>
+          <t>ADM - 2 (GCS526_1)</t>
         </is>
       </c>
       <c r="G37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 4 (GCS068_1)</t>
+          <t>ADM - 2 (GCS238_9)</t>
         </is>
       </c>
       <c r="H37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 3 (GCS529_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I37" s="7" t="inlineStr">
@@ -4074,27 +4074,27 @@
       </c>
       <c r="O37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 3 (GCS530_1)</t>
-        </is>
-      </c>
-      <c r="P37" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ADM - 3 (GCH087_1 - GCS528_1) </t>
+          <t>ADM - 5 (GCS538_1)</t>
+        </is>
+      </c>
+      <c r="P37" s="7" t="inlineStr">
+        <is>
+          <t>ADM - 5 (GCS540_1)</t>
         </is>
       </c>
       <c r="Q37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 3 (GEX210_3)</t>
+          <t>ADM - 5 (GCS536_1)</t>
         </is>
       </c>
       <c r="R37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 3 (GCS529_1)</t>
+          <t>ADM - 5 (GCS537_1)</t>
         </is>
       </c>
       <c r="S37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 3 (GCS531_1)</t>
+          <t>ADM - 5 (GCS539_1)</t>
         </is>
       </c>
       <c r="T37" s="7" t="inlineStr">
@@ -4137,7 +4137,7 @@
       </c>
       <c r="H38" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 3 (GCS529_1)</t>
         </is>
       </c>
       <c r="I38" s="7" t="inlineStr">
@@ -4152,12 +4152,12 @@
       </c>
       <c r="K38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 9 (GCS552_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 9 (GCS552_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M38" s="7" t="inlineStr">
@@ -4172,27 +4172,27 @@
       </c>
       <c r="O38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 5 (GCS538_1)</t>
-        </is>
-      </c>
-      <c r="P38" s="7" t="inlineStr">
-        <is>
-          <t>ADM - 9 (GCS549_1)</t>
+          <t>ADM - 3 (GCS530_1)</t>
+        </is>
+      </c>
+      <c r="P38" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ADM - 3 (GCH087_1 - GCS528_1) </t>
         </is>
       </c>
       <c r="Q38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 9 (GCS551_1)</t>
+          <t>ADM - 3 (GEX210_3)</t>
         </is>
       </c>
       <c r="R38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 5 (GCS537_1)</t>
+          <t>ADM - 3 (GCS529_1)</t>
         </is>
       </c>
       <c r="S38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 9 (GCS573_1)</t>
+          <t>ADM - 3 (GCS531_1)</t>
         </is>
       </c>
       <c r="T38" s="7" t="inlineStr">
@@ -4208,19 +4208,19 @@
           <t>301-B</t>
         </is>
       </c>
-      <c r="C39" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 1 (GSA140_1 - GSA271_1) </t>
+      <c r="C39" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 1 (GSA140_1) | MED - 1 (GSA271_1) </t>
         </is>
       </c>
       <c r="D39" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E39" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 1 (GSA140_1 - GSA271_1) </t>
+          <t>MED - 1 (GSA271_1)</t>
+        </is>
+      </c>
+      <c r="E39" s="7" t="inlineStr">
+        <is>
+          <t>MED - 1 (GSA140_1)</t>
         </is>
       </c>
       <c r="F39" s="7" t="inlineStr">
@@ -4230,7 +4230,7 @@
       </c>
       <c r="G39" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 1 (GSA271_1)</t>
         </is>
       </c>
       <c r="H39" s="7" t="inlineStr">
@@ -4250,7 +4250,7 @@
       </c>
       <c r="K39" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 1 (GSA271_1)</t>
         </is>
       </c>
       <c r="L39" s="7" t="inlineStr">
@@ -4258,9 +4258,9 @@
           <t>MED - 1 (GSA142_1)</t>
         </is>
       </c>
-      <c r="M39" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 1 (GSA143_1 - GSA268_1) </t>
+      <c r="M39" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 1 (GSA143_1) | MED - 1 (GSA268_1) </t>
         </is>
       </c>
       <c r="N39" s="7" t="inlineStr">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="I40" s="7" t="inlineStr">
         <is>
-          <t>CC - 2 (GEN253_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J40" s="7" t="inlineStr">
@@ -4368,7 +4368,7 @@
       </c>
       <c r="O40" s="7" t="inlineStr">
         <is>
-          <t>CC - 2 (GEX605_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P40" s="7" t="inlineStr">
@@ -4378,7 +4378,7 @@
       </c>
       <c r="Q40" s="7" t="inlineStr">
         <is>
-          <t>CC - 2 (GLA104_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R40" s="7" t="inlineStr">
@@ -4411,7 +4411,7 @@
       </c>
       <c r="D41" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 3 (GSA280_1)</t>
         </is>
       </c>
       <c r="E41" s="7" t="inlineStr">
@@ -4436,12 +4436,12 @@
       </c>
       <c r="I41" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J41" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 3 (GSA167_1 - GSA280_1) </t>
+          <t>MED - 3 (GSA280_1)</t>
+        </is>
+      </c>
+      <c r="J41" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 3 (GSA167_1) | MED - 3 (GSA280_1) </t>
         </is>
       </c>
       <c r="K41" s="7" t="inlineStr">
@@ -4449,9 +4449,9 @@
           <t>MED - 3 (GSA169_1)</t>
         </is>
       </c>
-      <c r="L41" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 3 (GSA167_1 - GSA280_1) </t>
+      <c r="L41" s="7" t="inlineStr">
+        <is>
+          <t>MED - 3 (GSA167_1)</t>
         </is>
       </c>
       <c r="M41" s="7" t="inlineStr">
@@ -4474,7 +4474,7 @@
           <t>GEO - 4 (GEX559_1)</t>
         </is>
       </c>
-      <c r="Q41" s="11" t="inlineStr">
+      <c r="Q41" s="10" t="inlineStr">
         <is>
           <t>GEO - 4 + HIS - 4 (GCH374_1)</t>
         </is>
@@ -4564,7 +4564,7 @@
       </c>
       <c r="O42" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 3 (GEX098_2)</t>
         </is>
       </c>
       <c r="P42" s="7" t="inlineStr">
@@ -4574,7 +4574,7 @@
       </c>
       <c r="Q42" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 3 (GEX608_1)</t>
         </is>
       </c>
       <c r="R42" s="7" t="inlineStr">
@@ -4582,7 +4582,7 @@
           <t>GEO - 6 (GCH622_1)</t>
         </is>
       </c>
-      <c r="S42" s="11" t="inlineStr">
+      <c r="S42" s="10" t="inlineStr">
         <is>
           <t>GEO - 6 + HIS - 6 (GCH383_1)</t>
         </is>
@@ -4617,17 +4617,17 @@
       </c>
       <c r="F43" s="7" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G43" s="7" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H43" s="7" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I43" s="8" t="inlineStr">
@@ -4635,24 +4635,24 @@
           <t xml:space="preserve">CC - 4 (GEX612_1) | CC - 4 (GEX613_2) </t>
         </is>
       </c>
-      <c r="J43" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 4 (GEN254_1) | CC - 4 (GEX102_1) </t>
+      <c r="J43" s="7" t="inlineStr">
+        <is>
+          <t>CC - 4 (GEX102_1)</t>
         </is>
       </c>
       <c r="K43" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">CC - 4 (GEX090_1) | CC - 4 (GEX612_1) </t>
+          <t xml:space="preserve">CC - opt (GEX1082_1) | CC - 4 (GEX612_1) </t>
         </is>
       </c>
       <c r="L43" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">CC - 4 (GEN254_1) | CC - 4 (GEX102_1) </t>
-        </is>
-      </c>
-      <c r="M43" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 4 (GEX090_1) | CC - 4 (GEX613_2) </t>
+          <t xml:space="preserve">CC - 4 (GEX102_1) | CC - opt (GEX1082_1) </t>
+        </is>
+      </c>
+      <c r="M43" s="7" t="inlineStr">
+        <is>
+          <t>CC - 4 (GEX613_2)</t>
         </is>
       </c>
       <c r="N43" s="7" t="inlineStr">
@@ -4662,27 +4662,27 @@
       </c>
       <c r="O43" s="7" t="inlineStr">
         <is>
-          <t>CC - 5 (GEX101_1)</t>
+          <t>CC - opt (GEX635_1)</t>
         </is>
       </c>
       <c r="P43" s="7" t="inlineStr">
         <is>
-          <t>CC - 5 (GEX091_1)</t>
+          <t>CC - 3 (GEX392_1)</t>
         </is>
       </c>
       <c r="Q43" s="7" t="inlineStr">
         <is>
-          <t>CC - 5 (GEX607_1)</t>
+          <t>CC - 4 (GCH290_5)</t>
         </is>
       </c>
       <c r="R43" s="7" t="inlineStr">
         <is>
-          <t>CC - 5 (GEX110_1)</t>
+          <t>CC - opt (GEX1083_1)</t>
         </is>
       </c>
       <c r="S43" s="7" t="inlineStr">
         <is>
-          <t>CC - 5 (GEX616_1)</t>
+          <t>CC - 3 (GEX609_1)</t>
         </is>
       </c>
       <c r="T43" s="7" t="inlineStr">
@@ -4715,42 +4715,42 @@
       </c>
       <c r="F44" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 8 (GEX658_1)</t>
         </is>
       </c>
       <c r="G44" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 8 (GEX658_1)</t>
         </is>
       </c>
       <c r="H44" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I44" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 6 (GEX105_1) | CC - 6 (GEX108_1) </t>
+          <t>CC - 8 (GEX658_1)</t>
+        </is>
+      </c>
+      <c r="I44" s="7" t="inlineStr">
+        <is>
+          <t>CC - 8 (GCS239_2)</t>
         </is>
       </c>
       <c r="J44" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">CC - 6 (GCS580_1) | CC - 6 (GEX614_1) </t>
+          <t xml:space="preserve">CC - 2 (GEN253_1) | CC - 2 (GEX605_2) </t>
         </is>
       </c>
       <c r="K44" s="7" t="inlineStr">
         <is>
-          <t>CC - 6 (GCH292_2)</t>
+          <t>CC - 2 (GEX195_1)</t>
         </is>
       </c>
       <c r="L44" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">CC - 6 (GCS580_1) | CC - 6 (GEX105_1) </t>
+          <t xml:space="preserve">CC - 2 (GEX055_1) | CC - 2 (GEX605_2) </t>
         </is>
       </c>
       <c r="M44" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">CC - 6 (GEX108_1) | CC - 6 (GEX614_1) </t>
+          <t xml:space="preserve">CC - 2 (GEX055_1) | CC - 2 (GEX195_1) </t>
         </is>
       </c>
       <c r="N44" s="7" t="inlineStr">
@@ -4760,27 +4760,27 @@
       </c>
       <c r="O44" s="7" t="inlineStr">
         <is>
-          <t>CC - 7 (GEX395_1)</t>
+          <t>CC - 5 (GEX101_1)</t>
         </is>
       </c>
       <c r="P44" s="7" t="inlineStr">
         <is>
-          <t>CC - 7 (GCS238_2)</t>
+          <t>CC - 5 (GEX091_1)</t>
         </is>
       </c>
       <c r="Q44" s="7" t="inlineStr">
         <is>
-          <t>CC - 7 (GEX618_1)</t>
+          <t>CC - 5 (GEX607_1)</t>
         </is>
       </c>
       <c r="R44" s="7" t="inlineStr">
         <is>
-          <t>CC - 7 (GEX107_1)</t>
+          <t>CC - 5 (GEX110_1)</t>
         </is>
       </c>
       <c r="S44" s="7" t="inlineStr">
         <is>
-          <t>CC - 7 (GEX617_1)</t>
+          <t>CC - 5 (GEX616_1)</t>
         </is>
       </c>
       <c r="T44" s="7" t="inlineStr">
@@ -4813,42 +4813,42 @@
       </c>
       <c r="F45" s="7" t="inlineStr">
         <is>
-          <t>CC - 8 (GEX658_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G45" s="7" t="inlineStr">
         <is>
-          <t>CC - 8 (GEX658_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H45" s="7" t="inlineStr">
         <is>
-          <t>CC - 8 (GEX658_1)</t>
-        </is>
-      </c>
-      <c r="I45" s="7" t="inlineStr">
-        <is>
-          <t>CC - 8 (GCS239_2)</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I45" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 6 (GEX105_1) | CC - 6 (GEX108_1) </t>
         </is>
       </c>
       <c r="J45" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">CC - 2 (GEN253_1) | CC - 2 (GEX605_3) </t>
+          <t xml:space="preserve">CC - 6 (GCS580_1) | CC - 6 (GEX614_1) </t>
         </is>
       </c>
       <c r="K45" s="7" t="inlineStr">
         <is>
-          <t>CC - 2 (GEX195_1)</t>
+          <t>CC - 6 (GCH292_2)</t>
         </is>
       </c>
       <c r="L45" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">CC - 2 (GEX055_1) | CC - 2 (GEX605_3) </t>
+          <t xml:space="preserve">CC - 6 (GCS580_1) | CC - 6 (GEX105_1) </t>
         </is>
       </c>
       <c r="M45" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">CC - 2 (GEX055_1) | CC - 2 (GEX195_1) </t>
+          <t xml:space="preserve">CC - 6 (GEX108_1) | CC - 6 (GEX614_1) </t>
         </is>
       </c>
       <c r="N45" s="7" t="inlineStr">
@@ -4858,27 +4858,27 @@
       </c>
       <c r="O45" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX098_1)</t>
+          <t>CC - 7 (GEX395_1)</t>
         </is>
       </c>
       <c r="P45" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX208_2)</t>
+          <t>CC - 7 (GCS238_2)</t>
         </is>
       </c>
       <c r="Q45" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX608_1)</t>
+          <t>CC - 7 (GEX618_1)</t>
         </is>
       </c>
       <c r="R45" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_2)</t>
+          <t>CC - 7 (GEX107_1)</t>
         </is>
       </c>
       <c r="S45" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX210_2)</t>
+          <t>CC - 7 (GEX617_1)</t>
         </is>
       </c>
       <c r="T45" s="7" t="inlineStr">
@@ -4911,17 +4911,17 @@
       </c>
       <c r="F46" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 9 (GEX657_1)</t>
         </is>
       </c>
       <c r="G46" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 9 (GEX657_1)</t>
         </is>
       </c>
       <c r="H46" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 9 (GEX657_1)</t>
         </is>
       </c>
       <c r="I46" s="8" t="inlineStr">
@@ -4929,24 +4929,24 @@
           <t xml:space="preserve">CC - 2 (GEX178_1) | CC - 4 (GEX613_1) </t>
         </is>
       </c>
-      <c r="J46" s="7" t="inlineStr">
-        <is>
-          <t>CC - 2 (GEX605_2)</t>
+      <c r="J46" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEN254_1) | CC - 2 (GEX605_3) </t>
         </is>
       </c>
       <c r="K46" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">CC - opt (GEX1082_1) | CC - 2 (GEX178_1) </t>
+          <t xml:space="preserve">CC - 4 (GEX090_1) | CC - 2 (GEX178_1) </t>
         </is>
       </c>
       <c r="L46" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">CC - opt (GEX1082_1) | CC - 2 (GEX605_2) </t>
-        </is>
-      </c>
-      <c r="M46" s="7" t="inlineStr">
-        <is>
-          <t>CC - 4 (GEX613_1)</t>
+          <t xml:space="preserve">CC - 4 (GEN254_1) | CC - 2 (GEX605_3) </t>
+        </is>
+      </c>
+      <c r="M46" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEX090_1) | CC - 4 (GEX613_1) </t>
         </is>
       </c>
       <c r="N46" s="7" t="inlineStr">
@@ -4956,27 +4956,27 @@
       </c>
       <c r="O46" s="7" t="inlineStr">
         <is>
-          <t>CC - opt (GEX635_1)</t>
+          <t>CC - 2 (GEX605_1)</t>
         </is>
       </c>
       <c r="P46" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX392_1)</t>
+          <t>CC - 1 (GEX208_2)</t>
         </is>
       </c>
       <c r="Q46" s="7" t="inlineStr">
         <is>
-          <t>CC - 4 (GCH290_5)</t>
+          <t>CC - 2 (GLA104_2)</t>
         </is>
       </c>
       <c r="R46" s="7" t="inlineStr">
         <is>
-          <t>CC - opt (GEX1083_1)</t>
+          <t>CC - 1 (GEX003_1)</t>
         </is>
       </c>
       <c r="S46" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX609_1)</t>
+          <t>CC - 1 (GEX210_2)</t>
         </is>
       </c>
       <c r="T46" s="7" t="inlineStr">
@@ -4994,12 +4994,12 @@
       </c>
       <c r="C47" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D47" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 5 (GSA191_1 - GSA284_1) </t>
+          <t>MED - 5 (GSA193_1)</t>
+        </is>
+      </c>
+      <c r="D47" s="7" t="inlineStr">
+        <is>
+          <t>MED - 5 (GSA191_1)</t>
         </is>
       </c>
       <c r="E47" s="7" t="inlineStr">
@@ -5022,24 +5022,24 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I47" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 5 (GSA188_1 - GSA193_1)  | MED - 9 (GSA296_1) </t>
-        </is>
-      </c>
-      <c r="J47" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 5 (GSA191_1 - GSA284_1) </t>
-        </is>
-      </c>
-      <c r="K47" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 5 (GSA188_1 - GSA193_1) </t>
-        </is>
-      </c>
-      <c r="L47" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 5 (GSA190_1 - GSA283_1) </t>
+      <c r="I47" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 5 (GSA188_1) | MED - 5 (GSA193_1)  | MED - 9 (GSA296_1) </t>
+        </is>
+      </c>
+      <c r="J47" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 5 (GSA191_1) | MED - 5 (GSA284_1) </t>
+        </is>
+      </c>
+      <c r="K47" s="7" t="inlineStr">
+        <is>
+          <t>MED - 5 (GSA188_1)</t>
+        </is>
+      </c>
+      <c r="L47" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 5 (GSA190_1) | MED - 5 (GSA283_1) </t>
         </is>
       </c>
       <c r="M47" s="7" t="inlineStr">
@@ -5067,9 +5067,9 @@
           <t>MED - 5 (GSA192_1)</t>
         </is>
       </c>
-      <c r="R47" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 5 (GSA190_1 - GSA283_1) </t>
+      <c r="R47" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 5 (GSA190_1) | MED - 5 (GSA283_1) </t>
         </is>
       </c>
       <c r="S47" s="7" t="inlineStr">
@@ -5092,7 +5092,7 @@
       </c>
       <c r="C48" s="7" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH859_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D48" s="7" t="inlineStr">
@@ -5117,7 +5117,7 @@
       </c>
       <c r="H48" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 6 (GCH854_1)</t>
         </is>
       </c>
       <c r="I48" s="7" t="inlineStr">
@@ -5127,7 +5127,7 @@
       </c>
       <c r="J48" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 6 (GCH837_1)</t>
         </is>
       </c>
       <c r="K48" s="7" t="inlineStr">
@@ -5147,32 +5147,32 @@
       </c>
       <c r="N48" s="7" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH843_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O48" s="7" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH852_1)</t>
+          <t>FIL - 6 (GCH839_2)</t>
         </is>
       </c>
       <c r="P48" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 6 (GCH837_1)</t>
         </is>
       </c>
       <c r="Q48" s="7" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH844_1)</t>
+          <t>FIL - 6 (GCH857_1)</t>
         </is>
       </c>
       <c r="R48" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 6 (GCH854_1)</t>
         </is>
       </c>
       <c r="S48" s="7" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH853_1)</t>
+          <t>FIL - 3 (GCH856_1)</t>
         </is>
       </c>
       <c r="T48" s="7" t="inlineStr">
@@ -5356,7 +5356,7 @@
           <t>HIS - 8 (GCH387_1)</t>
         </is>
       </c>
-      <c r="Q50" s="10" t="inlineStr">
+      <c r="Q50" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">HIS - opt (GCH459_1 - GCH467_1) </t>
         </is>
@@ -5386,7 +5386,7 @@
       </c>
       <c r="C51" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 8 (GCH859_1)</t>
         </is>
       </c>
       <c r="D51" s="7" t="inlineStr">
@@ -5441,32 +5441,32 @@
       </c>
       <c r="N51" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 8 (GCH843_1)</t>
         </is>
       </c>
       <c r="O51" s="7" t="inlineStr">
         <is>
-          <t>FIL - 4 (GCH847_1)</t>
-        </is>
-      </c>
-      <c r="P51" s="11" t="inlineStr">
-        <is>
-          <t>FIL - 4 + LET - 4 (GCH833_1)</t>
+          <t>FIL - 8 (GCH852_1)</t>
+        </is>
+      </c>
+      <c r="P51" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="Q51" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R51" s="11" t="inlineStr">
-        <is>
-          <t>FIL - 4 + MAT - 2 (GCH840_1)</t>
+          <t>FIL - 8 (GCH844_1)</t>
+        </is>
+      </c>
+      <c r="R51" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="S51" s="7" t="inlineStr">
         <is>
-          <t>FIL - 4 (GCH850_1)</t>
+          <t>FIL - 8 (GCH853_1)</t>
         </is>
       </c>
       <c r="T51" s="7" t="inlineStr">
@@ -5509,7 +5509,7 @@
       </c>
       <c r="H52" s="7" t="inlineStr">
         <is>
-          <t>FIL - 6 (GCH854_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I52" s="7" t="inlineStr">
@@ -5519,7 +5519,7 @@
       </c>
       <c r="J52" s="7" t="inlineStr">
         <is>
-          <t>FIL - 6 (GCH837_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K52" s="7" t="inlineStr">
@@ -5544,27 +5544,27 @@
       </c>
       <c r="O52" s="7" t="inlineStr">
         <is>
-          <t>FIL - 6 (GCH839_2)</t>
-        </is>
-      </c>
-      <c r="P52" s="7" t="inlineStr">
-        <is>
-          <t>FIL - 6 (GCH837_1)</t>
+          <t>FIL - 4 (GCH847_1)</t>
+        </is>
+      </c>
+      <c r="P52" s="10" t="inlineStr">
+        <is>
+          <t>FIL - 4 + LET - 4 (GCH833_1)</t>
         </is>
       </c>
       <c r="Q52" s="7" t="inlineStr">
         <is>
-          <t>FIL - 6 (GCH857_1)</t>
-        </is>
-      </c>
-      <c r="R52" s="7" t="inlineStr">
-        <is>
-          <t>FIL - 6 (GCH854_1)</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R52" s="10" t="inlineStr">
+        <is>
+          <t>FIL - 4 + MAT - 2 (GCH840_1)</t>
         </is>
       </c>
       <c r="S52" s="7" t="inlineStr">
         <is>
-          <t>FIL - 3 (GCH856_1)</t>
+          <t>FIL - 4 (GCH850_1)</t>
         </is>
       </c>
       <c r="T52" s="7" t="inlineStr">

</xml_diff>

<commit_message>
Novas restricoes para aproximar fases
</commit_message>
<xml_diff>
--- a/planilha_alocacoes.xlsx
+++ b/planilha_alocacoes.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -71,14 +71,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ff7b59"/>
-        <bgColor rgb="00ff7b59"/>
+        <fgColor rgb="00ab93f5"/>
+        <bgColor rgb="00ab93f5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ab93f5"/>
-        <bgColor rgb="00ab93f5"/>
+        <fgColor rgb="00ff7b59"/>
+        <bgColor rgb="00ff7b59"/>
       </patternFill>
     </fill>
   </fills>
@@ -202,10 +202,10 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -216,8 +216,8 @@
     <cellStyle name="estilo_header" xfId="1" hidden="0"/>
     <cellStyle name="estilo_index" xfId="2" hidden="0"/>
     <cellStyle name="compartilhamento" xfId="3" hidden="0"/>
-    <cellStyle name="fusao" xfId="4" hidden="0"/>
-    <cellStyle name="agrupamento" xfId="5" hidden="0"/>
+    <cellStyle name="agrupamento" xfId="4" hidden="0"/>
+    <cellStyle name="fusao" xfId="5" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -580,7 +580,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T57"/>
+  <dimension ref="A1:T53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -813,14 +813,14 @@
           <t xml:space="preserve">EAS - 6 (GEN042_1) | EAS - 6 (GEX395_2) </t>
         </is>
       </c>
-      <c r="J4" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 6 (GCA322_1) | EAS - 6 (GEN042_1) </t>
-        </is>
-      </c>
-      <c r="K4" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 6 (GCA322_1) | EAS - 6 (GEX297_1) </t>
+      <c r="J4" s="7" t="inlineStr">
+        <is>
+          <t>EAS - 6 (GEN042_1)</t>
+        </is>
+      </c>
+      <c r="K4" s="7" t="inlineStr">
+        <is>
+          <t>LET - opt (GLA004_2)</t>
         </is>
       </c>
       <c r="L4" s="8" t="inlineStr">
@@ -830,7 +830,7 @@
       </c>
       <c r="M4" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">EAS - 6 (GEN011_1) | EAS - 6 (GEN103_1) </t>
+          <t xml:space="preserve">EAS - 6 (GEN011_1) | EAS - 10 (GEN118_1) </t>
         </is>
       </c>
       <c r="N4" s="7" t="inlineStr">
@@ -845,22 +845,22 @@
       </c>
       <c r="P4" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q4" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>LET - opt (GCS239_10)</t>
+        </is>
+      </c>
+      <c r="Q4" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - opt (GCH293_4 - GLA004_3) </t>
         </is>
       </c>
       <c r="R4" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GEX006_2)</t>
         </is>
       </c>
       <c r="S4" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - 10 (GEN118_1)</t>
         </is>
       </c>
       <c r="T4" s="7" t="inlineStr">
@@ -870,15 +870,15 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="n"/>
+      <c r="A5" s="10" t="n"/>
       <c r="B5" s="6" t="inlineStr">
         <is>
           <t>202-A</t>
         </is>
       </c>
-      <c r="C5" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 8 (GCS253_1) | EAS - opt (GEN195_1) </t>
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>EAS - 8 (GCS253_1)</t>
         </is>
       </c>
       <c r="D5" s="8" t="inlineStr">
@@ -903,32 +903,32 @@
       </c>
       <c r="H5" s="7" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN204_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I5" s="7" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN196_1)</t>
+          <t>EAS - 10 (GEN119_1)</t>
         </is>
       </c>
       <c r="J5" s="7" t="inlineStr">
         <is>
-          <t>EAS - opt (GEX458_1)</t>
-        </is>
-      </c>
-      <c r="K5" s="7" t="inlineStr">
-        <is>
-          <t>EAS - opt (GCA321_1)</t>
+          <t>EAS - 6 (GCA322_1)</t>
+        </is>
+      </c>
+      <c r="K5" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - 6 (GCA322_1) | EAS - 6 (GEX297_1) </t>
         </is>
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">EAS - 8 (GCS241_1) | EAS - opt (GEN204_1) </t>
-        </is>
-      </c>
-      <c r="M5" s="7" t="inlineStr">
-        <is>
-          <t>EAS - 10 (GEN118_1)</t>
+          <t xml:space="preserve">EAS - 8 (GCS241_1) | EAS - 10 (GEN119_1) </t>
+        </is>
+      </c>
+      <c r="M5" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - 6 (GEN103_1) | EAS - 10 (GEN119_1) </t>
         </is>
       </c>
       <c r="N5" s="7" t="inlineStr">
@@ -938,17 +938,17 @@
       </c>
       <c r="O5" s="7" t="inlineStr">
         <is>
-          <t>MAT - 6 (GEX984_1)</t>
-        </is>
-      </c>
-      <c r="P5" s="10" t="inlineStr">
-        <is>
-          <t>MAT - 6 + PED - 5 (GCH837_2)</t>
+          <t>MAT - 4 (GEX979_1)</t>
+        </is>
+      </c>
+      <c r="P5" s="7" t="inlineStr">
+        <is>
+          <t>MAT - 4 (GEX978_1)</t>
         </is>
       </c>
       <c r="Q5" s="7" t="inlineStr">
         <is>
-          <t>MAT - 6 (GEX985_1)</t>
+          <t>EAS - 10 (GEN119_1)</t>
         </is>
       </c>
       <c r="R5" s="7" t="inlineStr">
@@ -958,7 +958,7 @@
       </c>
       <c r="S5" s="7" t="inlineStr">
         <is>
-          <t>EAS - 10 (GEN118_1)</t>
+          <t>MAT - 4 (GEX976_1)</t>
         </is>
       </c>
       <c r="T5" s="7" t="inlineStr">
@@ -968,7 +968,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="9" t="n"/>
+      <c r="A6" s="10" t="n"/>
       <c r="B6" s="6" t="inlineStr">
         <is>
           <t>203-A</t>
@@ -976,7 +976,7 @@
       </c>
       <c r="C6" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - opt (GEN195_1)</t>
         </is>
       </c>
       <c r="D6" s="7" t="inlineStr">
@@ -996,37 +996,37 @@
       </c>
       <c r="G6" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 4 (GCA045_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H6" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - opt (GEN204_1)</t>
         </is>
       </c>
       <c r="I6" s="7" t="inlineStr">
         <is>
-          <t>EAS - 10 (GEN119_1)</t>
-        </is>
-      </c>
-      <c r="J6" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 6 (GCA286_1 - GCA286_2) </t>
+          <t>EAS - opt (GEN196_1)</t>
+        </is>
+      </c>
+      <c r="J6" s="7" t="inlineStr">
+        <is>
+          <t>EAS - opt (GEX458_1)</t>
         </is>
       </c>
       <c r="K6" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - opt (GCA321_1)</t>
         </is>
       </c>
       <c r="L6" s="7" t="inlineStr">
         <is>
-          <t>EAS - 10 (GEN119_1)</t>
+          <t>EAS - opt (GEN204_1)</t>
         </is>
       </c>
       <c r="M6" s="7" t="inlineStr">
         <is>
-          <t>EAS - 10 (GEN119_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N6" s="7" t="inlineStr">
@@ -1036,27 +1036,27 @@
       </c>
       <c r="O6" s="7" t="inlineStr">
         <is>
-          <t>MAT - 4 (GEX979_1)</t>
-        </is>
-      </c>
-      <c r="P6" s="7" t="inlineStr">
-        <is>
-          <t>MAT - 4 (GEX978_1)</t>
+          <t>MAT - 6 (GEX984_1)</t>
+        </is>
+      </c>
+      <c r="P6" s="11" t="inlineStr">
+        <is>
+          <t>MAT - 6 + PED - 5 (GCH837_2)</t>
         </is>
       </c>
       <c r="Q6" s="7" t="inlineStr">
         <is>
-          <t>EAS - 10 (GEN119_1)</t>
+          <t>MAT - 6 (GEX985_1)</t>
         </is>
       </c>
       <c r="R6" s="7" t="inlineStr">
         <is>
-          <t>MAT - 4 (GEX977_1)</t>
-        </is>
-      </c>
-      <c r="S6" s="7" t="inlineStr">
-        <is>
-          <t>MAT - 4 (GEX976_1)</t>
+          <t>GEO - 6 (GCH622_1)</t>
+        </is>
+      </c>
+      <c r="S6" s="11" t="inlineStr">
+        <is>
+          <t>GEO - 6 + HIS - 6 (GCH383_1)</t>
         </is>
       </c>
       <c r="T6" s="7" t="inlineStr">
@@ -1066,7 +1066,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="9" t="n"/>
+      <c r="A7" s="10" t="n"/>
       <c r="B7" s="6" t="inlineStr">
         <is>
           <t>204-A</t>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="R7" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MAT - opt (GEX1000_1)</t>
         </is>
       </c>
       <c r="S7" s="7" t="inlineStr">
@@ -1164,13 +1164,13 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="n"/>
+      <c r="A8" s="10" t="n"/>
       <c r="B8" s="6" t="inlineStr">
         <is>
           <t>205-A</t>
         </is>
       </c>
-      <c r="C8" s="10" t="inlineStr">
+      <c r="C8" s="11" t="inlineStr">
         <is>
           <t>EAS - 2 + PED - 2 (GCH291_1)</t>
         </is>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="E8" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - opt (GCS556_1)</t>
         </is>
       </c>
       <c r="F8" s="7" t="inlineStr">
@@ -1230,14 +1230,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O8" s="11" t="inlineStr">
+      <c r="O8" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">MAT - 8 (GEX993_1 - GEX994_1) </t>
         </is>
       </c>
       <c r="P8" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - opt (GCS566_1)</t>
         </is>
       </c>
       <c r="Q8" s="7" t="inlineStr">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="R8" s="7" t="inlineStr">
         <is>
-          <t>MAT - opt (GEX1000_1)</t>
+          <t>ADM - opt (GCS554_1)</t>
         </is>
       </c>
       <c r="S8" s="7" t="inlineStr">
@@ -1262,7 +1262,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="n"/>
+      <c r="A9" s="10" t="n"/>
       <c r="B9" s="6" t="inlineStr">
         <is>
           <t>206-A</t>
@@ -1295,22 +1295,22 @@
       </c>
       <c r="H9" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA168_1)</t>
         </is>
       </c>
       <c r="I9" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GCS011_1)</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr">
         <is>
-          <t>LET - 10 (GLA054_1)</t>
-        </is>
-      </c>
-      <c r="K9" s="7" t="inlineStr">
-        <is>
-          <t>LET - 10 (GLA041_1)</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K9" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - opt (GLA104_5 - GLA552_1) </t>
         </is>
       </c>
       <c r="L9" s="7" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="O9" s="7" t="inlineStr">
         <is>
-          <t>LET - 10 (GLA043_1)</t>
+          <t>LET - opt (GEX212_3)</t>
         </is>
       </c>
       <c r="P9" s="7" t="inlineStr">
@@ -1340,17 +1340,17 @@
       </c>
       <c r="Q9" s="7" t="inlineStr">
         <is>
-          <t>LET - 10 (GLA041_1)</t>
+          <t>LET - opt (GLA168_1)</t>
         </is>
       </c>
       <c r="R9" s="7" t="inlineStr">
         <is>
-          <t>LET - 10 (GLA041_1)</t>
+          <t>LET - opt (GLA528_1)</t>
         </is>
       </c>
       <c r="S9" s="7" t="inlineStr">
         <is>
-          <t>LET - 10 (GLA059_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T9" s="7" t="inlineStr">
@@ -1360,7 +1360,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="n"/>
+      <c r="A10" s="10" t="n"/>
       <c r="B10" s="6" t="inlineStr">
         <is>
           <t>207-A</t>
@@ -1391,29 +1391,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H10" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 6 (GLA373_1 - GLA376_1) </t>
-        </is>
-      </c>
-      <c r="I10" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 6 (GLA374_1 - GLA375_1) </t>
+      <c r="H10" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="inlineStr">
+        <is>
+          <t>ENF - 4 (GCH012_2)</t>
         </is>
       </c>
       <c r="J10" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 4 (GSA014_1)</t>
         </is>
       </c>
       <c r="K10" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L10" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>ENF - 4 (GSA012_1)</t>
+        </is>
+      </c>
+      <c r="L10" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ENF - 4 (GCB029_1 - GCB076_1) </t>
         </is>
       </c>
       <c r="M10" s="7" t="inlineStr">
@@ -1421,34 +1421,34 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N10" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 6 (GLA373_1 - GLA376_1) </t>
-        </is>
-      </c>
-      <c r="O10" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 6 (GLA374_1 - GLA375_1) </t>
+      <c r="N10" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O10" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 4 (GLA365_1 - GLA367_1) </t>
         </is>
       </c>
       <c r="P10" s="7" t="inlineStr">
         <is>
-          <t>LET - 6 (GLA378_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q10" s="7" t="inlineStr">
         <is>
-          <t>LET - 6 (GCH1031_2)</t>
+          <t>LET - 4 (GLA366_1)</t>
         </is>
       </c>
       <c r="R10" s="7" t="inlineStr">
         <is>
-          <t>LET - 6 (GLA377_1)</t>
-        </is>
-      </c>
-      <c r="S10" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 6 (GLA373_1 - GLA376_1) </t>
+          <t>LET - 4 (GLA368_1)</t>
+        </is>
+      </c>
+      <c r="S10" s="7" t="inlineStr">
+        <is>
+          <t>LET - 4 (GLA364_1)</t>
         </is>
       </c>
       <c r="T10" s="7" t="inlineStr">
@@ -1458,7 +1458,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="n"/>
+      <c r="A11" s="10" t="n"/>
       <c r="B11" s="6" t="inlineStr">
         <is>
           <t>208-A</t>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="D11" s="7" t="inlineStr">
         <is>
-          <t>ENF - 2 (GEX212_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E11" s="7" t="inlineStr">
@@ -1496,22 +1496,22 @@
       </c>
       <c r="I11" s="7" t="inlineStr">
         <is>
-          <t>ENF - 2 (GCB064_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J11" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GSA014_1)</t>
+          <t>LET - 10 (GLA054_1)</t>
         </is>
       </c>
       <c r="K11" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GSA012_1)</t>
+          <t>LET - 10 (GLA041_1)</t>
         </is>
       </c>
       <c r="L11" s="7" t="inlineStr">
         <is>
-          <t>ENF - 2 (GCB019_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M11" s="7" t="inlineStr">
@@ -1524,9 +1524,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O11" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 4 (GLA365_1 - GLA367_1) </t>
+      <c r="O11" s="7" t="inlineStr">
+        <is>
+          <t>LET - 10 (GLA043_1)</t>
         </is>
       </c>
       <c r="P11" s="7" t="inlineStr">
@@ -1536,17 +1536,17 @@
       </c>
       <c r="Q11" s="7" t="inlineStr">
         <is>
-          <t>LET - 4 (GLA366_1)</t>
+          <t>LET - 10 (GLA041_1)</t>
         </is>
       </c>
       <c r="R11" s="7" t="inlineStr">
         <is>
-          <t>LET - 4 (GLA368_1)</t>
+          <t>LET - 10 (GLA041_1)</t>
         </is>
       </c>
       <c r="S11" s="7" t="inlineStr">
         <is>
-          <t>LET - 4 (GLA364_1)</t>
+          <t>LET - 10 (GLA059_1)</t>
         </is>
       </c>
       <c r="T11" s="7" t="inlineStr">
@@ -1556,7 +1556,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="n"/>
+      <c r="A12" s="10" t="n"/>
       <c r="B12" s="6" t="inlineStr">
         <is>
           <t>209-A</t>
@@ -1587,64 +1587,64 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H12" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I12" s="7" t="inlineStr">
-        <is>
-          <t>LET - opt (GLA552_1)</t>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 6 (GLA373_1 - GLA376_1) </t>
+        </is>
+      </c>
+      <c r="I12" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 6 (GLA374_1 - GLA375_1) </t>
         </is>
       </c>
       <c r="J12" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GLA552_1)</t>
+          <t>LET - 9 (GLA061_1)</t>
         </is>
       </c>
       <c r="K12" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GLA552_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L12" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GLA552_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M12" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GLA552_1)</t>
-        </is>
-      </c>
-      <c r="N12" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O12" s="7" t="inlineStr">
-        <is>
-          <t>LET - 2 (GCS238_4)</t>
-        </is>
-      </c>
-      <c r="P12" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 2 (GCH290_14 - GLA358_1) </t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N12" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 6 (GLA373_1 - GLA376_1) </t>
+        </is>
+      </c>
+      <c r="O12" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 6 (GLA374_1 - GLA375_1) </t>
+        </is>
+      </c>
+      <c r="P12" s="7" t="inlineStr">
+        <is>
+          <t>LET - 6 (GLA378_1)</t>
         </is>
       </c>
       <c r="Q12" s="7" t="inlineStr">
         <is>
-          <t>LET - 2 (GLA359_1)</t>
+          <t>LET - 6 (GCH1031_2)</t>
         </is>
       </c>
       <c r="R12" s="7" t="inlineStr">
         <is>
-          <t>LET - 2 (GCH293_5)</t>
-        </is>
-      </c>
-      <c r="S12" s="7" t="inlineStr">
-        <is>
-          <t>LET - 2 (GLA360_1)</t>
+          <t>LET - 6 (GLA377_1)</t>
+        </is>
+      </c>
+      <c r="S12" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 6 (GLA373_1 - GLA376_1) </t>
         </is>
       </c>
       <c r="T12" s="7" t="inlineStr">
@@ -1654,7 +1654,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="9" t="n"/>
+      <c r="A13" s="10" t="n"/>
       <c r="B13" s="6" t="inlineStr">
         <is>
           <t>210-A</t>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="H13" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GLA168_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I13" s="7" t="inlineStr">
@@ -1697,12 +1697,12 @@
       </c>
       <c r="J13" s="7" t="inlineStr">
         <is>
-          <t>LET - 9 (GLA061_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K13" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GLA104_5)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L13" s="7" t="inlineStr">
@@ -1722,27 +1722,27 @@
       </c>
       <c r="O13" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GEX212_3)</t>
-        </is>
-      </c>
-      <c r="P13" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>LET - 8 (GLA391_1)</t>
+        </is>
+      </c>
+      <c r="P13" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 8 (GLA388_1 - GLA389_1) </t>
         </is>
       </c>
       <c r="Q13" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GLA168_1)</t>
+          <t>LET - 8 (GLA390_1)</t>
         </is>
       </c>
       <c r="R13" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GLA528_1)</t>
+          <t>LET - 8 (GLA392_1)</t>
         </is>
       </c>
       <c r="S13" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - 8 (GLA387_1)</t>
         </is>
       </c>
       <c r="T13" s="7" t="inlineStr">
@@ -1752,7 +1752,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="n"/>
+      <c r="A14" s="10" t="n"/>
       <c r="B14" s="6" t="inlineStr">
         <is>
           <t>301-A</t>
@@ -1778,9 +1778,9 @@
           <t>AGRO - 6 (GEX080_1)</t>
         </is>
       </c>
-      <c r="G14" s="7" t="inlineStr">
-        <is>
-          <t>AGRO - opt (GCA655_1)</t>
+      <c r="G14" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 2 (GEX190_1 - GEX190_2) </t>
         </is>
       </c>
       <c r="H14" s="7" t="inlineStr">
@@ -1835,7 +1835,7 @@
       </c>
       <c r="R14" s="7" t="inlineStr">
         <is>
-          <t>MED - 7 (GSA216_1)</t>
+          <t>MED - 3 (GSA281_1)</t>
         </is>
       </c>
       <c r="S14" s="7" t="inlineStr">
@@ -1850,7 +1850,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="9" t="n"/>
+      <c r="A15" s="10" t="n"/>
       <c r="B15" s="6" t="inlineStr">
         <is>
           <t>302-A</t>
@@ -1871,14 +1871,14 @@
           <t>AGRO - 2 (GCB107_1)</t>
         </is>
       </c>
-      <c r="F15" s="11" t="inlineStr">
+      <c r="F15" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">AGRO - 2 (GCA210_3 - GCA210_4)  | AGRO - 2 (GCB056_4 - GCB056_5)  </t>
         </is>
       </c>
-      <c r="G15" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 2 (GEX190_1 - GEX190_2) </t>
+      <c r="G15" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - opt (GCA312_1) | AGRO - opt (GCA655_1) </t>
         </is>
       </c>
       <c r="H15" s="7" t="inlineStr">
@@ -1891,7 +1891,7 @@
           <t>AGRO - 3 (GCS005_1)</t>
         </is>
       </c>
-      <c r="J15" s="11" t="inlineStr">
+      <c r="J15" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">AGRO - 2 (GCB056_4 - GCB056_5) </t>
         </is>
@@ -1916,29 +1916,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O15" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="O15" s="11" t="inlineStr">
+        <is>
+          <t>CS - 8 + HIS - 4 (GCS238_5)</t>
         </is>
       </c>
       <c r="P15" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q15" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>CS - 4 (GCH1397_1)</t>
+        </is>
+      </c>
+      <c r="Q15" s="11" t="inlineStr">
+        <is>
+          <t>CS - 4 + FIL - 4 + MAT - 4 (GCH838_1)</t>
         </is>
       </c>
       <c r="R15" s="7" t="inlineStr">
         <is>
-          <t>MED - 3 (GSA281_1)</t>
-        </is>
-      </c>
-      <c r="S15" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>CS - 4 (GCH1395_1)</t>
+        </is>
+      </c>
+      <c r="S15" s="11" t="inlineStr">
+        <is>
+          <t>CS - 8 + MAT - 6 + PED - 7 (GCH1031_1)</t>
         </is>
       </c>
       <c r="T15" s="7" t="inlineStr">
@@ -1948,35 +1948,35 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="9" t="n"/>
+      <c r="A16" s="10" t="n"/>
       <c r="B16" s="6" t="inlineStr">
         <is>
           <t>303-A</t>
         </is>
       </c>
-      <c r="C16" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 4 (GCA210_1 - GCA210_2) </t>
+      <c r="C16" s="7" t="inlineStr">
+        <is>
+          <t>AGRO - 8 (GCA269_1)</t>
         </is>
       </c>
       <c r="D16" s="7" t="inlineStr">
         <is>
-          <t>AGRO - opt (GEX431_1)</t>
-        </is>
-      </c>
-      <c r="E16" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 4 (GCA218_2) | AGRO - 4 (GCB130_1) </t>
-        </is>
-      </c>
-      <c r="F16" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 4 (GCA037_1 - GCA037_2) </t>
-        </is>
-      </c>
-      <c r="G16" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - opt (GCA312_1) | AGRO - opt (GCA675_1) </t>
+          <t>AGRO - 8 (GCA245_1)</t>
+        </is>
+      </c>
+      <c r="E16" s="7" t="inlineStr">
+        <is>
+          <t>AGRO - 8 (GCS073_1)</t>
+        </is>
+      </c>
+      <c r="F16" s="7" t="inlineStr">
+        <is>
+          <t>AGRO - 8 (GCA257_1)</t>
+        </is>
+      </c>
+      <c r="G16" s="7" t="inlineStr">
+        <is>
+          <t>AGRO - opt (GCA657_1)</t>
         </is>
       </c>
       <c r="H16" s="7" t="inlineStr">
@@ -1984,29 +1984,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I16" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 4 (GEX116_1 - GEX116_2) </t>
+      <c r="I16" s="7" t="inlineStr">
+        <is>
+          <t>AGRO - 8 (GCA224_1)</t>
         </is>
       </c>
       <c r="J16" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 4 (GCH012_1)</t>
+          <t>AGRO - 8 (GCS056_1)</t>
         </is>
       </c>
       <c r="K16" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 4 (GCA034_1)</t>
+          <t>AGRO - 8 (GCA221_1)</t>
         </is>
       </c>
       <c r="L16" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 4 (GCH008_1)</t>
+          <t>AGRO - 8 (GCA255_1)</t>
         </is>
       </c>
       <c r="M16" s="7" t="inlineStr">
         <is>
-          <t>AGRO - opt (GCA315_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N16" s="7" t="inlineStr">
@@ -2014,29 +2014,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O16" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CS - 2 (GCH1325_1 - GLA102_1) </t>
+      <c r="O16" s="7" t="inlineStr">
+        <is>
+          <t>CS - 4 (GCH1394_1)</t>
         </is>
       </c>
       <c r="P16" s="7" t="inlineStr">
         <is>
-          <t>CS - 2 (GCH1334_1)</t>
-        </is>
-      </c>
-      <c r="Q16" s="7" t="inlineStr">
-        <is>
-          <t>CS - 2 (GCH1388_1)</t>
+          <t>CS - 6 (GCH1405_1)</t>
+        </is>
+      </c>
+      <c r="Q16" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CS - opt (GCH1420_1 - GCH1433_1) </t>
         </is>
       </c>
       <c r="R16" s="7" t="inlineStr">
         <is>
-          <t>CS - 2 (GCH1333_1)</t>
+          <t>CS - 6 (GCH1678_1)</t>
         </is>
       </c>
       <c r="S16" s="7" t="inlineStr">
         <is>
-          <t>CS - 2 (GCH292_9)</t>
+          <t>CS - 4 (GCH1396_1)</t>
         </is>
       </c>
       <c r="T16" s="7" t="inlineStr">
@@ -2046,35 +2046,35 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="9" t="n"/>
+      <c r="A17" s="10" t="n"/>
       <c r="B17" s="6" t="inlineStr">
         <is>
           <t>304-A</t>
         </is>
       </c>
-      <c r="C17" s="7" t="inlineStr">
-        <is>
-          <t>AGRO - 8 (GCA269_1)</t>
+      <c r="C17" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 4 (GCA210_1 - GCA210_2) </t>
         </is>
       </c>
       <c r="D17" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 8 (GCA245_1)</t>
-        </is>
-      </c>
-      <c r="E17" s="7" t="inlineStr">
-        <is>
-          <t>AGRO - 8 (GCS073_1)</t>
-        </is>
-      </c>
-      <c r="F17" s="7" t="inlineStr">
-        <is>
-          <t>AGRO - 8 (GCA257_1)</t>
+          <t>AGRO - opt (GEX431_1)</t>
+        </is>
+      </c>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 4 (GCA218_2) | AGRO - 4 (GCB130_1) </t>
+        </is>
+      </c>
+      <c r="F17" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 4 (GCA037_1 - GCA037_2) </t>
         </is>
       </c>
       <c r="G17" s="7" t="inlineStr">
         <is>
-          <t>AGRO - opt (GCA657_1)</t>
+          <t>AGRO - opt (GCA588_1)</t>
         </is>
       </c>
       <c r="H17" s="7" t="inlineStr">
@@ -2082,29 +2082,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I17" s="7" t="inlineStr">
-        <is>
-          <t>AGRO - 8 (GCA224_1)</t>
+      <c r="I17" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 4 (GEX116_1 - GEX116_2) </t>
         </is>
       </c>
       <c r="J17" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 8 (GCS056_1)</t>
+          <t>AGRO - 4 (GCH012_1)</t>
         </is>
       </c>
       <c r="K17" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 8 (GCA221_1)</t>
+          <t>AGRO - 4 (GCA034_1)</t>
         </is>
       </c>
       <c r="L17" s="7" t="inlineStr">
         <is>
-          <t>AGRO - 8 (GCA255_1)</t>
+          <t>AGRO - 4 (GCH008_1)</t>
         </is>
       </c>
       <c r="M17" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA315_1)</t>
         </is>
       </c>
       <c r="N17" s="7" t="inlineStr">
@@ -2112,29 +2112,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O17" s="7" t="inlineStr">
-        <is>
-          <t>CS - 6 (GCH1402_1)</t>
+      <c r="O17" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CS - 2 (GCH1325_1 - GLA102_1) </t>
         </is>
       </c>
       <c r="P17" s="7" t="inlineStr">
         <is>
-          <t>CS - 6 (GCH1405_1)</t>
+          <t>CS - 2 (GCH1334_1)</t>
         </is>
       </c>
       <c r="Q17" s="7" t="inlineStr">
         <is>
-          <t>CS - 6 (GCH1404_1)</t>
+          <t>CS - 2 (GCH1388_1)</t>
         </is>
       </c>
       <c r="R17" s="7" t="inlineStr">
         <is>
-          <t>CS - 6 (GCH1678_1)</t>
+          <t>CS - 2 (GCH1333_1)</t>
         </is>
       </c>
       <c r="S17" s="7" t="inlineStr">
         <is>
-          <t>CS - 6 (GCH1403_1)</t>
+          <t>CS - 2 (GCH292_9)</t>
         </is>
       </c>
       <c r="T17" s="7" t="inlineStr">
@@ -2144,7 +2144,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="9" t="n"/>
+      <c r="A18" s="10" t="n"/>
       <c r="B18" s="6" t="inlineStr">
         <is>
           <t>305-A</t>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="D18" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 10 (GSA049_1)</t>
         </is>
       </c>
       <c r="E18" s="7" t="inlineStr">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="G18" s="7" t="inlineStr">
         <is>
-          <t>AGRO - opt (GCA588_1)</t>
+          <t>AGRO - opt (GCA675_1)</t>
         </is>
       </c>
       <c r="H18" s="7" t="inlineStr">
@@ -2212,7 +2212,7 @@
       </c>
       <c r="O18" s="7" t="inlineStr">
         <is>
-          <t>CS - 4 (GCH1394_1)</t>
+          <t>CS - 6 (GCH1402_1)</t>
         </is>
       </c>
       <c r="P18" s="7" t="inlineStr">
@@ -2220,19 +2220,19 @@
           <t>CS - 8 (GCH1410_1)</t>
         </is>
       </c>
-      <c r="Q18" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CS - opt (GCH1420_1 - GCH1433_1) </t>
-        </is>
-      </c>
-      <c r="R18" s="7" t="inlineStr">
-        <is>
-          <t>CS - 4 (GCH1395_1)</t>
+      <c r="Q18" s="7" t="inlineStr">
+        <is>
+          <t>CS - 6 (GCH1404_1)</t>
+        </is>
+      </c>
+      <c r="R18" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CS - 8 (GCH1457_1 - GCH1460_1) </t>
         </is>
       </c>
       <c r="S18" s="7" t="inlineStr">
         <is>
-          <t>CS - 4 (GCH1396_1)</t>
+          <t>CS - 6 (GCH1403_1)</t>
         </is>
       </c>
       <c r="T18" s="7" t="inlineStr">
@@ -2242,7 +2242,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="9" t="n"/>
+      <c r="A19" s="10" t="n"/>
       <c r="B19" s="6" t="inlineStr">
         <is>
           <t>306-A</t>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="D19" s="7" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA049_1)</t>
+          <t>ENF - 2 (GEX212_1)</t>
         </is>
       </c>
       <c r="E19" s="7" t="inlineStr">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="G19" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 4 (GCA045_1)</t>
         </is>
       </c>
       <c r="H19" s="7" t="inlineStr">
@@ -2340,7 +2340,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="9" t="n"/>
+      <c r="A20" s="10" t="n"/>
       <c r="B20" s="6" t="inlineStr">
         <is>
           <t>307-A</t>
@@ -2348,22 +2348,22 @@
       </c>
       <c r="C20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA021_1)</t>
+          <t>ENF - 4 (GCB064_2)</t>
         </is>
       </c>
       <c r="D20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA021_1)</t>
+          <t>ENF - 4 (GSA017_1)</t>
         </is>
       </c>
       <c r="E20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA021_1)</t>
+          <t>ENF - 4 (GSA017_1)</t>
         </is>
       </c>
       <c r="F20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA021_1)</t>
+          <t>ENF - 4 (GSA017_1)</t>
         </is>
       </c>
       <c r="G20" s="7" t="inlineStr">
@@ -2378,27 +2378,27 @@
       </c>
       <c r="I20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA021_1)</t>
+          <t>ENF - 2 (GCB064_1)</t>
         </is>
       </c>
       <c r="J20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA044_1)</t>
+          <t>ENF - 2 (GSA0303_1)</t>
         </is>
       </c>
       <c r="K20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA021_1)</t>
+          <t>ENF - 2 (GSA0303_1)</t>
         </is>
       </c>
       <c r="L20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA044_1)</t>
+          <t>ENF - 2 (GCB019_1)</t>
         </is>
       </c>
       <c r="M20" s="7" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA021_1)</t>
+          <t>ENF - 4 (GCB019_2)</t>
         </is>
       </c>
       <c r="N20" s="7" t="inlineStr">
@@ -2408,27 +2408,27 @@
       </c>
       <c r="O20" s="7" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH290_15)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P20" s="7" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH291_3)</t>
+          <t>HIS - 4 (GCH372_1)</t>
         </is>
       </c>
       <c r="Q20" s="7" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH366_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R20" s="7" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH365_1)</t>
+          <t>HIS - 4 (GCH371_1)</t>
         </is>
       </c>
       <c r="S20" s="7" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH367_1)</t>
+          <t>HIS - 4 (GCH373_1)</t>
         </is>
       </c>
       <c r="T20" s="7" t="inlineStr">
@@ -2438,7 +2438,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="9" t="n"/>
+      <c r="A21" s="10" t="n"/>
       <c r="B21" s="6" t="inlineStr">
         <is>
           <t>308-A</t>
@@ -2446,22 +2446,22 @@
       </c>
       <c r="C21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GCB064_2)</t>
+          <t>ENF - 6 (GSA021_1)</t>
         </is>
       </c>
       <c r="D21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GSA017_1)</t>
+          <t>ENF - 6 (GSA021_1)</t>
         </is>
       </c>
       <c r="E21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GSA017_1)</t>
+          <t>ENF - 6 (GSA021_1)</t>
         </is>
       </c>
       <c r="F21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GSA017_1)</t>
+          <t>ENF - 6 (GSA021_1)</t>
         </is>
       </c>
       <c r="G21" s="7" t="inlineStr">
@@ -2476,27 +2476,27 @@
       </c>
       <c r="I21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GCH012_2)</t>
+          <t>ENF - 6 (GSA021_1)</t>
         </is>
       </c>
       <c r="J21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 2 (GSA0303_1)</t>
+          <t>ENF - 6 (GSA044_1)</t>
         </is>
       </c>
       <c r="K21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 2 (GSA0303_1)</t>
-        </is>
-      </c>
-      <c r="L21" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ENF - 4 (GCB029_1 - GCB076_1) </t>
+          <t>ENF - 6 (GSA021_1)</t>
+        </is>
+      </c>
+      <c r="L21" s="7" t="inlineStr">
+        <is>
+          <t>ENF - 6 (GSA044_1)</t>
         </is>
       </c>
       <c r="M21" s="7" t="inlineStr">
         <is>
-          <t>ENF - 4 (GCB019_2)</t>
+          <t>ENF - 6 (GSA021_1)</t>
         </is>
       </c>
       <c r="N21" s="7" t="inlineStr">
@@ -2506,27 +2506,27 @@
       </c>
       <c r="O21" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 2 (GCH290_15)</t>
         </is>
       </c>
       <c r="P21" s="7" t="inlineStr">
         <is>
-          <t>HIS - 4 (GCH372_1)</t>
+          <t>HIS - 2 (GCH291_3)</t>
         </is>
       </c>
       <c r="Q21" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 2 (GCH366_1)</t>
         </is>
       </c>
       <c r="R21" s="7" t="inlineStr">
         <is>
-          <t>HIS - 4 (GCH371_1)</t>
+          <t>HIS - 2 (GCH365_1)</t>
         </is>
       </c>
       <c r="S21" s="7" t="inlineStr">
         <is>
-          <t>HIS - 4 (GCH373_1)</t>
+          <t>HIS - 2 (GCH367_1)</t>
         </is>
       </c>
       <c r="T21" s="7" t="inlineStr">
@@ -2536,7 +2536,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="9" t="n"/>
+      <c r="A22" s="10" t="n"/>
       <c r="B22" s="6" t="inlineStr">
         <is>
           <t>309-A</t>
@@ -2604,27 +2604,27 @@
       </c>
       <c r="O22" s="7" t="inlineStr">
         <is>
-          <t>LET - 8 (GLA391_1)</t>
-        </is>
-      </c>
-      <c r="P22" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - 8 (GLA388_1 - GLA389_1) </t>
+          <t>LET - 2 (GCS238_4)</t>
+        </is>
+      </c>
+      <c r="P22" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LET - 2 (GCH290_14 - GLA358_1) </t>
         </is>
       </c>
       <c r="Q22" s="7" t="inlineStr">
         <is>
-          <t>LET - 8 (GLA390_1)</t>
+          <t>LET - 2 (GLA359_1)</t>
         </is>
       </c>
       <c r="R22" s="7" t="inlineStr">
         <is>
-          <t>LET - 8 (GLA392_1)</t>
+          <t>LET - 2 (GCH293_5)</t>
         </is>
       </c>
       <c r="S22" s="7" t="inlineStr">
         <is>
-          <t>LET - 8 (GLA387_1)</t>
+          <t>LET - 2 (GLA360_1)</t>
         </is>
       </c>
       <c r="T22" s="7" t="inlineStr">
@@ -2634,7 +2634,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="9" t="n"/>
+      <c r="A23" s="10" t="n"/>
       <c r="B23" s="6" t="inlineStr">
         <is>
           <t>401-A</t>
@@ -2675,9 +2675,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="J23" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 6 (GCA286_1 - GCA286_2) </t>
         </is>
       </c>
       <c r="K23" s="7" t="inlineStr">
@@ -2700,29 +2700,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O23" s="10" t="inlineStr">
-        <is>
-          <t>CS - 8 + HIS - 4 (GCS238_5)</t>
+      <c r="O23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="P23" s="7" t="inlineStr">
         <is>
-          <t>CS - 4 (GCH1397_1)</t>
-        </is>
-      </c>
-      <c r="Q23" s="10" t="inlineStr">
-        <is>
-          <t>CS - 4 + FIL - 4 + MAT - 4 (GCH838_1)</t>
-        </is>
-      </c>
-      <c r="R23" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CS - 8 (GCH1457_1 - GCH1460_1) </t>
-        </is>
-      </c>
-      <c r="S23" s="10" t="inlineStr">
-        <is>
-          <t>CS - 8 + MAT - 6 + PED - 7 (GCH1031_1)</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="T23" s="7" t="inlineStr">
@@ -2732,10 +2732,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="9" t="n"/>
+      <c r="A24" s="10" t="n"/>
       <c r="B24" s="6" t="inlineStr">
         <is>
-          <t>407-A</t>
+          <t>105-B</t>
         </is>
       </c>
       <c r="C24" s="7" t="inlineStr">
@@ -2810,12 +2810,12 @@
       </c>
       <c r="Q24" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - opt (GCH1301_1)</t>
         </is>
       </c>
       <c r="R24" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - opt (GCH1286_1)</t>
         </is>
       </c>
       <c r="S24" s="7" t="inlineStr">
@@ -2830,10 +2830,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="9" t="n"/>
+      <c r="A25" s="10" t="n"/>
       <c r="B25" s="6" t="inlineStr">
         <is>
-          <t>408-A</t>
+          <t>108-B</t>
         </is>
       </c>
       <c r="C25" s="7" t="inlineStr">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="I25" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GCS011_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J25" s="7" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="K25" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GLA004_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L25" s="7" t="inlineStr">
@@ -2898,22 +2898,22 @@
       </c>
       <c r="O25" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 1 (GCH293_2)</t>
         </is>
       </c>
       <c r="P25" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GCS239_10)</t>
-        </is>
-      </c>
-      <c r="Q25" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LET - opt (GCH293_4 - GLA004_3) </t>
+          <t>CC - 1 (GEX208_1)</t>
+        </is>
+      </c>
+      <c r="Q25" s="7" t="inlineStr">
+        <is>
+          <t>CC - 1 (GEX213_1)</t>
         </is>
       </c>
       <c r="R25" s="7" t="inlineStr">
         <is>
-          <t>LET - opt (GEX006_2)</t>
+          <t>CC - 1 (GEX003_2)</t>
         </is>
       </c>
       <c r="S25" s="7" t="inlineStr">
@@ -2928,10 +2928,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="9" t="n"/>
+      <c r="A26" s="10" t="n"/>
       <c r="B26" s="6" t="inlineStr">
         <is>
-          <t>408-B</t>
+          <t>201-B</t>
         </is>
       </c>
       <c r="C26" s="7" t="inlineStr">
@@ -2996,27 +2996,27 @@
       </c>
       <c r="O26" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GCH293_2)</t>
+          <t>CC - opt (GEX635_1)</t>
         </is>
       </c>
       <c r="P26" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX208_1)</t>
+          <t>ADM - 7 (GCS077_1)</t>
         </is>
       </c>
       <c r="Q26" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX213_1)</t>
+          <t>ADM - 7 (GCS544_1)</t>
         </is>
       </c>
       <c r="R26" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_2)</t>
+          <t>CC - opt (GEX1083_1)</t>
         </is>
       </c>
       <c r="S26" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 7 (GCS239_3)</t>
         </is>
       </c>
       <c r="T26" s="7" t="inlineStr">
@@ -3026,10 +3026,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="9" t="n"/>
+      <c r="A27" s="10" t="n"/>
       <c r="B27" s="6" t="inlineStr">
         <is>
-          <t>105-B</t>
+          <t>202-B</t>
         </is>
       </c>
       <c r="C27" s="7" t="inlineStr">
@@ -3037,29 +3037,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D27" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="D27" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 2 (GCH1038_1 - GCH1039_1) </t>
         </is>
       </c>
       <c r="E27" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 2 (GCH1037_1)</t>
         </is>
       </c>
       <c r="F27" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 2 (GCH839_1)</t>
         </is>
       </c>
       <c r="G27" s="7" t="inlineStr">
         <is>
-          <t>PED - 6 (GCH1116_1)</t>
+          <t>PED - 2 (GCS239_4)</t>
         </is>
       </c>
       <c r="H27" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 2 (GCH839_1)</t>
         </is>
       </c>
       <c r="I27" s="7" t="inlineStr">
@@ -3094,27 +3094,27 @@
       </c>
       <c r="O27" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 5 (GLA237_1)</t>
         </is>
       </c>
       <c r="P27" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 5 (GCH1111_1)</t>
         </is>
       </c>
       <c r="Q27" s="7" t="inlineStr">
         <is>
-          <t>PED - opt (GCH1301_1)</t>
+          <t>PED - 5 (GCH1110_1)</t>
         </is>
       </c>
       <c r="R27" s="7" t="inlineStr">
         <is>
-          <t>PED - opt (GCH1286_1)</t>
-        </is>
-      </c>
-      <c r="S27" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>PED - 5 (GCH1107_1)</t>
+        </is>
+      </c>
+      <c r="S27" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 5 (GCH1108_1 - GCH1109_1) </t>
         </is>
       </c>
       <c r="T27" s="7" t="inlineStr">
@@ -3124,40 +3124,40 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="9" t="n"/>
+      <c r="A28" s="10" t="n"/>
       <c r="B28" s="6" t="inlineStr">
         <is>
-          <t>108-B</t>
+          <t>203-B</t>
         </is>
       </c>
       <c r="C28" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 8 (GEX777_1)</t>
         </is>
       </c>
       <c r="D28" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 8 (GCH1123_1)</t>
         </is>
       </c>
       <c r="E28" s="7" t="inlineStr">
         <is>
-          <t>ADM - opt (GCS556_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F28" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G28" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>PED - 8 (GCH1124_1)</t>
+        </is>
+      </c>
+      <c r="G28" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 8 (GCH1122_1 - GCH1126_1) </t>
         </is>
       </c>
       <c r="H28" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 8 (GCH1121_1)</t>
         </is>
       </c>
       <c r="I28" s="7" t="inlineStr">
@@ -3192,27 +3192,27 @@
       </c>
       <c r="O28" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 3 (GCH1086_1)</t>
         </is>
       </c>
       <c r="P28" s="7" t="inlineStr">
         <is>
-          <t>ADM - opt (GCS566_1)</t>
+          <t>PED - 3 (GCH1087_1)</t>
         </is>
       </c>
       <c r="Q28" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 3 (GCH833_2)</t>
         </is>
       </c>
       <c r="R28" s="7" t="inlineStr">
         <is>
-          <t>ADM - opt (GCS554_1)</t>
-        </is>
-      </c>
-      <c r="S28" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>PED - 3 (GCH840_2)</t>
+        </is>
+      </c>
+      <c r="S28" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 3 (GCH1088_1 - GCH1099_1) </t>
         </is>
       </c>
       <c r="T28" s="7" t="inlineStr">
@@ -3222,45 +3222,45 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="9" t="n"/>
+      <c r="A29" s="10" t="n"/>
       <c r="B29" s="6" t="inlineStr">
         <is>
-          <t>201-B</t>
+          <t>204-B</t>
         </is>
       </c>
       <c r="C29" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 6 (GLA239_1)</t>
         </is>
       </c>
       <c r="D29" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 6 (GCH1112_1)</t>
         </is>
       </c>
       <c r="E29" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F29" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G29" s="7" t="inlineStr">
-        <is>
-          <t>PED - 8 (GCH1126_1)</t>
-        </is>
-      </c>
-      <c r="H29" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>PED - 6 (GLA238_1)</t>
+        </is>
+      </c>
+      <c r="F29" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 6 (GCH1114_1 - GCH1115_1) </t>
+        </is>
+      </c>
+      <c r="G29" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 6 (GCH1113_1 - GCH1116_1) </t>
+        </is>
+      </c>
+      <c r="H29" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 9 (GCH1128_1 - GCH1131_1) </t>
         </is>
       </c>
       <c r="I29" s="7" t="inlineStr">
         <is>
-          <t>CC - 2 (GEN253_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J29" s="7" t="inlineStr">
@@ -3283,34 +3283,34 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N29" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="N29" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 9 (GCH1128_1 - GCH1131_1) </t>
         </is>
       </c>
       <c r="O29" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX098_1)</t>
-        </is>
-      </c>
-      <c r="P29" s="7" t="inlineStr">
-        <is>
-          <t>ADM - 9 (GCS549_1)</t>
-        </is>
-      </c>
-      <c r="Q29" s="7" t="inlineStr">
-        <is>
-          <t>ADM - 9 (GCS551_1)</t>
+          <t>PED - 9 (GCH1130_1)</t>
+        </is>
+      </c>
+      <c r="P29" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 9 (GCH1128_1 - GCH1131_1) </t>
+        </is>
+      </c>
+      <c r="Q29" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 9 (GCH1129_1 - GCH1279_1) </t>
         </is>
       </c>
       <c r="R29" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX606_1)</t>
+          <t>PED - 9 (GCH1280_1)</t>
         </is>
       </c>
       <c r="S29" s="7" t="inlineStr">
         <is>
-          <t>ADM - 9 (GCS573_1)</t>
+          <t>PED - 9 (GCH1127_1)</t>
         </is>
       </c>
       <c r="T29" s="7" t="inlineStr">
@@ -3320,40 +3320,40 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="9" t="n"/>
+      <c r="A30" s="10" t="n"/>
       <c r="B30" s="6" t="inlineStr">
         <is>
-          <t>202-B</t>
+          <t>205-B</t>
         </is>
       </c>
       <c r="C30" s="7" t="inlineStr">
         <is>
-          <t>PED - 6 (GLA239_1)</t>
+          <t>PED - 10 (GCH1133_1)</t>
         </is>
       </c>
       <c r="D30" s="7" t="inlineStr">
         <is>
-          <t>PED - 6 (GCH1112_1)</t>
-        </is>
-      </c>
-      <c r="E30" s="7" t="inlineStr">
-        <is>
-          <t>PED - 6 (GLA238_1)</t>
-        </is>
-      </c>
-      <c r="F30" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 6 (GCH1114_1 - GCH1115_1) </t>
-        </is>
-      </c>
-      <c r="G30" s="7" t="inlineStr">
-        <is>
-          <t>PED - 6 (GCH1113_1)</t>
-        </is>
-      </c>
-      <c r="H30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E30" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - opt (GCH1302_1 - GCH1303_1) </t>
+        </is>
+      </c>
+      <c r="F30" s="7" t="inlineStr">
+        <is>
+          <t>PED - 10 (GCS238_3)</t>
+        </is>
+      </c>
+      <c r="G30" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 10 (GCH1132_1 - GCH1134_1) </t>
+        </is>
+      </c>
+      <c r="H30" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 7 (GCH1117_1 - GCH1120_1) </t>
         </is>
       </c>
       <c r="I30" s="7" t="inlineStr">
@@ -3381,34 +3381,34 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="N30" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 7 (GCH1117_1 - GCH1120_1) </t>
         </is>
       </c>
       <c r="O30" s="7" t="inlineStr">
         <is>
-          <t>PED - 5 (GLA237_1)</t>
-        </is>
-      </c>
-      <c r="P30" s="7" t="inlineStr">
-        <is>
-          <t>PED - 5 (GCH1111_1)</t>
-        </is>
-      </c>
-      <c r="Q30" s="7" t="inlineStr">
-        <is>
-          <t>PED - 5 (GCH1110_1)</t>
-        </is>
-      </c>
-      <c r="R30" s="7" t="inlineStr">
-        <is>
-          <t>PED - 5 (GCH1107_1)</t>
-        </is>
-      </c>
-      <c r="S30" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 5 (GCH1108_1 - GCH1109_1) </t>
+          <t>PED - 7 (GLA213_1)</t>
+        </is>
+      </c>
+      <c r="P30" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 7 (GCH1118_1 - GEX776_1) </t>
+        </is>
+      </c>
+      <c r="Q30" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 7 (GCH1117_1 - GCH1120_1) </t>
+        </is>
+      </c>
+      <c r="R30" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 7 (GCH160_1 - GLA240_1) </t>
+        </is>
+      </c>
+      <c r="S30" s="7" t="inlineStr">
+        <is>
+          <t>PED - opt (GCH1284_1)</t>
         </is>
       </c>
       <c r="T30" s="7" t="inlineStr">
@@ -3418,40 +3418,40 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="9" t="n"/>
+      <c r="A31" s="10" t="n"/>
       <c r="B31" s="6" t="inlineStr">
         <is>
-          <t>203-B</t>
-        </is>
-      </c>
-      <c r="C31" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D31" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 2 (GCH1038_1 - GCH1039_1) </t>
-        </is>
-      </c>
-      <c r="E31" s="7" t="inlineStr">
-        <is>
-          <t>PED - 2 (GCH1037_1)</t>
+          <t>206-B</t>
+        </is>
+      </c>
+      <c r="C31" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 4 (GCH1102_1 - GCH1106_1) </t>
+        </is>
+      </c>
+      <c r="D31" s="7" t="inlineStr">
+        <is>
+          <t>PED - 4 (GCH838_2)</t>
+        </is>
+      </c>
+      <c r="E31" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 4 (GCH1104_1 - GCH1105_1) </t>
         </is>
       </c>
       <c r="F31" s="7" t="inlineStr">
         <is>
-          <t>PED - 2 (GCH839_1)</t>
+          <t>PED - 4 (GCH1103_1)</t>
         </is>
       </c>
       <c r="G31" s="7" t="inlineStr">
         <is>
-          <t>PED - 2 (GCS239_4)</t>
+          <t>PED - 4 (GEX210_4)</t>
         </is>
       </c>
       <c r="H31" s="7" t="inlineStr">
         <is>
-          <t>PED - 2 (GCH839_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I31" s="7" t="inlineStr">
@@ -3484,7 +3484,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O31" s="11" t="inlineStr">
+      <c r="O31" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">PED - 1 (GCH1036_1 - GCH1100_1) </t>
         </is>
@@ -3516,40 +3516,40 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="9" t="n"/>
+      <c r="A32" s="10" t="n"/>
       <c r="B32" s="6" t="inlineStr">
         <is>
-          <t>204-B</t>
+          <t>207-B</t>
         </is>
       </c>
       <c r="C32" s="7" t="inlineStr">
         <is>
-          <t>PED - 10 (GCH1133_1)</t>
+          <t>ADM - 8 (GCS235_1)</t>
         </is>
       </c>
       <c r="D32" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E32" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - opt (GCH1302_1 - GCH1303_1) </t>
+          <t>ADM - 8 (GCS546_1)</t>
+        </is>
+      </c>
+      <c r="E32" s="7" t="inlineStr">
+        <is>
+          <t>ADM - 8 (GCS548_1)</t>
         </is>
       </c>
       <c r="F32" s="7" t="inlineStr">
         <is>
-          <t>PED - 10 (GCS238_3)</t>
-        </is>
-      </c>
-      <c r="G32" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 10 (GCH1132_1 - GCH1134_1) </t>
-        </is>
-      </c>
-      <c r="H32" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 7 (GCH1117_1 - GCH1120_1) </t>
+          <t>ADM - 8 (GCS082_1)</t>
+        </is>
+      </c>
+      <c r="G32" s="7" t="inlineStr">
+        <is>
+          <t>ADM - 8 (GCS547_1)</t>
+        </is>
+      </c>
+      <c r="H32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="I32" s="7" t="inlineStr">
@@ -3564,12 +3564,12 @@
       </c>
       <c r="K32" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 9 (GCS552_1)</t>
         </is>
       </c>
       <c r="L32" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 9 (GCS552_1)</t>
         </is>
       </c>
       <c r="M32" s="7" t="inlineStr">
@@ -3577,34 +3577,34 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N32" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 7 (GCH1117_1 - GCH1120_1) </t>
+      <c r="N32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="O32" s="7" t="inlineStr">
         <is>
-          <t>PED - 7 (GLA213_1)</t>
-        </is>
-      </c>
-      <c r="P32" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 7 (GCH1118_1 - GEX776_1) </t>
-        </is>
-      </c>
-      <c r="Q32" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 7 (GCH1117_1 - GCH1120_1) </t>
-        </is>
-      </c>
-      <c r="R32" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 7 (GCH160_1 - GLA240_1) </t>
+          <t>ADM - 7 (GCS080_1)</t>
+        </is>
+      </c>
+      <c r="P32" s="7" t="inlineStr">
+        <is>
+          <t>ADM - 9 (GCS549_1)</t>
+        </is>
+      </c>
+      <c r="Q32" s="7" t="inlineStr">
+        <is>
+          <t>ADM - 9 (GCS551_1)</t>
+        </is>
+      </c>
+      <c r="R32" s="7" t="inlineStr">
+        <is>
+          <t>ADM - 7 (GCS545_1)</t>
         </is>
       </c>
       <c r="S32" s="7" t="inlineStr">
         <is>
-          <t>PED - opt (GCH1284_1)</t>
+          <t>ADM - 9 (GCS573_1)</t>
         </is>
       </c>
       <c r="T32" s="7" t="inlineStr">
@@ -3614,40 +3614,40 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="9" t="n"/>
+      <c r="A33" s="10" t="n"/>
       <c r="B33" s="6" t="inlineStr">
         <is>
-          <t>205-B</t>
-        </is>
-      </c>
-      <c r="C33" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 4 (GCH1102_1 - GCH1106_1) </t>
+          <t>208-B</t>
+        </is>
+      </c>
+      <c r="C33" s="7" t="inlineStr">
+        <is>
+          <t>ADM - 2 (GCH293_3)</t>
         </is>
       </c>
       <c r="D33" s="7" t="inlineStr">
         <is>
-          <t>PED - 4 (GCH838_2)</t>
-        </is>
-      </c>
-      <c r="E33" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 4 (GCH1104_1 - GCH1105_1) </t>
+          <t>ADM - 2 (GCS527_1)</t>
+        </is>
+      </c>
+      <c r="E33" s="7" t="inlineStr">
+        <is>
+          <t>ADM - 2 (GEX094_1)</t>
         </is>
       </c>
       <c r="F33" s="7" t="inlineStr">
         <is>
-          <t>PED - 4 (GCH1103_1)</t>
+          <t>ADM - 2 (GCS526_1)</t>
         </is>
       </c>
       <c r="G33" s="7" t="inlineStr">
         <is>
-          <t>PED - 4 (GEX210_4)</t>
-        </is>
-      </c>
-      <c r="H33" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 9 (GCH1128_1 - GCH1131_1) </t>
+          <t>ADM - 2 (GCS238_9)</t>
+        </is>
+      </c>
+      <c r="H33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="I33" s="7" t="inlineStr">
@@ -3675,34 +3675,34 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N33" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 9 (GCH1128_1 - GCH1131_1) </t>
+      <c r="N33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="O33" s="7" t="inlineStr">
         <is>
-          <t>PED - 9 (GCH1130_1)</t>
-        </is>
-      </c>
-      <c r="P33" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 9 (GCH1128_1 - GCH1131_1) </t>
-        </is>
-      </c>
-      <c r="Q33" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 9 (GCH1129_1 - GCH1279_1) </t>
+          <t>ADM - 1 (GEX212_4)</t>
+        </is>
+      </c>
+      <c r="P33" s="7" t="inlineStr">
+        <is>
+          <t>ADM - 1 (GCH290_11)</t>
+        </is>
+      </c>
+      <c r="Q33" s="7" t="inlineStr">
+        <is>
+          <t>ADM - 1 (GCS534_1)</t>
         </is>
       </c>
       <c r="R33" s="7" t="inlineStr">
         <is>
-          <t>PED - 9 (GCH1280_1)</t>
+          <t>ADM - 1 (GLA104_3)</t>
         </is>
       </c>
       <c r="S33" s="7" t="inlineStr">
         <is>
-          <t>PED - 9 (GCH1127_1)</t>
+          <t>ADM - 1 (GCS525_1)</t>
         </is>
       </c>
       <c r="T33" s="7" t="inlineStr">
@@ -3712,40 +3712,40 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="9" t="n"/>
+      <c r="A34" s="10" t="n"/>
       <c r="B34" s="6" t="inlineStr">
         <is>
-          <t>206-B</t>
+          <t>209-B</t>
         </is>
       </c>
       <c r="C34" s="7" t="inlineStr">
         <is>
-          <t>PED - 8 (GEX777_1)</t>
+          <t>ADM - 6 (GCS072_1)</t>
         </is>
       </c>
       <c r="D34" s="7" t="inlineStr">
         <is>
-          <t>PED - 8 (GCH1123_1)</t>
+          <t>ADM - 6 (GCS541_1)</t>
         </is>
       </c>
       <c r="E34" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 6 (GCS543_1)</t>
         </is>
       </c>
       <c r="F34" s="7" t="inlineStr">
         <is>
-          <t>PED - 8 (GCH1124_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G34" s="7" t="inlineStr">
         <is>
-          <t>PED - 8 (GCH1122_1)</t>
+          <t>ADM - 6 (GCS542_1)</t>
         </is>
       </c>
       <c r="H34" s="7" t="inlineStr">
         <is>
-          <t>PED - 8 (GCH1121_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I34" s="7" t="inlineStr">
@@ -3780,27 +3780,27 @@
       </c>
       <c r="O34" s="7" t="inlineStr">
         <is>
-          <t>PED - 3 (GCH1086_1)</t>
+          <t>ADM - 5 (GCS538_1)</t>
         </is>
       </c>
       <c r="P34" s="7" t="inlineStr">
         <is>
-          <t>PED - 3 (GCH1087_1)</t>
+          <t>ADM - 5 (GCS540_1)</t>
         </is>
       </c>
       <c r="Q34" s="7" t="inlineStr">
         <is>
-          <t>PED - 3 (GCH833_2)</t>
+          <t>ADM - 5 (GCS536_1)</t>
         </is>
       </c>
       <c r="R34" s="7" t="inlineStr">
         <is>
-          <t>PED - 3 (GCH840_2)</t>
-        </is>
-      </c>
-      <c r="S34" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 3 (GCH1088_1 - GCH1099_1) </t>
+          <t>ADM - 5 (GCS537_1)</t>
+        </is>
+      </c>
+      <c r="S34" s="7" t="inlineStr">
+        <is>
+          <t>ADM - 5 (GCS539_1)</t>
         </is>
       </c>
       <c r="T34" s="7" t="inlineStr">
@@ -3810,40 +3810,40 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="9" t="n"/>
+      <c r="A35" s="10" t="n"/>
       <c r="B35" s="6" t="inlineStr">
         <is>
-          <t>207-B</t>
+          <t>210-B</t>
         </is>
       </c>
       <c r="C35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 6 (GCS072_1)</t>
+          <t>ADM - 4 (GCS532_1)</t>
         </is>
       </c>
       <c r="D35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 6 (GCS541_1)</t>
+          <t>ADM - 4 (GCS535_1)</t>
         </is>
       </c>
       <c r="E35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 6 (GCS543_1)</t>
+          <t>ADM - 4 (GCS533_1)</t>
         </is>
       </c>
       <c r="F35" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 4 (GCS066_1)</t>
         </is>
       </c>
       <c r="G35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 6 (GCS542_1)</t>
+          <t>ADM - 4 (GCS068_1)</t>
         </is>
       </c>
       <c r="H35" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 3 (GCS529_1)</t>
         </is>
       </c>
       <c r="I35" s="7" t="inlineStr">
@@ -3858,12 +3858,12 @@
       </c>
       <c r="K35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 9 (GCS552_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 9 (GCS552_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M35" s="7" t="inlineStr">
@@ -3878,27 +3878,27 @@
       </c>
       <c r="O35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 1 (GEX212_4)</t>
-        </is>
-      </c>
-      <c r="P35" s="7" t="inlineStr">
-        <is>
-          <t>ADM - 1 (GCH290_11)</t>
+          <t>ADM - 3 (GCS530_1)</t>
+        </is>
+      </c>
+      <c r="P35" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ADM - 3 (GCH087_1 - GCS528_1) </t>
         </is>
       </c>
       <c r="Q35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 1 (GCS534_1)</t>
+          <t>ADM - 3 (GEX210_3)</t>
         </is>
       </c>
       <c r="R35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 1 (GLA104_3)</t>
+          <t>ADM - 3 (GCS529_1)</t>
         </is>
       </c>
       <c r="S35" s="7" t="inlineStr">
         <is>
-          <t>ADM - 1 (GCS525_1)</t>
+          <t>ADM - 3 (GCS531_1)</t>
         </is>
       </c>
       <c r="T35" s="7" t="inlineStr">
@@ -3908,65 +3908,65 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="9" t="n"/>
+      <c r="A36" s="10" t="n"/>
       <c r="B36" s="6" t="inlineStr">
         <is>
-          <t>208-B</t>
-        </is>
-      </c>
-      <c r="C36" s="7" t="inlineStr">
-        <is>
-          <t>ADM - 4 (GCS532_1)</t>
+          <t>301-B</t>
+        </is>
+      </c>
+      <c r="C36" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 1 (GSA140_1) | MED - 1 (GSA271_1) </t>
         </is>
       </c>
       <c r="D36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 4 (GCS535_1)</t>
+          <t>MED - 1 (GSA271_1)</t>
         </is>
       </c>
       <c r="E36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 4 (GCS533_1)</t>
+          <t>MED - 1 (GSA140_1)</t>
         </is>
       </c>
       <c r="F36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 4 (GCS066_1)</t>
+          <t>MED - 1 (GCH290_13)</t>
         </is>
       </c>
       <c r="G36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 4 (GCS068_1)</t>
+          <t>MED - 1 (GSA271_1)</t>
         </is>
       </c>
       <c r="H36" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GEO - 2 (GCH620_1)</t>
         </is>
       </c>
       <c r="I36" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 1 (GCH293_8)</t>
         </is>
       </c>
       <c r="J36" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 1 (GSA142_1)</t>
         </is>
       </c>
       <c r="K36" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 1 (GSA271_1)</t>
         </is>
       </c>
       <c r="L36" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M36" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>MED - 1 (GSA142_1)</t>
+        </is>
+      </c>
+      <c r="M36" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 1 (GSA143_1) | MED - 1 (GSA268_1) </t>
         </is>
       </c>
       <c r="N36" s="7" t="inlineStr">
@@ -3976,27 +3976,27 @@
       </c>
       <c r="O36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 7 (GCS080_1)</t>
+          <t>GEO - 2 (GCH620_1)</t>
         </is>
       </c>
       <c r="P36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 7 (GCS077_1)</t>
+          <t>GEO - 2 (GEX557_1)</t>
         </is>
       </c>
       <c r="Q36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 7 (GCS544_1)</t>
+          <t>GEO - 2 (GCH290_8)</t>
         </is>
       </c>
       <c r="R36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 7 (GCS545_1)</t>
+          <t>GEO - 2 (GEX210_8)</t>
         </is>
       </c>
       <c r="S36" s="7" t="inlineStr">
         <is>
-          <t>ADM - 7 (GCS239_3)</t>
+          <t>MED - 1 (GLA104_8)</t>
         </is>
       </c>
       <c r="T36" s="7" t="inlineStr">
@@ -4006,35 +4006,35 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="9" t="n"/>
+      <c r="A37" s="10" t="n"/>
       <c r="B37" s="6" t="inlineStr">
         <is>
-          <t>209-B</t>
+          <t>302-B</t>
         </is>
       </c>
       <c r="C37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 2 (GCH293_3)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 2 (GCS527_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 2 (GEX094_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 2 (GCS526_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 2 (GCS238_9)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H37" s="7" t="inlineStr">
@@ -4049,7 +4049,7 @@
       </c>
       <c r="J37" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GEO - 8 (GCH628_1)</t>
         </is>
       </c>
       <c r="K37" s="7" t="inlineStr">
@@ -4069,32 +4069,32 @@
       </c>
       <c r="N37" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GEO - 9 (GCH637_1)</t>
         </is>
       </c>
       <c r="O37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 5 (GCS538_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 5 (GCS540_1)</t>
-        </is>
-      </c>
-      <c r="Q37" s="7" t="inlineStr">
-        <is>
-          <t>ADM - 5 (GCS536_1)</t>
+          <t>GEO - 8 (GCH628_1)</t>
+        </is>
+      </c>
+      <c r="Q37" s="11" t="inlineStr">
+        <is>
+          <t>GEO - 4 + HIS - 4 (GCH374_1)</t>
         </is>
       </c>
       <c r="R37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 5 (GCS537_1)</t>
+          <t>GEO - 8 (GCH292_10)</t>
         </is>
       </c>
       <c r="S37" s="7" t="inlineStr">
         <is>
-          <t>ADM - 5 (GCS539_1)</t>
+          <t>GEO - 8 (GCH634_1)</t>
         </is>
       </c>
       <c r="T37" s="7" t="inlineStr">
@@ -4104,60 +4104,60 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="9" t="n"/>
+      <c r="A38" s="10" t="n"/>
       <c r="B38" s="6" t="inlineStr">
         <is>
-          <t>210-B</t>
+          <t>303-B</t>
         </is>
       </c>
       <c r="C38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 8 (GCS235_1)</t>
+          <t>MED - 3 (GSA168_1)</t>
         </is>
       </c>
       <c r="D38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 8 (GCS546_1)</t>
+          <t>MED - 3 (GSA280_1)</t>
         </is>
       </c>
       <c r="E38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 8 (GCS548_1)</t>
+          <t>MED - 3 (GSA171_1)</t>
         </is>
       </c>
       <c r="F38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 8 (GCS082_1)</t>
+          <t>MED - 3 (GSA168_1)</t>
         </is>
       </c>
       <c r="G38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 8 (GCS547_1)</t>
+          <t>MED - 5 (GSA192_1)</t>
         </is>
       </c>
       <c r="H38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 3 (GCS529_1)</t>
-        </is>
-      </c>
-      <c r="I38" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J38" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>GEO - 4 (GEX559_1)</t>
+        </is>
+      </c>
+      <c r="I38" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 3 (GSA280_1) | MED - 9 (GSA296_1) </t>
+        </is>
+      </c>
+      <c r="J38" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 3 (GSA167_1) | MED - 3 (GSA280_1) </t>
         </is>
       </c>
       <c r="K38" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 3 (GSA169_1)</t>
         </is>
       </c>
       <c r="L38" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 3 (GSA167_1)</t>
         </is>
       </c>
       <c r="M38" s="7" t="inlineStr">
@@ -4172,27 +4172,27 @@
       </c>
       <c r="O38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 3 (GCS530_1)</t>
-        </is>
-      </c>
-      <c r="P38" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ADM - 3 (GCH087_1 - GCS528_1) </t>
+          <t>MED - 9 (GSA296_1)</t>
+        </is>
+      </c>
+      <c r="P38" s="7" t="inlineStr">
+        <is>
+          <t>GEO - 4 (GEX559_1)</t>
         </is>
       </c>
       <c r="Q38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 3 (GEX210_3)</t>
+          <t>MED - 5 (GSA192_1)</t>
         </is>
       </c>
       <c r="R38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 3 (GCS529_1)</t>
+          <t>GEO - 4 (GCH623_1)</t>
         </is>
       </c>
       <c r="S38" s="7" t="inlineStr">
         <is>
-          <t>ADM - 3 (GCS531_1)</t>
+          <t>GEO - 4 (GCH293_6)</t>
         </is>
       </c>
       <c r="T38" s="7" t="inlineStr">
@@ -4202,65 +4202,65 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="9" t="n"/>
+      <c r="A39" s="10" t="n"/>
       <c r="B39" s="6" t="inlineStr">
         <is>
-          <t>301-B</t>
-        </is>
-      </c>
-      <c r="C39" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 1 (GSA140_1) | MED - 1 (GSA271_1) </t>
+          <t>304-B</t>
+        </is>
+      </c>
+      <c r="C39" s="7" t="inlineStr">
+        <is>
+          <t>MED - 5 (GSA193_1)</t>
         </is>
       </c>
       <c r="D39" s="7" t="inlineStr">
         <is>
-          <t>MED - 1 (GSA271_1)</t>
+          <t>MED - 5 (GSA191_1)</t>
         </is>
       </c>
       <c r="E39" s="7" t="inlineStr">
         <is>
-          <t>MED - 1 (GSA140_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F39" s="7" t="inlineStr">
         <is>
-          <t>MED - 1 (GCH290_13)</t>
+          <t>MED - 5 (GSA189_1)</t>
         </is>
       </c>
       <c r="G39" s="7" t="inlineStr">
         <is>
-          <t>MED - 1 (GSA271_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H39" s="7" t="inlineStr">
         <is>
-          <t>GEO - 2 (GCH620_1)</t>
-        </is>
-      </c>
-      <c r="I39" s="7" t="inlineStr">
-        <is>
-          <t>MED - 1 (GCH293_8)</t>
-        </is>
-      </c>
-      <c r="J39" s="7" t="inlineStr">
-        <is>
-          <t>MED - 1 (GSA142_1)</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I39" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 8 (GCS239_2) | MED - 5 (GSA188_1)  | MED - 5 (GSA193_1) </t>
+        </is>
+      </c>
+      <c r="J39" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 5 (GSA191_1) | MED - 5 (GSA284_1) </t>
         </is>
       </c>
       <c r="K39" s="7" t="inlineStr">
         <is>
-          <t>MED - 1 (GSA271_1)</t>
-        </is>
-      </c>
-      <c r="L39" s="7" t="inlineStr">
-        <is>
-          <t>MED - 1 (GSA142_1)</t>
-        </is>
-      </c>
-      <c r="M39" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 1 (GSA143_1) | MED - 1 (GSA268_1) </t>
+          <t>MED - 5 (GSA188_1)</t>
+        </is>
+      </c>
+      <c r="L39" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 5 (GSA190_1) | MED - 5 (GSA283_1) </t>
+        </is>
+      </c>
+      <c r="M39" s="7" t="inlineStr">
+        <is>
+          <t>MED - 5 (GSA189_1)</t>
         </is>
       </c>
       <c r="N39" s="7" t="inlineStr">
@@ -4270,27 +4270,27 @@
       </c>
       <c r="O39" s="7" t="inlineStr">
         <is>
-          <t>GEO - 2 (GCH620_1)</t>
+          <t>CC - 3 (GEX098_2)</t>
         </is>
       </c>
       <c r="P39" s="7" t="inlineStr">
         <is>
-          <t>GEO - 2 (GEX557_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q39" s="7" t="inlineStr">
         <is>
-          <t>GEO - 2 (GCH290_8)</t>
-        </is>
-      </c>
-      <c r="R39" s="7" t="inlineStr">
-        <is>
-          <t>GEO - 2 (GEX210_8)</t>
+          <t>CC - 3 (GEX608_1)</t>
+        </is>
+      </c>
+      <c r="R39" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 5 (GSA190_1) | MED - 5 (GSA283_1) </t>
         </is>
       </c>
       <c r="S39" s="7" t="inlineStr">
         <is>
-          <t>MED - 1 (GLA104_8)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T39" s="7" t="inlineStr">
@@ -4300,10 +4300,10 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="9" t="n"/>
+      <c r="A40" s="10" t="n"/>
       <c r="B40" s="6" t="inlineStr">
         <is>
-          <t>302-B</t>
+          <t>305-B</t>
         </is>
       </c>
       <c r="C40" s="7" t="inlineStr">
@@ -4323,72 +4323,72 @@
       </c>
       <c r="F40" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 8 (GEX658_1)</t>
         </is>
       </c>
       <c r="G40" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 8 (GEX658_1)</t>
         </is>
       </c>
       <c r="H40" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I40" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>CC - 8 (GEX658_1)</t>
+        </is>
+      </c>
+      <c r="I40" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 8 (GCS239_2) | CC - 4 (GEX613_2) </t>
         </is>
       </c>
       <c r="J40" s="7" t="inlineStr">
         <is>
-          <t>GEO - 8 (GCH628_1)</t>
+          <t>CC - 4 (GEX102_1)</t>
         </is>
       </c>
       <c r="K40" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L40" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>CC - opt (GEX1082_1)</t>
+        </is>
+      </c>
+      <c r="L40" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEX102_1) | CC - opt (GEX1082_1) </t>
         </is>
       </c>
       <c r="M40" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX613_2)</t>
         </is>
       </c>
       <c r="N40" s="7" t="inlineStr">
         <is>
-          <t>GEO - 9 (GCH637_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O40" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 3 (GEX098_1)</t>
         </is>
       </c>
       <c r="P40" s="7" t="inlineStr">
         <is>
-          <t>GEO - 8 (GCH628_1)</t>
+          <t>CC - 3 (GEX392_1)</t>
         </is>
       </c>
       <c r="Q40" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GCH290_5)</t>
         </is>
       </c>
       <c r="R40" s="7" t="inlineStr">
         <is>
-          <t>GEO - 8 (GCH292_10)</t>
+          <t>CC - 3 (GEX606_1)</t>
         </is>
       </c>
       <c r="S40" s="7" t="inlineStr">
         <is>
-          <t>GEO - 8 (GCH634_1)</t>
+          <t>CC - 3 (GEX609_1)</t>
         </is>
       </c>
       <c r="T40" s="7" t="inlineStr">
@@ -4398,65 +4398,65 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="9" t="n"/>
+      <c r="A41" s="10" t="n"/>
       <c r="B41" s="6" t="inlineStr">
         <is>
-          <t>303-B</t>
+          <t>308-B</t>
         </is>
       </c>
       <c r="C41" s="7" t="inlineStr">
         <is>
-          <t>MED - 3 (GSA168_1)</t>
+          <t>CC - 4 (GEX612_1)</t>
         </is>
       </c>
       <c r="D41" s="7" t="inlineStr">
         <is>
-          <t>MED - 3 (GSA280_1)</t>
+          <t>CC - 4 (GEX612_1)</t>
         </is>
       </c>
       <c r="E41" s="7" t="inlineStr">
         <is>
-          <t>MED - 3 (GSA171_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F41" s="7" t="inlineStr">
         <is>
-          <t>MED - 3 (GSA168_1)</t>
+          <t>CC - 9 (GEX657_1)</t>
         </is>
       </c>
       <c r="G41" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 9 (GEX657_1)</t>
         </is>
       </c>
       <c r="H41" s="7" t="inlineStr">
         <is>
-          <t>GEO - 4 (GEX559_1)</t>
-        </is>
-      </c>
-      <c r="I41" s="7" t="inlineStr">
-        <is>
-          <t>MED - 3 (GSA280_1)</t>
+          <t>CC - 9 (GEX657_1)</t>
+        </is>
+      </c>
+      <c r="I41" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEX612_1) | CC - 4 (GEX613_1) </t>
         </is>
       </c>
       <c r="J41" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">MED - 3 (GSA167_1) | MED - 3 (GSA280_1) </t>
-        </is>
-      </c>
-      <c r="K41" s="7" t="inlineStr">
-        <is>
-          <t>MED - 3 (GSA169_1)</t>
-        </is>
-      </c>
-      <c r="L41" s="7" t="inlineStr">
-        <is>
-          <t>MED - 3 (GSA167_1)</t>
-        </is>
-      </c>
-      <c r="M41" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t xml:space="preserve">CC - 4 (GEN254_1) | CC - 2 (GEX605_3) </t>
+        </is>
+      </c>
+      <c r="K41" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEX090_1) | CC - 4 (GEX612_1) </t>
+        </is>
+      </c>
+      <c r="L41" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEN254_1) | CC - 2 (GEX605_3) </t>
+        </is>
+      </c>
+      <c r="M41" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEX090_1) | CC - 4 (GEX613_1) </t>
         </is>
       </c>
       <c r="N41" s="7" t="inlineStr">
@@ -4466,27 +4466,27 @@
       </c>
       <c r="O41" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 2 (GEX605_1)</t>
         </is>
       </c>
       <c r="P41" s="7" t="inlineStr">
         <is>
-          <t>GEO - 4 (GEX559_1)</t>
-        </is>
-      </c>
-      <c r="Q41" s="10" t="inlineStr">
-        <is>
-          <t>GEO - 4 + HIS - 4 (GCH374_1)</t>
+          <t>CC - 1 (GEX208_2)</t>
+        </is>
+      </c>
+      <c r="Q41" s="7" t="inlineStr">
+        <is>
+          <t>CC - 2 (GLA104_2)</t>
         </is>
       </c>
       <c r="R41" s="7" t="inlineStr">
         <is>
-          <t>GEO - 4 (GCH623_1)</t>
+          <t>CC - 1 (GEX003_1)</t>
         </is>
       </c>
       <c r="S41" s="7" t="inlineStr">
         <is>
-          <t>GEO - 4 (GCH293_6)</t>
+          <t>CC - 1 (GEX210_2)</t>
         </is>
       </c>
       <c r="T41" s="7" t="inlineStr">
@@ -4496,35 +4496,35 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="9" t="n"/>
+      <c r="A42" s="10" t="n"/>
       <c r="B42" s="6" t="inlineStr">
         <is>
-          <t>304-B</t>
+          <t>309-B</t>
         </is>
       </c>
       <c r="C42" s="7" t="inlineStr">
         <is>
-          <t>MED - 7 (GSA213_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D42" s="7" t="inlineStr">
         <is>
-          <t>MED - 7 (GSA214_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E42" s="7" t="inlineStr">
         <is>
-          <t>MED - 7 (GSA287_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F42" s="7" t="inlineStr">
         <is>
-          <t>MED - 7 (GCS239_11)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G42" s="7" t="inlineStr">
         <is>
-          <t>MED - 7 (GSA186_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H42" s="7" t="inlineStr">
@@ -4532,29 +4532,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I42" s="7" t="inlineStr">
-        <is>
-          <t>MED - 7 (GSA217_1)</t>
-        </is>
-      </c>
-      <c r="J42" s="7" t="inlineStr">
-        <is>
-          <t>MED - 7 (GSA214_1)</t>
-        </is>
-      </c>
-      <c r="K42" s="7" t="inlineStr">
-        <is>
-          <t>MED - 7 (GSA215_1)</t>
-        </is>
-      </c>
-      <c r="L42" s="7" t="inlineStr">
-        <is>
-          <t>MED - 7 (GSA216_1)</t>
-        </is>
-      </c>
-      <c r="M42" s="7" t="inlineStr">
-        <is>
-          <t>MED - 7 (GSA215_1)</t>
+      <c r="I42" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 2 (GEN253_1) | CC - 2 (GEX178_1) </t>
+        </is>
+      </c>
+      <c r="J42" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 2 (GEN253_1) | CC - 2 (GEX605_2) </t>
+        </is>
+      </c>
+      <c r="K42" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 2 (GEX178_1) | CC - 2 (GEX195_1) </t>
+        </is>
+      </c>
+      <c r="L42" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 2 (GEX055_1) | CC - 2 (GEX605_2) </t>
+        </is>
+      </c>
+      <c r="M42" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 2 (GEX055_1) | CC - 2 (GEX195_1) </t>
         </is>
       </c>
       <c r="N42" s="7" t="inlineStr">
@@ -4564,27 +4564,27 @@
       </c>
       <c r="O42" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX098_2)</t>
+          <t>CC - 7 (GEX395_1)</t>
         </is>
       </c>
       <c r="P42" s="7" t="inlineStr">
         <is>
-          <t>MED - 7 (GSA213_1)</t>
+          <t>CC - 7 (GCS238_2)</t>
         </is>
       </c>
       <c r="Q42" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX608_1)</t>
+          <t>CC - 7 (GEX618_1)</t>
         </is>
       </c>
       <c r="R42" s="7" t="inlineStr">
         <is>
-          <t>GEO - 6 (GCH622_1)</t>
-        </is>
-      </c>
-      <c r="S42" s="10" t="inlineStr">
-        <is>
-          <t>GEO - 6 + HIS - 6 (GCH383_1)</t>
+          <t>CC - 7 (GEX107_1)</t>
+        </is>
+      </c>
+      <c r="S42" s="7" t="inlineStr">
+        <is>
+          <t>CC - 7 (GEX617_1)</t>
         </is>
       </c>
       <c r="T42" s="7" t="inlineStr">
@@ -4594,20 +4594,20 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="9" t="n"/>
+      <c r="A43" s="10" t="n"/>
       <c r="B43" s="6" t="inlineStr">
         <is>
-          <t>305-B</t>
+          <t>310-B</t>
         </is>
       </c>
       <c r="C43" s="7" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX612_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D43" s="7" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX612_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E43" s="7" t="inlineStr">
@@ -4632,27 +4632,27 @@
       </c>
       <c r="I43" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">CC - 4 (GEX612_1) | CC - 4 (GEX613_2) </t>
-        </is>
-      </c>
-      <c r="J43" s="7" t="inlineStr">
-        <is>
-          <t>CC - 4 (GEX102_1)</t>
-        </is>
-      </c>
-      <c r="K43" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - opt (GEX1082_1) | CC - 4 (GEX612_1) </t>
+          <t xml:space="preserve">CC - 6 (GEX105_1) | CC - 6 (GEX108_1) </t>
+        </is>
+      </c>
+      <c r="J43" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 6 (GCS580_1) | CC - 6 (GEX614_1) </t>
+        </is>
+      </c>
+      <c r="K43" s="7" t="inlineStr">
+        <is>
+          <t>CC - 6 (GCH292_2)</t>
         </is>
       </c>
       <c r="L43" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">CC - 4 (GEX102_1) | CC - opt (GEX1082_1) </t>
-        </is>
-      </c>
-      <c r="M43" s="7" t="inlineStr">
-        <is>
-          <t>CC - 4 (GEX613_2)</t>
+          <t xml:space="preserve">CC - 6 (GCS580_1) | CC - 6 (GEX105_1) </t>
+        </is>
+      </c>
+      <c r="M43" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 6 (GEX108_1) | CC - 6 (GEX614_1) </t>
         </is>
       </c>
       <c r="N43" s="7" t="inlineStr">
@@ -4662,27 +4662,27 @@
       </c>
       <c r="O43" s="7" t="inlineStr">
         <is>
-          <t>CC - opt (GEX635_1)</t>
+          <t>CC - 5 (GEX101_1)</t>
         </is>
       </c>
       <c r="P43" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX392_1)</t>
+          <t>CC - 5 (GEX091_1)</t>
         </is>
       </c>
       <c r="Q43" s="7" t="inlineStr">
         <is>
-          <t>CC - 4 (GCH290_5)</t>
+          <t>CC - 5 (GEX607_1)</t>
         </is>
       </c>
       <c r="R43" s="7" t="inlineStr">
         <is>
-          <t>CC - opt (GEX1083_1)</t>
+          <t>CC - 5 (GEX110_1)</t>
         </is>
       </c>
       <c r="S43" s="7" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX609_1)</t>
+          <t>CC - 5 (GEX616_1)</t>
         </is>
       </c>
       <c r="T43" s="7" t="inlineStr">
@@ -4692,65 +4692,65 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="9" t="n"/>
+      <c r="A44" s="10" t="n"/>
       <c r="B44" s="6" t="inlineStr">
         <is>
-          <t>308-B</t>
+          <t>103-C</t>
         </is>
       </c>
       <c r="C44" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 7 (GSA213_1)</t>
         </is>
       </c>
       <c r="D44" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 7 (GSA214_1)</t>
         </is>
       </c>
       <c r="E44" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 7 (GSA287_1)</t>
         </is>
       </c>
       <c r="F44" s="7" t="inlineStr">
         <is>
-          <t>CC - 8 (GEX658_1)</t>
+          <t>MED - 7 (GCS239_11)</t>
         </is>
       </c>
       <c r="G44" s="7" t="inlineStr">
         <is>
-          <t>CC - 8 (GEX658_1)</t>
+          <t>MED - 7 (GSA186_1)</t>
         </is>
       </c>
       <c r="H44" s="7" t="inlineStr">
         <is>
-          <t>CC - 8 (GEX658_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I44" s="7" t="inlineStr">
         <is>
-          <t>CC - 8 (GCS239_2)</t>
-        </is>
-      </c>
-      <c r="J44" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 2 (GEN253_1) | CC - 2 (GEX605_2) </t>
+          <t>MED - 7 (GSA217_1)</t>
+        </is>
+      </c>
+      <c r="J44" s="7" t="inlineStr">
+        <is>
+          <t>MED - 7 (GSA214_1)</t>
         </is>
       </c>
       <c r="K44" s="7" t="inlineStr">
         <is>
-          <t>CC - 2 (GEX195_1)</t>
-        </is>
-      </c>
-      <c r="L44" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 2 (GEX055_1) | CC - 2 (GEX605_2) </t>
-        </is>
-      </c>
-      <c r="M44" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 2 (GEX055_1) | CC - 2 (GEX195_1) </t>
+          <t>MED - 7 (GSA215_1)</t>
+        </is>
+      </c>
+      <c r="L44" s="7" t="inlineStr">
+        <is>
+          <t>MED - 7 (GSA216_1)</t>
+        </is>
+      </c>
+      <c r="M44" s="7" t="inlineStr">
+        <is>
+          <t>MED - 7 (GSA215_1)</t>
         </is>
       </c>
       <c r="N44" s="7" t="inlineStr">
@@ -4760,27 +4760,27 @@
       </c>
       <c r="O44" s="7" t="inlineStr">
         <is>
-          <t>CC - 5 (GEX101_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P44" s="7" t="inlineStr">
         <is>
-          <t>CC - 5 (GEX091_1)</t>
+          <t>MED - 7 (GSA213_1)</t>
         </is>
       </c>
       <c r="Q44" s="7" t="inlineStr">
         <is>
-          <t>CC - 5 (GEX607_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R44" s="7" t="inlineStr">
         <is>
-          <t>CC - 5 (GEX110_1)</t>
+          <t>MED - 7 (GSA216_1)</t>
         </is>
       </c>
       <c r="S44" s="7" t="inlineStr">
         <is>
-          <t>CC - 5 (GEX616_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T44" s="7" t="inlineStr">
@@ -4790,15 +4790,15 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="9" t="n"/>
+      <c r="A45" s="10" t="n"/>
       <c r="B45" s="6" t="inlineStr">
         <is>
-          <t>309-B</t>
+          <t>105-C</t>
         </is>
       </c>
       <c r="C45" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 8 (GCH859_1)</t>
         </is>
       </c>
       <c r="D45" s="7" t="inlineStr">
@@ -4826,59 +4826,59 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I45" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 6 (GEX105_1) | CC - 6 (GEX108_1) </t>
-        </is>
-      </c>
-      <c r="J45" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 6 (GCS580_1) | CC - 6 (GEX614_1) </t>
+      <c r="I45" s="7" t="inlineStr">
+        <is>
+          <t>FIL - 9 (GCH860_1)</t>
+        </is>
+      </c>
+      <c r="J45" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="K45" s="7" t="inlineStr">
         <is>
-          <t>CC - 6 (GCH292_2)</t>
-        </is>
-      </c>
-      <c r="L45" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 6 (GCS580_1) | CC - 6 (GEX105_1) </t>
-        </is>
-      </c>
-      <c r="M45" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 6 (GEX108_1) | CC - 6 (GEX614_1) </t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L45" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M45" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="N45" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 8 (GCH843_1)</t>
         </is>
       </c>
       <c r="O45" s="7" t="inlineStr">
         <is>
-          <t>CC - 7 (GEX395_1)</t>
+          <t>FIL - 8 (GCH852_1)</t>
         </is>
       </c>
       <c r="P45" s="7" t="inlineStr">
         <is>
-          <t>CC - 7 (GCS238_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q45" s="7" t="inlineStr">
         <is>
-          <t>CC - 7 (GEX618_1)</t>
+          <t>FIL - 8 (GCH844_1)</t>
         </is>
       </c>
       <c r="R45" s="7" t="inlineStr">
         <is>
-          <t>CC - 7 (GEX107_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S45" s="7" t="inlineStr">
         <is>
-          <t>CC - 7 (GEX617_1)</t>
+          <t>FIL - 8 (GCH853_1)</t>
         </is>
       </c>
       <c r="T45" s="7" t="inlineStr">
@@ -4888,10 +4888,10 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="9" t="n"/>
+      <c r="A46" s="10" t="n"/>
       <c r="B46" s="6" t="inlineStr">
         <is>
-          <t>310-B</t>
+          <t>215-C</t>
         </is>
       </c>
       <c r="C46" s="7" t="inlineStr">
@@ -4911,42 +4911,42 @@
       </c>
       <c r="F46" s="7" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G46" s="7" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H46" s="7" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
-        </is>
-      </c>
-      <c r="I46" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 2 (GEX178_1) | CC - 4 (GEX613_1) </t>
-        </is>
-      </c>
-      <c r="J46" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 4 (GEN254_1) | CC - 2 (GEX605_3) </t>
-        </is>
-      </c>
-      <c r="K46" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 4 (GEX090_1) | CC - 2 (GEX178_1) </t>
-        </is>
-      </c>
-      <c r="L46" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 4 (GEN254_1) | CC - 2 (GEX605_3) </t>
-        </is>
-      </c>
-      <c r="M46" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 4 (GEX090_1) | CC - 4 (GEX613_1) </t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I46" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J46" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K46" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L46" s="7" t="inlineStr">
+        <is>
+          <t>FIL - 2 (GCH845_1)</t>
+        </is>
+      </c>
+      <c r="M46" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="N46" s="7" t="inlineStr">
@@ -4956,27 +4956,27 @@
       </c>
       <c r="O46" s="7" t="inlineStr">
         <is>
-          <t>CC - 2 (GEX605_1)</t>
+          <t>FIL - 2 (GCH848_1)</t>
         </is>
       </c>
       <c r="P46" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX208_2)</t>
+          <t>FIL - 2 (GLA103_3)</t>
         </is>
       </c>
       <c r="Q46" s="7" t="inlineStr">
         <is>
-          <t>CC - 2 (GLA104_2)</t>
+          <t>FIL - 2 (GEX211_2)</t>
         </is>
       </c>
       <c r="R46" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_1)</t>
+          <t>FIL - 2 (GCH845_1)</t>
         </is>
       </c>
       <c r="S46" s="7" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX210_2)</t>
+          <t>FIL - 3 (GCH856_1)</t>
         </is>
       </c>
       <c r="T46" s="7" t="inlineStr">
@@ -4986,20 +4986,20 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="9" t="n"/>
+      <c r="A47" s="10" t="n"/>
       <c r="B47" s="6" t="inlineStr">
         <is>
-          <t>103-C</t>
+          <t>216-C</t>
         </is>
       </c>
       <c r="C47" s="7" t="inlineStr">
         <is>
-          <t>MED - 5 (GSA193_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D47" s="7" t="inlineStr">
         <is>
-          <t>MED - 5 (GSA191_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E47" s="7" t="inlineStr">
@@ -5009,12 +5009,12 @@
       </c>
       <c r="F47" s="7" t="inlineStr">
         <is>
-          <t>MED - 5 (GSA189_1)</t>
+          <t>HIS - 8 (GCH390_1)</t>
         </is>
       </c>
       <c r="G47" s="7" t="inlineStr">
         <is>
-          <t>MED - 5 (GSA192_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H47" s="7" t="inlineStr">
@@ -5022,29 +5022,29 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I47" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 5 (GSA188_1) | MED - 5 (GSA193_1)  | MED - 9 (GSA296_1) </t>
-        </is>
-      </c>
-      <c r="J47" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 5 (GSA191_1) | MED - 5 (GSA284_1) </t>
+      <c r="I47" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J47" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="K47" s="7" t="inlineStr">
         <is>
-          <t>MED - 5 (GSA188_1)</t>
-        </is>
-      </c>
-      <c r="L47" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 5 (GSA190_1) | MED - 5 (GSA283_1) </t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L47" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="M47" s="7" t="inlineStr">
         <is>
-          <t>MED - 5 (GSA189_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N47" s="7" t="inlineStr">
@@ -5054,27 +5054,27 @@
       </c>
       <c r="O47" s="7" t="inlineStr">
         <is>
-          <t>MED - 9 (GSA296_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P47" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q47" s="7" t="inlineStr">
-        <is>
-          <t>MED - 5 (GSA192_1)</t>
-        </is>
-      </c>
-      <c r="R47" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 5 (GSA190_1) | MED - 5 (GSA283_1) </t>
+          <t>HIS - 8 (GCH387_1)</t>
+        </is>
+      </c>
+      <c r="Q47" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HIS - opt (GCH459_1 - GCH467_1) </t>
+        </is>
+      </c>
+      <c r="R47" s="7" t="inlineStr">
+        <is>
+          <t>HIS - 8 (GCH390_1)</t>
         </is>
       </c>
       <c r="S47" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 8 (GCH388_1)</t>
         </is>
       </c>
       <c r="T47" s="7" t="inlineStr">
@@ -5084,10 +5084,10 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="9" t="n"/>
+      <c r="A48" s="10" t="n"/>
       <c r="B48" s="6" t="inlineStr">
         <is>
-          <t>105-C</t>
+          <t>217-C</t>
         </is>
       </c>
       <c r="C48" s="7" t="inlineStr">
@@ -5122,7 +5122,7 @@
       </c>
       <c r="I48" s="7" t="inlineStr">
         <is>
-          <t>FIL - 9 (GCH860_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J48" s="7" t="inlineStr">
@@ -5172,7 +5172,7 @@
       </c>
       <c r="S48" s="7" t="inlineStr">
         <is>
-          <t>FIL - 3 (GCH856_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T48" s="7" t="inlineStr">
@@ -5182,10 +5182,10 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="9" t="n"/>
+      <c r="A49" s="10" t="n"/>
       <c r="B49" s="6" t="inlineStr">
         <is>
-          <t>215-C</t>
+          <t>218-C</t>
         </is>
       </c>
       <c r="C49" s="7" t="inlineStr">
@@ -5235,7 +5235,7 @@
       </c>
       <c r="L49" s="7" t="inlineStr">
         <is>
-          <t>FIL - 2 (GCH845_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M49" s="7" t="inlineStr">
@@ -5250,27 +5250,27 @@
       </c>
       <c r="O49" s="7" t="inlineStr">
         <is>
-          <t>FIL - 2 (GCH848_1)</t>
-        </is>
-      </c>
-      <c r="P49" s="7" t="inlineStr">
-        <is>
-          <t>FIL - 2 (GLA103_3)</t>
+          <t>FIL - 4 (GCH847_1)</t>
+        </is>
+      </c>
+      <c r="P49" s="11" t="inlineStr">
+        <is>
+          <t>FIL - 4 + LET - 4 (GCH833_1)</t>
         </is>
       </c>
       <c r="Q49" s="7" t="inlineStr">
         <is>
-          <t>FIL - 2 (GEX211_2)</t>
-        </is>
-      </c>
-      <c r="R49" s="7" t="inlineStr">
-        <is>
-          <t>FIL - 2 (GCH845_1)</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R49" s="11" t="inlineStr">
+        <is>
+          <t>FIL - 4 + MAT - 2 (GCH840_1)</t>
         </is>
       </c>
       <c r="S49" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 4 (GCH850_1)</t>
         </is>
       </c>
       <c r="T49" s="7" t="inlineStr">
@@ -5280,10 +5280,10 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="9" t="n"/>
+      <c r="A50" s="10" t="n"/>
       <c r="B50" s="6" t="inlineStr">
         <is>
-          <t>216-C</t>
+          <t>302-C</t>
         </is>
       </c>
       <c r="C50" s="7" t="inlineStr">
@@ -5303,7 +5303,7 @@
       </c>
       <c r="F50" s="7" t="inlineStr">
         <is>
-          <t>HIS - 8 (GCH390_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G50" s="7" t="inlineStr">
@@ -5348,27 +5348,27 @@
       </c>
       <c r="O50" s="7" t="inlineStr">
         <is>
-          <t>HIS - 8 (GCH389_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P50" s="7" t="inlineStr">
         <is>
-          <t>HIS - 8 (GCH387_1)</t>
-        </is>
-      </c>
-      <c r="Q50" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">HIS - opt (GCH459_1 - GCH467_1) </t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q50" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R50" s="7" t="inlineStr">
         <is>
-          <t>HIS - 8 (GCH390_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S50" s="7" t="inlineStr">
         <is>
-          <t>HIS - 8 (GCH388_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T50" s="7" t="inlineStr">
@@ -5378,15 +5378,15 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="9" t="n"/>
+      <c r="A51" s="10" t="n"/>
       <c r="B51" s="6" t="inlineStr">
         <is>
-          <t>217-C</t>
+          <t>311-C</t>
         </is>
       </c>
       <c r="C51" s="7" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH859_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D51" s="7" t="inlineStr">
@@ -5441,12 +5441,12 @@
       </c>
       <c r="N51" s="7" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH843_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O51" s="7" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH852_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P51" s="7" t="inlineStr">
@@ -5456,7 +5456,7 @@
       </c>
       <c r="Q51" s="7" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH844_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R51" s="7" t="inlineStr">
@@ -5466,7 +5466,7 @@
       </c>
       <c r="S51" s="7" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH853_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T51" s="7" t="inlineStr">
@@ -5476,10 +5476,10 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="9" t="n"/>
+      <c r="A52" s="10" t="n"/>
       <c r="B52" s="6" t="inlineStr">
         <is>
-          <t>218-C</t>
+          <t>109-DE</t>
         </is>
       </c>
       <c r="C52" s="7" t="inlineStr">
@@ -5544,12 +5544,12 @@
       </c>
       <c r="O52" s="7" t="inlineStr">
         <is>
-          <t>FIL - 4 (GCH847_1)</t>
-        </is>
-      </c>
-      <c r="P52" s="10" t="inlineStr">
-        <is>
-          <t>FIL - 4 + LET - 4 (GCH833_1)</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P52" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="Q52" s="7" t="inlineStr">
@@ -5557,14 +5557,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="R52" s="10" t="inlineStr">
-        <is>
-          <t>FIL - 4 + MAT - 2 (GCH840_1)</t>
+      <c r="R52" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="S52" s="7" t="inlineStr">
         <is>
-          <t>FIL - 4 (GCH850_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T52" s="7" t="inlineStr">
@@ -5574,10 +5574,10 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="9" t="n"/>
+      <c r="A53" s="12" t="n"/>
       <c r="B53" s="6" t="inlineStr">
         <is>
-          <t>302-C</t>
+          <t>110-DE</t>
         </is>
       </c>
       <c r="C53" s="7" t="inlineStr">
@@ -5666,398 +5666,6 @@
         </is>
       </c>
       <c r="T53" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="9" t="n"/>
-      <c r="B54" s="6" t="inlineStr">
-        <is>
-          <t>311-C</t>
-        </is>
-      </c>
-      <c r="C54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T54" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="9" t="n"/>
-      <c r="B55" s="6" t="inlineStr">
-        <is>
-          <t>311-DE</t>
-        </is>
-      </c>
-      <c r="C55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T55" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="9" t="n"/>
-      <c r="B56" s="6" t="inlineStr">
-        <is>
-          <t>109-DE</t>
-        </is>
-      </c>
-      <c r="C56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T56" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="12" t="n"/>
-      <c r="B57" s="6" t="inlineStr">
-        <is>
-          <t>110-DE</t>
-        </is>
-      </c>
-      <c r="C57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S57" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T57" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -6065,7 +5673,7 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A4:A57"/>
+    <mergeCell ref="A4:A53"/>
     <mergeCell ref="O1:T1"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="P1:T1"/>

</xml_diff>

<commit_message>
Adiciona mais informações na tabela_alocacoes.csv
</commit_message>
<xml_diff>
--- a/planilha_alocacoes.xlsx
+++ b/planilha_alocacoes.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Organiza arquivos + Adiciona planilha e tabela de alocações do semestre atual
</commit_message>
<xml_diff>
--- a/planilha_alocacoes.xlsx
+++ b/planilha_alocacoes.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Envio de e-mails funcional
</commit_message>
<xml_diff>
--- a/planilha_alocacoes.xlsx
+++ b/planilha_alocacoes.xlsx
@@ -951,7 +951,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>MAT - 1 (GEX213_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>MAT - 1 (GLA104_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
@@ -1059,12 +1059,12 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>MAT - 3 (GEX969_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>MAT - 3 (GEX968_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1079,7 +1079,7 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>MAT - 3 (GCH839_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN198_1) | EAS - opt (GEN199_1) COMPARTILHAMENTO</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN200_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN193_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1853,32 +1853,32 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>AGRO - 9 (GCS085_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>AGRO - 9 (GCA060_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>AGRO - 9 (GCA268_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>AGRO - 9 (GCA057_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>AGRO - opt (GEN190_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>AGRO - 9 (GCA282_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1888,12 +1888,12 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>AGRO - 9 (GCA061_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>AGRO - 9 (GCA259_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1903,17 +1903,17 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>AGRO - opt (GCA316_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>AGRO - opt (GCA647_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>AGRO - 9 (GCA282_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1961,17 +1961,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>AGRO - 5 (GCB058_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>AGRO - 5 (GEN081_1)</t>
+          <t>MED - 8 (GSA298_1)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>AGRO - 5 (GCA238_1) | AGRO - 5 (GCB140_1) COMPARTILHAMENTO</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>AGRO - opt (GCA657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1996,27 +1996,27 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>AGRO - 5 (GCA039_1)</t>
+          <t>MED - 8 (GSA291_1)</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>AGRO - 5 (GCA038_1)</t>
+          <t>MED - 8 (GSA298_1)</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>AGRO - 5 (GCB052_1)</t>
+          <t>MED - 8 (GSA289_1)</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>AGRO - opt (GCA646_1)</t>
+          <t>MED - 8 (GSA290_1)</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>AGRO - opt (GCA653_1)</t>
+          <t>MED - 8 (GSA289_1)</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -2031,7 +2031,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA291_1)</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -2046,7 +2046,7 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA290_1)</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
@@ -2074,17 +2074,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>AGRO - 7 (GCA225_1) | AGRO - 7 (GCA041_1) COMPARTILHAMENTO</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>AGRO - 7 (GCA225_1) | AGRO - 7 (GCS247_1) COMPARTILHAMENTO</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>MED - 6 (GSA197_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -2104,27 +2104,27 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>MED - 6 (GSA196_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>AGRO - 7 (GEN090_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t xml:space="preserve">MED - 6 (GSA285_1 - AGRUPAMENTO GSA286_1) </t>
+          <t>MED - 6 (GSA286_1)</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>AGRO - 7 (GCA252_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>MED - 6 (GSA197_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -2177,12 +2177,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>AGRO - 6 (GCA231_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>AGRO - 3 (GCA0683_2)</t>
+          <t>AGRO - 5 (GEN081_1)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -2192,12 +2192,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>AGRO - 7 (GCS091_1) | AGRO - 7 (GCA287_1) COMPARTILHAMENTO</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA657_1)</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -2212,7 +2212,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>AGRO - 7 (GCA244_1)</t>
+          <t>AGRO - 5 (GCA039_1)</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -2222,17 +2222,17 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>AGRO - 3 (GEX1047_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA646_1)</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA653_1)</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
@@ -2285,32 +2285,32 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>AGRO - 3 (GCA0685_1) | AGRO - 10 (GCA283_1) COMPARTILHAMENTO</t>
+          <t>AGRO - 6 (GCA231_1)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>AGRO - 3 (GCA0683_1) | AGRO - 10 (GCA283_1) COMPARTILHAMENTO | MED - 8 (GSA298_1) COMPARTILHAMENTO</t>
+          <t>AGRO - 7 (GCA225_1) | AGRO - 7 (GCA041_1) COMPARTILHAMENTO</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>AGRO - 3 (GCA0683_1) | AGRO - 10 (GCA283_1) COMPARTILHAMENTO</t>
+          <t>AGRO - 7 (GCA225_1) | AGRO - 7 (GCS247_1) COMPARTILHAMENTO</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>AGRO - 3 (GCB0607_1) | AGRO - 3 (GCB0608_1) COMPARTILHAMENTO | AGRO - 10 (GCA283_1) COMPARTILHAMENTO</t>
+          <t>AGRO - 7 (GCS091_1)</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>AGRO - 10 (GCA283_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>AGRO - 10 (GCA283_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -2320,32 +2320,32 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA291_1)</t>
+          <t>AGRO - 7 (GCA244_1)</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA298_1)</t>
+          <t>AGRO - 7 (GEN090_1)</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA289_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA290_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA289_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>AGRO - 10 (GCA283_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2355,7 +2355,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA291_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2370,17 +2370,17 @@
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA290_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>AGRO - 10 (GCA283_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>AGRO - 10 (GCA283_1)</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -2398,7 +2398,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>AGRO - 3 (GCB057_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA298_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2609,12 +2609,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ENF - 3 (GCS011_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ENF - 1 (GCH029_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -2644,7 +2644,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>ENF - 1 (GLA001_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>ENF - 3 (GCS010_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -2717,22 +2717,22 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ENF - 5 (GSA018_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ENF - 5 (GSA019_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>ENF - 5 (GSA018_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>ENF - 5 (GSA018_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2752,27 +2752,27 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>ENF - 5 (GCB080_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>ENF - 5 (GSA020_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>ENF - 5 (GSA019_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>ENF - 5 (GSA019_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>ENF - 5 (GSA018_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>HIS - 3 (GCH369_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
@@ -3257,7 +3257,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 7 (GCH1120_1)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -3272,12 +3272,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 7 (GLA240_1)</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 7 (GEX776_1)</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -3327,12 +3327,12 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 7 (GCH162_1)</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 8 (GCH1123_1)</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
@@ -3342,12 +3342,12 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 8 (GCH1124_1)</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 8 (GCH1125_1)</t>
         </is>
       </c>
       <c r="V28" t="inlineStr">
@@ -3797,7 +3797,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>PED - 7 (GCH1120_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -3812,12 +3812,12 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>PED - 7 (GLA240_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>PED - 7 (GEX776_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -3867,12 +3867,12 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>PED - 7 (GCH162_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>PED - 8 (GCH1123_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S33" t="inlineStr">
@@ -3882,12 +3882,12 @@
       </c>
       <c r="T33" t="inlineStr">
         <is>
-          <t>PED - 8 (GCH1124_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>PED - 8 (GCH1125_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
@@ -4372,27 +4372,27 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 1 (GEX003_2) | CC - 1 (GEX208_2) COMPARTILHAMENTO</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 1 (GEX003_2) | CC - 1 (GEX208_2) COMPARTILHAMENTO</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 1 (GEX210_1) | CC - 1 (GCH293_1) COMPARTILHAMENTO</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 1 (GEX210_1)</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 1 (GCH293_1)</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
@@ -4407,27 +4407,27 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX615_1)</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX613_1)</t>
         </is>
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX612_1)</t>
         </is>
       </c>
       <c r="T38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX090_1)</t>
         </is>
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX195_1)</t>
         </is>
       </c>
       <c r="V38" t="inlineStr">
@@ -4480,17 +4480,17 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX098_1) | CC - 7 (GEX395_1) COMPARTILHAMENTO</t>
+          <t>CC - 1 (GEX003_1) | CC - 1 (GEX208_1) COMPARTILHAMENTO</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX098_1)</t>
+          <t>CC - 1 (GEX003_1) | CC - 1 (GEX208_1) COMPARTILHAMENTO</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>CC - 7 (GEX395_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
@@ -4515,27 +4515,27 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX615_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX613_1)</t>
+          <t>CC - 4 (GEX613_2)</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX612_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T39" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX090_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX195_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
@@ -4588,17 +4588,17 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX098_2)</t>
+          <t>CC - 3 (GEX098_1)</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX098_2)</t>
+          <t>CC - 3 (GEX098_1)</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>CC - 7 (GCS238_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
@@ -4628,7 +4628,7 @@
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX613_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S40" t="inlineStr">
@@ -4696,27 +4696,27 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_1) | CC - 1 (GEX208_1) COMPARTILHAMENTO</t>
+          <t>CC - 3 (GEX098_2)</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_1) | CC - 1 (GEX208_1) COMPARTILHAMENTO</t>
+          <t>CC - 3 (GEX098_2)</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX210_1) | CC - 1 (GCH293_1) COMPARTILHAMENTO</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX210_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>CC - 1 (GCH293_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
@@ -4804,22 +4804,22 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_2) | CC - 1 (GEX208_2) COMPARTILHAMENTO</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_2) | CC - 1 (GEX208_2) COMPARTILHAMENTO</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>CC - opt (GEX1087_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>CC - opt (GEX1087_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
@@ -5811,7 +5811,7 @@
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>FIL - 2 (GCH855_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
@@ -5821,7 +5821,7 @@
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>FIL - opt (GCH892_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T51" t="inlineStr">
@@ -5919,7 +5919,7 @@
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>FIL - 1 (GCH293_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -5929,17 +5929,17 @@
       </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>FIL - 1 (GCH822_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T52" t="inlineStr">
         <is>
-          <t>FIL - 1 (GCH823_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>FIL - 1 (GCH290_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V52" t="inlineStr">
@@ -6424,27 +6424,27 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>LET - opt (GLA553_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>LET - opt (GLA553_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>LET - opt (GLA553_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>LET - opt (GLA553_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>LET - opt (GLA553_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O57" t="inlineStr">
@@ -6459,12 +6459,12 @@
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>LET - 1 (GCH292_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R57" t="inlineStr">
         <is>
-          <t>LET - 1 (GLA355_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S57" t="inlineStr">
@@ -6474,12 +6474,12 @@
       </c>
       <c r="T57" t="inlineStr">
         <is>
-          <t>LET - opt (GLA517_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U57" t="inlineStr">
         <is>
-          <t>LET - opt (GLA550_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V57" t="inlineStr">

</xml_diff>

<commit_message>
Mudança no fluxo da interface web para permitir apenas uma alocação por vez.
</commit_message>
<xml_diff>
--- a/planilha_alocacoes.xlsx
+++ b/planilha_alocacoes.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V57"/>
+  <dimension ref="A1:V52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1853,27 +1853,27 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 6 (GCA231_1)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 7 (GCA225_1) | AGRO - 7 (GCA041_1) COMPARTILHAMENTO</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 7 (GCA225_1) | AGRO - 7 (GCS247_1) COMPARTILHAMENTO</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 7 (GCS091_1)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA657_1)</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1888,12 +1888,12 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 7 (GCA244_1)</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 7 (GEN090_1)</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1903,12 +1903,12 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA646_1)</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA653_1)</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA298_1)</t>
+          <t>AGRO - 5 (GEN081_1)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1996,27 +1996,27 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA291_1)</t>
+          <t>AGRO - 5 (GCA039_1)</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA298_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA289_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA290_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA289_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -2031,7 +2031,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA291_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -2046,7 +2046,7 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>MED - 8 (GSA290_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
@@ -2114,7 +2114,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>MED - 6 (GSA286_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -2182,7 +2182,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>AGRO - 5 (GEN081_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>AGRO - opt (GCA657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -2212,7 +2212,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>AGRO - 5 (GCA039_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -2222,17 +2222,17 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 6 (GSA286_1)</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>AGRO - opt (GCA646_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>AGRO - opt (GCA653_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
@@ -2285,22 +2285,22 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>AGRO - 6 (GCA231_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>AGRO - 7 (GCA225_1) | AGRO - 7 (GCA041_1) COMPARTILHAMENTO</t>
+          <t>MED - 8 (GSA298_1)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>AGRO - 7 (GCA225_1) | AGRO - 7 (GCS247_1) COMPARTILHAMENTO</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>AGRO - 7 (GCS091_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -2320,27 +2320,27 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>AGRO - 7 (GCA244_1)</t>
+          <t>MED - 8 (GSA291_1)</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>AGRO - 7 (GEN090_1)</t>
+          <t>MED - 8 (GSA298_1)</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA289_1)</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA290_1)</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA289_1)</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
@@ -2355,7 +2355,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA291_1)</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA290_1)</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
@@ -2624,7 +2624,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>ENF - opt (GSA0307_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -2664,7 +2664,7 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>ENF - opt (GSA0307_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
@@ -2732,7 +2732,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - opt (GSA0307_1)</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2772,7 +2772,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - opt (GSA0307_1)</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
@@ -2820,37 +2820,37 @@
       <c r="A24" s="1" t="n"/>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>401-A</t>
+          <t>BLOCO B</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -2860,32 +2860,32 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2895,32 +2895,32 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
     </row>
@@ -2928,37 +2928,37 @@
       <c r="A25" s="1" t="n"/>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>BLOCO B</t>
+          <t>201-B</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -2968,32 +2968,32 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -3003,32 +3003,32 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -3036,7 +3036,7 @@
       <c r="A26" s="1" t="n"/>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>105-B</t>
+          <t>202-B</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -3144,7 +3144,7 @@
       <c r="A27" s="1" t="n"/>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>108-B</t>
+          <t>203-B</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -3252,12 +3252,12 @@
       <c r="A28" s="1" t="n"/>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>201-B</t>
+          <t>204-B</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>PED - 7 (GCH1120_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -3272,12 +3272,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>PED - 7 (GLA240_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>PED - 7 (GEX776_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -3327,12 +3327,12 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>PED - 7 (GCH162_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>PED - 8 (GCH1123_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
@@ -3342,12 +3342,12 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>PED - 8 (GCH1124_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>PED - 8 (GCH1125_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V28" t="inlineStr">
@@ -3360,7 +3360,7 @@
       <c r="A29" s="1" t="n"/>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>202-B</t>
+          <t>205-B</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -3468,12 +3468,12 @@
       <c r="A30" s="1" t="n"/>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>203-B</t>
+          <t>206-B</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 7 (GCH1120_1)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -3488,12 +3488,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 7 (GLA240_1)</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 7 (GEX776_1)</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -3543,12 +3543,12 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 7 (GCH162_1)</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 8 (GCH1123_1)</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
@@ -3558,12 +3558,12 @@
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 8 (GCH1124_1)</t>
         </is>
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 8 (GCH1125_1)</t>
         </is>
       </c>
       <c r="V30" t="inlineStr">
@@ -3576,7 +3576,7 @@
       <c r="A31" s="1" t="n"/>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>204-B</t>
+          <t>207-B</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -3684,7 +3684,7 @@
       <c r="A32" s="1" t="n"/>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>205-B</t>
+          <t>208-B</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -3792,7 +3792,7 @@
       <c r="A33" s="1" t="n"/>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>206-B</t>
+          <t>209-B</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -3900,22 +3900,22 @@
       <c r="A34" s="1" t="n"/>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>207-B</t>
+          <t>210-B</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 9 (GCS550_1)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 9 (GCS551_1)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 9 (GCS573_1)</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3985,7 +3985,7 @@
       </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - opt (GCS555_1)</t>
         </is>
       </c>
       <c r="T34" t="inlineStr">
@@ -4008,7 +4008,7 @@
       <c r="A35" s="1" t="n"/>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>208-B</t>
+          <t>301-B</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -4116,22 +4116,22 @@
       <c r="A36" s="1" t="n"/>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>209-B</t>
+          <t>302-B</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ADM - 9 (GCS550_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>ADM - 9 (GCS551_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>ADM - 9 (GCS573_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4156,12 +4156,12 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 3 (GEX098_2)</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 3 (GEX098_2)</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -4191,17 +4191,17 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX615_1)</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX613_2)</t>
         </is>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>ADM - opt (GCS555_1)</t>
+          <t>CC - 4 (GEX612_1)</t>
         </is>
       </c>
       <c r="T36" t="inlineStr">
@@ -4211,7 +4211,7 @@
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX195_1)</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
@@ -4224,7 +4224,7 @@
       <c r="A37" s="1" t="n"/>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>210-B</t>
+          <t>303-B</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -4264,12 +4264,12 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 3 (GEX098_1)</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 3 (GEX098_1)</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -4304,7 +4304,7 @@
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX613_1)</t>
         </is>
       </c>
       <c r="S37" t="inlineStr">
@@ -4314,7 +4314,7 @@
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX090_1)</t>
         </is>
       </c>
       <c r="U37" t="inlineStr">
@@ -4332,7 +4332,7 @@
       <c r="A38" s="1" t="n"/>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>301-B</t>
+          <t>304-B</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -4372,12 +4372,12 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_2) | CC - 1 (GEX208_2) COMPARTILHAMENTO</t>
+          <t>CC - 1 (GEX003_2) | CC - 1 (GEX208_1) COMPARTILHAMENTO</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_2) | CC - 1 (GEX208_2) COMPARTILHAMENTO</t>
+          <t>CC - 1 (GEX003_2) | CC - 1 (GEX208_1) COMPARTILHAMENTO</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -4407,27 +4407,27 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX615_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX613_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX612_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T38" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX090_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX195_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V38" t="inlineStr">
@@ -4440,7 +4440,7 @@
       <c r="A39" s="1" t="n"/>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>302-B</t>
+          <t>305-B</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -4480,12 +4480,12 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_1) | CC - 1 (GEX208_1) COMPARTILHAMENTO</t>
+          <t>CC - 1 (GEX003_1) | CC - 1 (GEX208_2) COMPARTILHAMENTO</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_1) | CC - 1 (GEX208_1) COMPARTILHAMENTO</t>
+          <t>CC - 1 (GEX003_1) | CC - 1 (GEX208_2) COMPARTILHAMENTO</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -4520,7 +4520,7 @@
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX613_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
@@ -4548,7 +4548,7 @@
       <c r="A40" s="1" t="n"/>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>303-B</t>
+          <t>308-B</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -4588,12 +4588,12 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX098_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX098_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -4656,7 +4656,7 @@
       <c r="A41" s="1" t="n"/>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>304-B</t>
+          <t>309-B</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -4696,12 +4696,12 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX098_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>CC - 3 (GEX098_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -4764,7 +4764,7 @@
       <c r="A42" s="1" t="n"/>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>305-B</t>
+          <t>310-B</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -4872,37 +4872,37 @@
       <c r="A43" s="1" t="n"/>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>308-B</t>
+          <t>BLOCO C</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -4912,32 +4912,32 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -4947,32 +4947,32 @@
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="S43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="T43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="U43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>#</t>
         </is>
       </c>
     </row>
@@ -4980,7 +4980,7 @@
       <c r="A44" s="1" t="n"/>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>309-B</t>
+          <t>103-C</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -5088,7 +5088,7 @@
       <c r="A45" s="1" t="n"/>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>310-B</t>
+          <t>105-C</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -5196,37 +5196,37 @@
       <c r="A46" s="1" t="n"/>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>BLOCO C</t>
+          <t>203-C</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -5236,32 +5236,32 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -5271,32 +5271,32 @@
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -5304,7 +5304,7 @@
       <c r="A47" s="1" t="n"/>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>103-C</t>
+          <t>204-C</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -5412,7 +5412,7 @@
       <c r="A48" s="1" t="n"/>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>105-C</t>
+          <t>205-C</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -5520,7 +5520,7 @@
       <c r="A49" s="1" t="n"/>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>215-C</t>
+          <t>212-C</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -5628,7 +5628,7 @@
       <c r="A50" s="1" t="n"/>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>216-C</t>
+          <t>215-C</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -5736,7 +5736,7 @@
       <c r="A51" s="1" t="n"/>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>217-C</t>
+          <t>216-C</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -5943,546 +5943,6 @@
         </is>
       </c>
       <c r="V52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n"/>
-      <c r="B53" s="1" t="inlineStr">
-        <is>
-          <t>302-C</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="U53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n"/>
-      <c r="B54" s="1" t="inlineStr">
-        <is>
-          <t>311-C</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P54" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="U54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n"/>
-      <c r="B55" s="1" t="inlineStr">
-        <is>
-          <t>BLOCO DE</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="P55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="T55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="U55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="V55" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n"/>
-      <c r="B56" s="1" t="inlineStr">
-        <is>
-          <t>109-DE</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P56" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="U56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n"/>
-      <c r="B57" s="1" t="inlineStr">
-        <is>
-          <t>110-DE</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P57" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="U57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V57" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -6492,8 +5952,8 @@
   <mergeCells count="4">
     <mergeCell ref="R1:V1"/>
     <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A4:A57"/>
     <mergeCell ref="D1:H1"/>
+    <mergeCell ref="A4:A52"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>